<commit_message>
support recording delta for each nurse in swap. optimize block swap in non-tabu condition. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33210" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="35550" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,21 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_PP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>TSR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_PBAF</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -65,43 +57,39 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;n1,n1</t>
+    <t>ACBR_RBNP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>?</t>
+    <t>ACBR_RBWP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_RBNF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_RBNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_RBWF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_RBWO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OldMin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NewMin</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Min</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>≈3543.15</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_PFAO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_PFAF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_PFNF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_PFSF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_PFWF</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -462,7 +450,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -658,6 +646,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -787,7 +788,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -824,6 +825,9 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -833,19 +837,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -902,7 +897,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -920,14 +922,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FF66FF66"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FF33CC33"/>
         </patternFill>
       </fill>
     </dxf>
@@ -935,6 +937,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FF66"/>
+      <color rgb="FF33CC33"/>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FFFF7C80"/>
     </mruColors>
   </colors>
@@ -1212,17 +1217,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="10.5" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
@@ -1231,971 +1235,1043 @@
     <col min="11" max="11" width="10.5" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.625" style="3"/>
-    <col min="15" max="16384" width="10.625" style="1"/>
+    <col min="14" max="15" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="22"/>
-    </row>
-    <row r="2" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="I2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>2</v>
+      <c r="C3" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>1</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4">
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>3501.7647058823532</v>
+      </c>
+      <c r="B4" s="9">
         <f>AVERAGE(B5:B128)</f>
-        <v>3641.7647058823532</v>
+        <v>3561.1764705882351</v>
       </c>
       <c r="C4" s="9">
-        <f t="shared" ref="C4:N4" si="0">AVERAGE(C5:C128)</f>
-        <v>3618.8235294117649</v>
+        <f t="shared" ref="C4:O4" si="0">AVERAGE(C5:C128)</f>
+        <v>3584.1176470588234</v>
       </c>
       <c r="D4" s="4">
         <f>AVERAGE(D5:D128)</f>
-        <v>3599.1176470588234</v>
+        <v>3604.705882352941</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>3590.8823529411766</v>
+        <v>3579.1176470588234</v>
       </c>
       <c r="F4" s="4">
         <f>AVERAGE(F5:F128)</f>
-        <v>3581.7647058823532</v>
+        <v>3618.2352941176468</v>
       </c>
       <c r="G4" s="11">
         <f t="shared" si="0"/>
-        <v>3591.7647058823532</v>
+        <v>3554.1176470588234</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>3620.294117647059</v>
+        <v>3580.8823529411766</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" si="0"/>
-        <v>3622.0588235294117</v>
+        <v>3560.294117647059</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
-        <v>3643.5294117647059</v>
+        <v>3580.294117647059</v>
       </c>
       <c r="K4" s="10">
         <f t="shared" si="0"/>
-        <v>3628.8235294117649</v>
+        <v>3556.1764705882351</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>3627.0588235294117</v>
+        <v>3591.1764705882351</v>
       </c>
       <c r="M4" s="11">
         <f t="shared" si="0"/>
-        <v>3586.7647058823532</v>
+        <v>3526.4705882352941</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
-        <v>3501.7647058823532</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
-        <v>1585</v>
-      </c>
-      <c r="B5" s="3">
+        <v>3471.7647058823532</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="0"/>
+        <v>3467.0588235294117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>1560</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1615</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1625</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1610</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1615</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1660</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1610</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1640</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1600</v>
+      </c>
+      <c r="J5" s="1">
         <v>1630</v>
       </c>
-      <c r="C5" s="1">
-        <v>1660</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1570</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="K5" s="1">
         <v>1630</v>
       </c>
-      <c r="F5" s="3">
-        <v>1615</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1630</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1630</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1630</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="L5" s="1">
+        <v>1625</v>
+      </c>
+      <c r="M5" s="1">
         <v>1600</v>
       </c>
-      <c r="K5" s="7">
-        <v>1610</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1630</v>
-      </c>
-      <c r="M5" s="1">
+      <c r="N5" s="12">
+        <f>MIN(B5:M5)</f>
+        <v>1600</v>
+      </c>
+      <c r="O5" s="3">
+        <f>MIN(A5,N5)</f>
         <v>1560</v>
       </c>
-      <c r="N5" s="16">
-        <f>MIN(B5:M5)</f>
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
-        <v>3035</v>
-      </c>
-      <c r="B6" s="3">
-        <v>3240</v>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>3075</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3105</v>
       </c>
       <c r="C6" s="1">
+        <v>3020</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3120</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3050</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3190</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3005</v>
+      </c>
+      <c r="H6" s="1">
         <v>3075</v>
       </c>
-      <c r="D6" s="3">
+      <c r="I6" s="1">
+        <v>3130</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3015</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3065</v>
+      </c>
+      <c r="L6" s="1">
         <v>3120</v>
       </c>
-      <c r="E6" s="3">
-        <v>3095</v>
-      </c>
-      <c r="F6" s="3">
-        <v>3180</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3120</v>
-      </c>
-      <c r="H6" s="3">
-        <v>3080</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3155</v>
-      </c>
-      <c r="J6" s="3">
-        <v>3175</v>
-      </c>
-      <c r="K6" s="7">
-        <v>3140</v>
-      </c>
-      <c r="L6" s="3">
-        <v>3085</v>
-      </c>
       <c r="M6" s="1">
-        <v>3080</v>
-      </c>
-      <c r="N6" s="16">
+        <v>3050</v>
+      </c>
+      <c r="N6" s="12">
         <f t="shared" ref="N6:N21" si="1">MIN(B6:M6)</f>
-        <v>3075</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
-        <v>2045</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2025</v>
+        <v>3005</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" ref="O6:O21" si="2">MIN(A6,N6)</f>
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>1965</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1980</v>
       </c>
       <c r="C7" s="1">
-        <v>2040</v>
-      </c>
-      <c r="D7" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1970</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2010</v>
+      </c>
+      <c r="F7" s="1">
         <v>2005</v>
       </c>
-      <c r="E7" s="3">
+      <c r="G7" s="1">
+        <v>1995</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1990</v>
+      </c>
+      <c r="J7" s="1">
         <v>2030</v>
       </c>
-      <c r="F7" s="3">
-        <v>1985</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H7" s="3">
-        <v>2015</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2015</v>
-      </c>
-      <c r="J7" s="3">
+      <c r="K7" s="1">
+        <v>1990</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1990</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2020</v>
+      </c>
+      <c r="N7" s="12">
+        <f t="shared" si="1"/>
         <v>1970</v>
       </c>
-      <c r="K7" s="7">
-        <v>2045</v>
-      </c>
-      <c r="L7" s="3">
-        <v>2030</v>
-      </c>
-      <c r="M7" s="1">
+      <c r="O7" s="3">
+        <f t="shared" si="2"/>
         <v>1965</v>
       </c>
-      <c r="N7" s="16">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>2310</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2320</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2325</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2330</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2295</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2365</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2330</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2380</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2340</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2340</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2305</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2355</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2350</v>
+      </c>
+      <c r="N8" s="12">
         <f t="shared" si="1"/>
-        <v>1965</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>2335</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2390</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2320</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2355</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2320</v>
-      </c>
-      <c r="F8" s="3">
-        <v>2340</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2310</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2325</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2350</v>
-      </c>
-      <c r="J8" s="3">
-        <v>2315</v>
-      </c>
-      <c r="K8" s="7">
-        <v>2360</v>
-      </c>
-      <c r="L8" s="3">
-        <v>2365</v>
-      </c>
-      <c r="M8" s="1">
-        <v>2360</v>
-      </c>
-      <c r="N8" s="16">
-        <f t="shared" si="1"/>
-        <v>2310</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
+        <v>2295</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="2"/>
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>3195</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3220</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3295</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3315</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3325</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3375</v>
+      </c>
+      <c r="G9" s="1">
         <v>3305</v>
       </c>
-      <c r="B9" s="3">
-        <v>3335</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3245</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="H9" s="1">
         <v>3330</v>
       </c>
-      <c r="E9" s="3">
-        <v>3315</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="I9" s="1">
+        <v>3320</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3300</v>
+      </c>
+      <c r="K9" s="1">
         <v>3305</v>
       </c>
-      <c r="G9" s="1">
+      <c r="L9" s="1">
+        <v>3325</v>
+      </c>
+      <c r="M9" s="1">
         <v>3195</v>
       </c>
-      <c r="H9" s="3">
-        <v>3250</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3335</v>
-      </c>
-      <c r="J9" s="3">
-        <v>3355</v>
-      </c>
-      <c r="K9" s="7">
-        <v>3425</v>
-      </c>
-      <c r="L9" s="3">
-        <v>3370</v>
-      </c>
-      <c r="M9" s="1">
-        <v>3215</v>
-      </c>
-      <c r="N9" s="16">
+      <c r="N9" s="12">
         <f t="shared" si="1"/>
         <v>3195</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
-        <v>2055</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2170</v>
+      <c r="O9" s="3">
+        <f t="shared" si="2"/>
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>2065</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2175</v>
       </c>
       <c r="C10" s="1">
-        <v>2125</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2120</v>
-      </c>
-      <c r="E10" s="3">
-        <v>2195</v>
-      </c>
-      <c r="F10" s="3">
+        <v>2150</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2160</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2190</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2205</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2155</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2165</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2090</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2185</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2090</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2070</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2090</v>
+      </c>
+      <c r="N10" s="12">
+        <f t="shared" si="1"/>
+        <v>2070</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="2"/>
         <v>2065</v>
       </c>
-      <c r="G10" s="1">
-        <v>2135</v>
-      </c>
-      <c r="H10" s="3">
-        <v>2180</v>
-      </c>
-      <c r="I10" s="1">
-        <v>2215</v>
-      </c>
-      <c r="J10" s="3">
-        <v>2165</v>
-      </c>
-      <c r="K10" s="7">
-        <v>2120</v>
-      </c>
-      <c r="L10" s="3">
-        <v>2150</v>
-      </c>
-      <c r="M10" s="1">
-        <v>2100</v>
-      </c>
-      <c r="N10" s="16">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>3545</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3780</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3685</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3725</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3600</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3665</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3685</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3630</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3580</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3665</v>
+      </c>
+      <c r="K11" s="1">
+        <v>3685</v>
+      </c>
+      <c r="L11" s="1">
+        <v>3620</v>
+      </c>
+      <c r="M11" s="1">
+        <v>3505</v>
+      </c>
+      <c r="N11" s="12">
         <f t="shared" si="1"/>
-        <v>2065</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
-        <v>3565</v>
-      </c>
-      <c r="B11" s="3">
-        <v>3650</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3680</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3745</v>
-      </c>
-      <c r="E11" s="3">
-        <v>3555</v>
-      </c>
-      <c r="F11" s="3">
-        <v>3720</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3695</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3545</v>
-      </c>
-      <c r="I11" s="1">
-        <v>3690</v>
-      </c>
-      <c r="J11" s="3">
-        <v>3600</v>
-      </c>
-      <c r="K11" s="7">
-        <v>3615</v>
-      </c>
-      <c r="L11" s="3">
-        <v>3585</v>
-      </c>
-      <c r="M11" s="1">
-        <v>3615</v>
-      </c>
-      <c r="N11" s="16">
+        <v>3505</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="2"/>
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
+        <v>2250</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2265</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2285</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2320</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2290</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2340</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2340</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2250</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2220</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2345</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2275</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2210</v>
+      </c>
+      <c r="M12" s="1">
+        <v>2335</v>
+      </c>
+      <c r="N12" s="12">
         <f t="shared" si="1"/>
-        <v>3545</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
-        <v>2270</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2335</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2250</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2250</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2255</v>
-      </c>
-      <c r="F12" s="3">
-        <v>2290</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2300</v>
-      </c>
-      <c r="H12" s="3">
-        <v>2355</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2300</v>
-      </c>
-      <c r="J12" s="3">
-        <v>2255</v>
-      </c>
-      <c r="K12" s="7">
-        <v>2290</v>
-      </c>
-      <c r="L12" s="3">
-        <v>2310</v>
-      </c>
-      <c r="M12" s="1">
-        <v>2320</v>
-      </c>
-      <c r="N12" s="16">
+        <v>2210</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="2"/>
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
+        <v>6800</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6830</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6880</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6855</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6850</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6870</v>
+      </c>
+      <c r="G13" s="1">
+        <v>6850</v>
+      </c>
+      <c r="H13" s="1">
+        <v>6830</v>
+      </c>
+      <c r="I13" s="1">
+        <v>7000</v>
+      </c>
+      <c r="J13" s="1">
+        <v>7005</v>
+      </c>
+      <c r="K13" s="1">
+        <v>6990</v>
+      </c>
+      <c r="L13" s="1">
+        <v>7085</v>
+      </c>
+      <c r="M13" s="1">
+        <v>6920</v>
+      </c>
+      <c r="N13" s="12">
         <f t="shared" si="1"/>
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
-        <v>6795</v>
-      </c>
-      <c r="B13" s="3">
-        <v>7060</v>
-      </c>
-      <c r="C13" s="1">
-        <v>7130</v>
-      </c>
-      <c r="D13" s="3">
-        <v>6925</v>
-      </c>
-      <c r="E13" s="3">
-        <v>6965</v>
-      </c>
-      <c r="F13" s="3">
+        <v>6830</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="2"/>
         <v>6800</v>
       </c>
-      <c r="G13" s="1">
-        <v>7110</v>
-      </c>
-      <c r="H13" s="3">
-        <v>6955</v>
-      </c>
-      <c r="I13" s="1">
-        <v>7030</v>
-      </c>
-      <c r="J13" s="3">
-        <v>7065</v>
-      </c>
-      <c r="K13" s="7">
-        <v>6955</v>
-      </c>
-      <c r="L13" s="3">
-        <v>7145</v>
-      </c>
-      <c r="M13" s="1">
-        <v>7030</v>
-      </c>
-      <c r="N13" s="16">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>2800</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2810</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2795</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2780</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2860</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2950</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2895</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2925</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2795</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2845</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2890</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2835</v>
+      </c>
+      <c r="M14" s="1">
+        <v>2865</v>
+      </c>
+      <c r="N14" s="12">
         <f t="shared" si="1"/>
-        <v>6800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
-        <v>2835</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2900</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2995</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2885</v>
-      </c>
-      <c r="E14" s="3">
-        <v>2955</v>
-      </c>
-      <c r="F14" s="3">
-        <v>2905</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2920</v>
-      </c>
-      <c r="H14" s="3">
-        <v>2855</v>
-      </c>
-      <c r="I14" s="1">
-        <v>2995</v>
-      </c>
-      <c r="J14" s="3">
-        <v>2905</v>
-      </c>
-      <c r="K14" s="7">
-        <v>2800</v>
-      </c>
-      <c r="L14" s="3">
-        <v>2925</v>
-      </c>
-      <c r="M14" s="1">
-        <v>2980</v>
-      </c>
-      <c r="N14" s="16">
+        <v>2780</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="2"/>
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
+        <v>3780</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3760</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4025</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4085</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4010</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4065</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3820</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3795</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3915</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3915</v>
+      </c>
+      <c r="K15" s="1">
+        <v>3855</v>
+      </c>
+      <c r="L15" s="1">
+        <v>3880</v>
+      </c>
+      <c r="M15" s="1">
+        <v>3740</v>
+      </c>
+      <c r="N15" s="12">
         <f t="shared" si="1"/>
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
+        <v>3740</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="2"/>
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A16" s="3">
+        <v>3950</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4045</v>
+      </c>
+      <c r="C16" s="1">
         <v>3995</v>
       </c>
-      <c r="B15" s="3">
+      <c r="D16" s="1">
+        <v>4060</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4005</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4010</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4040</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4040</v>
+      </c>
+      <c r="I16" s="1">
+        <v>4025</v>
+      </c>
+      <c r="J16" s="1">
         <v>3950</v>
       </c>
-      <c r="C15" s="1">
-        <v>3910</v>
-      </c>
-      <c r="D15" s="3">
-        <v>4035</v>
-      </c>
-      <c r="E15" s="3">
-        <v>3860</v>
-      </c>
-      <c r="F15" s="3">
-        <v>3940</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3980</v>
-      </c>
-      <c r="H15" s="3">
-        <v>4095</v>
-      </c>
-      <c r="I15" s="1">
-        <v>3780</v>
-      </c>
-      <c r="J15" s="3">
-        <v>4045</v>
-      </c>
-      <c r="K15" s="7">
-        <v>3935</v>
-      </c>
-      <c r="L15" s="3">
-        <v>4020</v>
-      </c>
-      <c r="M15" s="1">
-        <v>3940</v>
-      </c>
-      <c r="N15" s="16">
-        <f t="shared" si="1"/>
-        <v>3780</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
-        <v>4005</v>
-      </c>
-      <c r="B16" s="3">
-        <v>4010</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4020</v>
-      </c>
-      <c r="D16" s="3">
-        <v>4040</v>
-      </c>
-      <c r="E16" s="3">
-        <v>4100</v>
-      </c>
-      <c r="F16" s="3">
-        <v>4135</v>
-      </c>
-      <c r="G16" s="1">
-        <v>3950</v>
-      </c>
-      <c r="H16" s="3">
-        <v>4050</v>
-      </c>
-      <c r="I16" s="1">
-        <v>4230</v>
-      </c>
-      <c r="J16" s="3">
-        <v>4110</v>
-      </c>
-      <c r="K16" s="7">
-        <v>4085</v>
-      </c>
-      <c r="L16" s="3">
-        <v>4085</v>
+      <c r="K16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4145</v>
       </c>
       <c r="M16" s="1">
-        <v>4100</v>
-      </c>
-      <c r="N16" s="16">
+        <v>4025</v>
+      </c>
+      <c r="N16" s="12">
         <f t="shared" si="1"/>
         <v>3950</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
-        <v>5985</v>
-      </c>
-      <c r="B17" s="3">
-        <v>6165</v>
+      <c r="O16" s="3">
+        <f t="shared" si="2"/>
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A17" s="3">
+        <v>5940</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6090</v>
       </c>
       <c r="C17" s="1">
-        <v>6115</v>
-      </c>
-      <c r="D17" s="3">
-        <v>6080</v>
-      </c>
-      <c r="E17" s="3">
-        <v>6085</v>
-      </c>
-      <c r="F17" s="3">
-        <v>6105</v>
+        <v>6155</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6195</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6155</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6010</v>
       </c>
       <c r="G17" s="1">
-        <v>6025</v>
-      </c>
-      <c r="H17" s="3">
-        <v>6345</v>
+        <v>6075</v>
+      </c>
+      <c r="H17" s="1">
+        <v>6070</v>
       </c>
       <c r="I17" s="1">
-        <v>5970</v>
-      </c>
-      <c r="J17" s="3">
-        <v>6370</v>
-      </c>
-      <c r="K17" s="7">
-        <v>6265</v>
-      </c>
-      <c r="L17" s="3">
-        <v>6020</v>
+        <v>6055</v>
+      </c>
+      <c r="J17" s="1">
+        <v>5930</v>
+      </c>
+      <c r="K17" s="1">
+        <v>5940</v>
+      </c>
+      <c r="L17" s="1">
+        <v>6120</v>
       </c>
       <c r="M17" s="1">
-        <v>5940</v>
-      </c>
-      <c r="N17" s="16">
+        <v>5945</v>
+      </c>
+      <c r="N17" s="12">
         <f t="shared" si="1"/>
-        <v>5940</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
+        <v>5930</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" si="2"/>
+        <v>5930</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>2995</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3040</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3105</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3030</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2930</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3070</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3100</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3010</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2965</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3095</v>
+      </c>
+      <c r="K18" s="1">
+        <v>3040</v>
+      </c>
+      <c r="L18" s="1">
+        <v>3150</v>
+      </c>
+      <c r="M18" s="1">
+        <v>3070</v>
+      </c>
+      <c r="N18" s="12">
+        <f t="shared" si="1"/>
+        <v>2930</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" si="2"/>
+        <v>2930</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
+        <v>5060</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5285</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5150</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5390</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5305</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5105</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5190</v>
+      </c>
+      <c r="H19" s="1">
+        <v>5370</v>
+      </c>
+      <c r="I19" s="1">
+        <v>5055</v>
+      </c>
+      <c r="J19" s="1">
+        <v>5255</v>
+      </c>
+      <c r="K19" s="1">
+        <v>5170</v>
+      </c>
+      <c r="L19" s="1">
+        <v>5220</v>
+      </c>
+      <c r="M19" s="1">
+        <v>5140</v>
+      </c>
+      <c r="N19" s="12">
+        <f t="shared" si="1"/>
+        <v>5055</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" si="2"/>
+        <v>5055</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>2925</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2985</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2960</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2845</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2935</v>
+      </c>
+      <c r="F20" s="1">
         <v>3060</v>
       </c>
-      <c r="B18" s="3">
-        <v>3180</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3110</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3050</v>
-      </c>
-      <c r="E18" s="3">
-        <v>3160</v>
-      </c>
-      <c r="F18" s="3">
-        <v>3035</v>
-      </c>
-      <c r="G18" s="1">
-        <v>3075</v>
-      </c>
-      <c r="H18" s="3">
-        <v>3060</v>
-      </c>
-      <c r="I18" s="1">
-        <v>3080</v>
-      </c>
-      <c r="J18" s="3">
-        <v>3140</v>
-      </c>
-      <c r="K18" s="7">
-        <v>3205</v>
-      </c>
-      <c r="L18" s="3">
-        <v>3050</v>
-      </c>
-      <c r="M18" s="1">
-        <v>2995</v>
-      </c>
-      <c r="N18" s="16">
+      <c r="G20" s="1">
+        <v>2835</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2925</v>
+      </c>
+      <c r="I20" s="1">
+        <v>2970</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K20" s="1">
+        <v>2815</v>
+      </c>
+      <c r="L20" s="1">
+        <v>2960</v>
+      </c>
+      <c r="M20" s="1">
+        <v>2765</v>
+      </c>
+      <c r="N20" s="12">
         <f t="shared" si="1"/>
-        <v>2995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="3">
-        <v>5165</v>
-      </c>
-      <c r="C19" s="1">
-        <v>5320</v>
-      </c>
-      <c r="D19" s="3">
-        <v>5320</v>
-      </c>
-      <c r="E19" s="3">
-        <v>5060</v>
-      </c>
-      <c r="F19" s="3">
-        <v>5180</v>
-      </c>
-      <c r="G19" s="1">
-        <v>5135</v>
-      </c>
-      <c r="H19" s="3">
-        <v>5270</v>
-      </c>
-      <c r="I19" s="1">
-        <v>5210</v>
-      </c>
-      <c r="J19" s="3">
-        <v>5325</v>
-      </c>
-      <c r="K19" s="7">
-        <v>5195</v>
-      </c>
-      <c r="L19" s="3">
+        <v>2765</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" si="2"/>
+        <v>2765</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A21" s="3">
+        <v>5315</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5235</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5460</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5490</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5420</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5565</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5190</v>
+      </c>
+      <c r="H21" s="1">
+        <v>5440</v>
+      </c>
+      <c r="I21" s="1">
+        <v>5475</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5360</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5410</v>
+      </c>
+      <c r="L21" s="1">
+        <v>5340</v>
+      </c>
+      <c r="M21" s="1">
         <v>5335</v>
       </c>
-      <c r="M19" s="1">
-        <v>5310</v>
-      </c>
-      <c r="N19" s="16">
+      <c r="N21" s="12">
         <f t="shared" si="1"/>
-        <v>5060</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
-        <v>2895</v>
-      </c>
-      <c r="B20" s="3">
-        <v>3110</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2995</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2925</v>
-      </c>
-      <c r="E20" s="3">
-        <v>3010</v>
-      </c>
-      <c r="F20" s="3">
-        <v>2975</v>
-      </c>
-      <c r="G20" s="1">
-        <v>2995</v>
-      </c>
-      <c r="H20" s="3">
-        <v>3090</v>
-      </c>
-      <c r="I20" s="1">
-        <v>2990</v>
-      </c>
-      <c r="J20" s="3">
-        <v>3025</v>
-      </c>
-      <c r="K20" s="7">
-        <v>3130</v>
-      </c>
-      <c r="L20" s="3">
-        <v>3000</v>
-      </c>
-      <c r="M20" s="1">
-        <v>2935</v>
-      </c>
-      <c r="N20" s="16">
-        <f t="shared" si="1"/>
-        <v>2925</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="3">
-        <v>5595</v>
-      </c>
-      <c r="C21" s="1">
-        <v>5530</v>
-      </c>
-      <c r="D21" s="3">
-        <v>5430</v>
-      </c>
-      <c r="E21" s="3">
-        <v>5455</v>
-      </c>
-      <c r="F21" s="3">
-        <v>5315</v>
-      </c>
-      <c r="G21" s="1">
-        <v>5485</v>
-      </c>
-      <c r="H21" s="3">
-        <v>5445</v>
-      </c>
-      <c r="I21" s="1">
-        <v>5600</v>
-      </c>
-      <c r="J21" s="3">
-        <v>5520</v>
-      </c>
-      <c r="K21" s="7">
-        <v>5515</v>
-      </c>
-      <c r="L21" s="3">
-        <v>5555</v>
-      </c>
-      <c r="M21" s="1">
-        <v>5530</v>
-      </c>
-      <c r="N21" s="16">
-        <f t="shared" si="1"/>
-        <v>5315</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+        <v>5190</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" si="2"/>
+        <v>5190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.15">
@@ -2372,17 +2448,20 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:Z128">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>A4=SMALL($A4:$Z4,1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>A4=SMALL($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>A4=LARGE($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>A4=LARGE($A4:$Z4,1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>A4=SMALL($A4:$Z4,3)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new search method SwapChainSearch. speed up rebuild() when the objective value of the assignment is available. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="35550" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="36720" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -29,55 +29,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_RBAF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBAO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBAP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBAR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RFAF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RFAO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>1;w1,w1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBNP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBWP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBNF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBNO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBWF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_RBWO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -90,6 +42,50 @@
   </si>
   <si>
     <t>Min</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5;w1,w1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_FNF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_FNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BAF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BAP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BNP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_FAO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_FWF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_FWO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BNR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -828,6 +824,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -835,12 +837,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1220,21 +1216,20 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.625" style="1"/>
   </cols>
@@ -1242,75 +1237,77 @@
     <row r="1" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="17"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="M2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1322,25 +1319,25 @@
       <c r="F3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="6" t="s">
@@ -1348,64 +1345,64 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>3501.7647058823532</v>
       </c>
       <c r="B4" s="9">
         <f>AVERAGE(B5:B128)</f>
-        <v>3561.1764705882351</v>
+        <v>3640.294117647059</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ref="C4:O4" si="0">AVERAGE(C5:C128)</f>
-        <v>3584.1176470588234</v>
+        <v>3593.5294117647059</v>
       </c>
       <c r="D4" s="4">
         <f>AVERAGE(D5:D128)</f>
-        <v>3604.705882352941</v>
+        <v>3585</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>3579.1176470588234</v>
+        <v>3614.1176470588234</v>
       </c>
       <c r="F4" s="4">
         <f>AVERAGE(F5:F128)</f>
-        <v>3618.2352941176468</v>
+        <v>3577.9411764705883</v>
       </c>
       <c r="G4" s="11">
         <f t="shared" si="0"/>
-        <v>3554.1176470588234</v>
-      </c>
-      <c r="H4" s="4">
+        <v>3562.6470588235293</v>
+      </c>
+      <c r="H4" s="10">
         <f t="shared" si="0"/>
-        <v>3580.8823529411766</v>
-      </c>
-      <c r="I4" s="9">
+        <v>3575.294117647059</v>
+      </c>
+      <c r="I4" s="4">
         <f t="shared" si="0"/>
-        <v>3560.294117647059</v>
+        <v>3584.1176470588234</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
-        <v>3580.294117647059</v>
+        <v>3613.5294117647059</v>
       </c>
       <c r="K4" s="10">
         <f t="shared" si="0"/>
-        <v>3556.1764705882351</v>
+        <v>3589.4117647058824</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>3591.1764705882351</v>
-      </c>
-      <c r="M4" s="11">
+        <v>3563.2352941176468</v>
+      </c>
+      <c r="M4" s="9">
         <f t="shared" si="0"/>
-        <v>3526.4705882352941</v>
+        <v>3582.0588235294117</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
-        <v>3471.7647058823532</v>
+        <v>3488.8235294117649</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>3467.0588235294117</v>
+        <v>3475.8823529411766</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
@@ -1413,44 +1410,44 @@
         <v>1560</v>
       </c>
       <c r="B5" s="1">
+        <v>1560</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1610</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1630</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1560</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1560</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1585</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1630</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1610</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1660</v>
+      </c>
+      <c r="L5" s="8">
         <v>1615</v>
       </c>
-      <c r="C5" s="1">
-        <v>1625</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1610</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1615</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1660</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1610</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1640</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1600</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1630</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1630</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1625</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1600</v>
+      <c r="M5" s="5">
+        <v>1560</v>
       </c>
       <c r="N5" s="12">
         <f>MIN(B5:M5)</f>
-        <v>1600</v>
+        <v>1560</v>
       </c>
       <c r="O5" s="3">
         <f>MIN(A5,N5)</f>
@@ -1462,48 +1459,48 @@
         <v>3075</v>
       </c>
       <c r="B6" s="1">
-        <v>3105</v>
+        <v>3070</v>
       </c>
       <c r="C6" s="1">
-        <v>3020</v>
+        <v>3115</v>
       </c>
       <c r="D6" s="1">
-        <v>3120</v>
+        <v>3080</v>
       </c>
       <c r="E6" s="1">
-        <v>3050</v>
+        <v>3170</v>
       </c>
       <c r="F6" s="1">
-        <v>3190</v>
+        <v>3090</v>
       </c>
       <c r="G6" s="1">
-        <v>3005</v>
+        <v>3015</v>
       </c>
       <c r="H6" s="1">
-        <v>3075</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3130</v>
-      </c>
-      <c r="J6" s="1">
-        <v>3015</v>
-      </c>
-      <c r="K6" s="1">
-        <v>3065</v>
-      </c>
-      <c r="L6" s="1">
-        <v>3120</v>
-      </c>
-      <c r="M6" s="1">
-        <v>3050</v>
+        <v>3115</v>
+      </c>
+      <c r="I6" s="7">
+        <v>3025</v>
+      </c>
+      <c r="J6" s="8">
+        <v>3060</v>
+      </c>
+      <c r="K6" s="8">
+        <v>3080</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2945</v>
+      </c>
+      <c r="M6" s="5">
+        <v>3135</v>
       </c>
       <c r="N6" s="12">
         <f t="shared" ref="N6:N21" si="1">MIN(B6:M6)</f>
-        <v>3005</v>
+        <v>2945</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" ref="O6:O21" si="2">MIN(A6,N6)</f>
-        <v>3005</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
@@ -1511,44 +1508,44 @@
         <v>1965</v>
       </c>
       <c r="B7" s="1">
-        <v>1980</v>
+        <v>2045</v>
       </c>
       <c r="C7" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="1">
         <v>2020</v>
       </c>
-      <c r="D7" s="1">
-        <v>1970</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2010</v>
-      </c>
       <c r="F7" s="1">
-        <v>2005</v>
+        <v>1990</v>
       </c>
       <c r="G7" s="1">
+        <v>1990</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1985</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2020</v>
+      </c>
+      <c r="J7" s="8">
         <v>1995</v>
       </c>
-      <c r="H7" s="1">
-        <v>2000</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1990</v>
-      </c>
-      <c r="J7" s="1">
-        <v>2030</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1990</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1990</v>
-      </c>
-      <c r="M7" s="1">
-        <v>2020</v>
+      <c r="K7" s="8">
+        <v>2015</v>
+      </c>
+      <c r="L7" s="8">
+        <v>2035</v>
+      </c>
+      <c r="M7" s="5">
+        <v>2035</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" si="1"/>
-        <v>1970</v>
+        <v>1985</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="2"/>
@@ -1560,48 +1557,48 @@
         <v>2310</v>
       </c>
       <c r="B8" s="1">
+        <v>2345</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2370</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2335</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2380</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2295</v>
+      </c>
+      <c r="G8" s="1">
         <v>2320</v>
       </c>
-      <c r="C8" s="1">
+      <c r="H8" s="1">
         <v>2325</v>
       </c>
-      <c r="D8" s="1">
+      <c r="I8" s="7">
+        <v>2270</v>
+      </c>
+      <c r="J8" s="8">
+        <v>2365</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2305</v>
+      </c>
+      <c r="L8" s="8">
+        <v>2380</v>
+      </c>
+      <c r="M8" s="5">
         <v>2330</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2295</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2365</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2330</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2380</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2340</v>
-      </c>
-      <c r="J8" s="1">
-        <v>2340</v>
-      </c>
-      <c r="K8" s="1">
-        <v>2305</v>
-      </c>
-      <c r="L8" s="1">
-        <v>2355</v>
-      </c>
-      <c r="M8" s="1">
-        <v>2350</v>
       </c>
       <c r="N8" s="12">
         <f t="shared" si="1"/>
-        <v>2295</v>
+        <v>2270</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="2"/>
-        <v>2295</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
@@ -1609,44 +1606,44 @@
         <v>3195</v>
       </c>
       <c r="B9" s="1">
-        <v>3220</v>
+        <v>3360</v>
       </c>
       <c r="C9" s="1">
+        <v>3210</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3310</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3245</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3380</v>
+      </c>
+      <c r="G9" s="1">
         <v>3295</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3315</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3325</v>
-      </c>
-      <c r="F9" s="1">
-        <v>3375</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3305</v>
       </c>
       <c r="H9" s="1">
         <v>3330</v>
       </c>
-      <c r="I9" s="1">
-        <v>3320</v>
-      </c>
-      <c r="J9" s="1">
-        <v>3300</v>
-      </c>
-      <c r="K9" s="1">
-        <v>3305</v>
-      </c>
-      <c r="L9" s="1">
-        <v>3325</v>
-      </c>
-      <c r="M9" s="1">
-        <v>3195</v>
+      <c r="I9" s="7">
+        <v>3330</v>
+      </c>
+      <c r="J9" s="8">
+        <v>3330</v>
+      </c>
+      <c r="K9" s="8">
+        <v>3215</v>
+      </c>
+      <c r="L9" s="8">
+        <v>3390</v>
+      </c>
+      <c r="M9" s="5">
+        <v>3285</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="1"/>
-        <v>3195</v>
+        <v>3210</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="2"/>
@@ -1658,44 +1655,44 @@
         <v>2065</v>
       </c>
       <c r="B10" s="1">
-        <v>2175</v>
+        <v>2110</v>
       </c>
       <c r="C10" s="1">
+        <v>2245</v>
+      </c>
+      <c r="D10" s="1">
         <v>2150</v>
       </c>
-      <c r="D10" s="1">
-        <v>2160</v>
-      </c>
       <c r="E10" s="1">
+        <v>2115</v>
+      </c>
+      <c r="F10" s="1">
         <v>2190</v>
       </c>
-      <c r="F10" s="1">
-        <v>2205</v>
-      </c>
       <c r="G10" s="1">
-        <v>2155</v>
+        <v>2145</v>
       </c>
       <c r="H10" s="1">
         <v>2165</v>
       </c>
-      <c r="I10" s="1">
-        <v>2090</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="I10" s="7">
+        <v>2215</v>
+      </c>
+      <c r="J10" s="8">
+        <v>2210</v>
+      </c>
+      <c r="K10" s="8">
+        <v>2115</v>
+      </c>
+      <c r="L10" s="8">
         <v>2185</v>
       </c>
-      <c r="K10" s="1">
-        <v>2090</v>
-      </c>
-      <c r="L10" s="1">
-        <v>2070</v>
-      </c>
-      <c r="M10" s="1">
-        <v>2090</v>
+      <c r="M10" s="5">
+        <v>2130</v>
       </c>
       <c r="N10" s="12">
         <f t="shared" si="1"/>
-        <v>2070</v>
+        <v>2110</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="2"/>
@@ -1707,48 +1704,48 @@
         <v>3545</v>
       </c>
       <c r="B11" s="1">
-        <v>3780</v>
+        <v>3790</v>
       </c>
       <c r="C11" s="1">
-        <v>3685</v>
+        <v>3525</v>
       </c>
       <c r="D11" s="1">
-        <v>3725</v>
+        <v>3620</v>
       </c>
       <c r="E11" s="1">
-        <v>3600</v>
+        <v>3670</v>
       </c>
       <c r="F11" s="1">
-        <v>3665</v>
+        <v>3525</v>
       </c>
       <c r="G11" s="1">
-        <v>3685</v>
+        <v>3625</v>
       </c>
       <c r="H11" s="1">
-        <v>3630</v>
-      </c>
-      <c r="I11" s="1">
-        <v>3580</v>
-      </c>
-      <c r="J11" s="1">
-        <v>3665</v>
-      </c>
-      <c r="K11" s="1">
-        <v>3685</v>
-      </c>
-      <c r="L11" s="1">
+        <v>3535</v>
+      </c>
+      <c r="I11" s="7">
+        <v>3640</v>
+      </c>
+      <c r="J11" s="8">
+        <v>3525</v>
+      </c>
+      <c r="K11" s="8">
+        <v>3555</v>
+      </c>
+      <c r="L11" s="8">
         <v>3620</v>
       </c>
-      <c r="M11" s="1">
-        <v>3505</v>
+      <c r="M11" s="5">
+        <v>3670</v>
       </c>
       <c r="N11" s="12">
         <f t="shared" si="1"/>
-        <v>3505</v>
+        <v>3525</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="2"/>
-        <v>3505</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
@@ -1756,48 +1753,48 @@
         <v>2250</v>
       </c>
       <c r="B12" s="1">
-        <v>2265</v>
+        <v>2295</v>
       </c>
       <c r="C12" s="1">
-        <v>2285</v>
+        <v>2290</v>
       </c>
       <c r="D12" s="1">
-        <v>2320</v>
+        <v>2330</v>
       </c>
       <c r="E12" s="1">
-        <v>2290</v>
+        <v>2280</v>
       </c>
       <c r="F12" s="1">
-        <v>2340</v>
+        <v>2305</v>
       </c>
       <c r="G12" s="1">
         <v>2340</v>
       </c>
       <c r="H12" s="1">
-        <v>2250</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2220</v>
-      </c>
-      <c r="J12" s="1">
-        <v>2345</v>
-      </c>
-      <c r="K12" s="1">
-        <v>2275</v>
-      </c>
-      <c r="L12" s="1">
-        <v>2210</v>
-      </c>
-      <c r="M12" s="1">
+        <v>2300</v>
+      </c>
+      <c r="I12" s="7">
+        <v>2310</v>
+      </c>
+      <c r="J12" s="8">
         <v>2335</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2330</v>
+      </c>
+      <c r="L12" s="8">
+        <v>2285</v>
+      </c>
+      <c r="M12" s="5">
+        <v>2280</v>
       </c>
       <c r="N12" s="12">
         <f t="shared" si="1"/>
-        <v>2210</v>
+        <v>2280</v>
       </c>
       <c r="O12" s="3">
         <f t="shared" si="2"/>
-        <v>2210</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
@@ -1805,44 +1802,44 @@
         <v>6800</v>
       </c>
       <c r="B13" s="1">
-        <v>6830</v>
+        <v>7080</v>
       </c>
       <c r="C13" s="1">
-        <v>6880</v>
+        <v>6850</v>
       </c>
       <c r="D13" s="1">
-        <v>6855</v>
+        <v>6950</v>
       </c>
       <c r="E13" s="1">
-        <v>6850</v>
+        <v>6930</v>
       </c>
       <c r="F13" s="1">
-        <v>6870</v>
+        <v>6980</v>
       </c>
       <c r="G13" s="1">
-        <v>6850</v>
+        <v>6990</v>
       </c>
       <c r="H13" s="1">
-        <v>6830</v>
-      </c>
-      <c r="I13" s="1">
+        <v>7030</v>
+      </c>
+      <c r="I13" s="7">
+        <v>6980</v>
+      </c>
+      <c r="J13" s="8">
         <v>7000</v>
       </c>
-      <c r="J13" s="1">
-        <v>7005</v>
-      </c>
-      <c r="K13" s="1">
-        <v>6990</v>
-      </c>
-      <c r="L13" s="1">
-        <v>7085</v>
-      </c>
-      <c r="M13" s="1">
-        <v>6920</v>
+      <c r="K13" s="8">
+        <v>6945</v>
+      </c>
+      <c r="L13" s="8">
+        <v>6860</v>
+      </c>
+      <c r="M13" s="5">
+        <v>7010</v>
       </c>
       <c r="N13" s="12">
         <f t="shared" si="1"/>
-        <v>6830</v>
+        <v>6850</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" si="2"/>
@@ -1854,48 +1851,48 @@
         <v>2800</v>
       </c>
       <c r="B14" s="1">
-        <v>2810</v>
+        <v>2955</v>
       </c>
       <c r="C14" s="1">
-        <v>2795</v>
+        <v>2905</v>
       </c>
       <c r="D14" s="1">
-        <v>2780</v>
+        <v>2930</v>
       </c>
       <c r="E14" s="1">
-        <v>2860</v>
+        <v>2960</v>
       </c>
       <c r="F14" s="1">
-        <v>2950</v>
+        <v>2770</v>
       </c>
       <c r="G14" s="1">
         <v>2895</v>
       </c>
       <c r="H14" s="1">
-        <v>2925</v>
-      </c>
-      <c r="I14" s="1">
-        <v>2795</v>
-      </c>
-      <c r="J14" s="1">
-        <v>2845</v>
-      </c>
-      <c r="K14" s="1">
-        <v>2890</v>
-      </c>
-      <c r="L14" s="1">
-        <v>2835</v>
-      </c>
-      <c r="M14" s="1">
-        <v>2865</v>
+        <v>2850</v>
+      </c>
+      <c r="I14" s="7">
+        <v>2910</v>
+      </c>
+      <c r="J14" s="8">
+        <v>2850</v>
+      </c>
+      <c r="K14" s="8">
+        <v>2900</v>
+      </c>
+      <c r="L14" s="8">
+        <v>2945</v>
+      </c>
+      <c r="M14" s="5">
+        <v>2825</v>
       </c>
       <c r="N14" s="12">
         <f t="shared" si="1"/>
-        <v>2780</v>
+        <v>2770</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="2"/>
-        <v>2780</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
@@ -1903,48 +1900,48 @@
         <v>3780</v>
       </c>
       <c r="B15" s="1">
-        <v>3760</v>
+        <v>3920</v>
       </c>
       <c r="C15" s="1">
-        <v>4025</v>
+        <v>4015</v>
       </c>
       <c r="D15" s="1">
-        <v>4085</v>
+        <v>3920</v>
       </c>
       <c r="E15" s="1">
-        <v>4010</v>
+        <v>3830</v>
       </c>
       <c r="F15" s="1">
-        <v>4065</v>
+        <v>3950</v>
       </c>
       <c r="G15" s="1">
-        <v>3820</v>
+        <v>3985</v>
       </c>
       <c r="H15" s="1">
-        <v>3795</v>
-      </c>
-      <c r="I15" s="1">
-        <v>3915</v>
-      </c>
-      <c r="J15" s="1">
-        <v>3915</v>
-      </c>
-      <c r="K15" s="1">
-        <v>3855</v>
-      </c>
-      <c r="L15" s="1">
-        <v>3880</v>
-      </c>
-      <c r="M15" s="1">
-        <v>3740</v>
+        <v>3885</v>
+      </c>
+      <c r="I15" s="7">
+        <v>4005</v>
+      </c>
+      <c r="J15" s="8">
+        <v>3935</v>
+      </c>
+      <c r="K15" s="8">
+        <v>4045</v>
+      </c>
+      <c r="L15" s="8">
+        <v>3845</v>
+      </c>
+      <c r="M15" s="5">
+        <v>3830</v>
       </c>
       <c r="N15" s="12">
         <f t="shared" si="1"/>
-        <v>3740</v>
+        <v>3830</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="2"/>
-        <v>3740</v>
+        <v>3780</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
@@ -1952,48 +1949,48 @@
         <v>3950</v>
       </c>
       <c r="B16" s="1">
-        <v>4045</v>
+        <v>4200</v>
       </c>
       <c r="C16" s="1">
-        <v>3995</v>
+        <v>4135</v>
       </c>
       <c r="D16" s="1">
-        <v>4060</v>
+        <v>4125</v>
       </c>
       <c r="E16" s="1">
-        <v>4005</v>
+        <v>4145</v>
       </c>
       <c r="F16" s="1">
-        <v>4010</v>
+        <v>3940</v>
       </c>
       <c r="G16" s="1">
-        <v>4040</v>
+        <v>4025</v>
       </c>
       <c r="H16" s="1">
-        <v>4040</v>
-      </c>
-      <c r="I16" s="1">
-        <v>4025</v>
-      </c>
-      <c r="J16" s="1">
-        <v>3950</v>
-      </c>
-      <c r="K16" s="1">
-        <v>4000</v>
-      </c>
-      <c r="L16" s="1">
-        <v>4145</v>
-      </c>
-      <c r="M16" s="1">
-        <v>4025</v>
+        <v>4090</v>
+      </c>
+      <c r="I16" s="7">
+        <v>4100</v>
+      </c>
+      <c r="J16" s="8">
+        <v>4080</v>
+      </c>
+      <c r="K16" s="8">
+        <v>3960</v>
+      </c>
+      <c r="L16" s="8">
+        <v>4055</v>
+      </c>
+      <c r="M16" s="5">
+        <v>4075</v>
       </c>
       <c r="N16" s="12">
         <f t="shared" si="1"/>
-        <v>3950</v>
+        <v>3940</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="2"/>
-        <v>3950</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
@@ -2001,48 +1998,48 @@
         <v>5940</v>
       </c>
       <c r="B17" s="1">
-        <v>6090</v>
+        <v>6120</v>
       </c>
       <c r="C17" s="1">
-        <v>6155</v>
+        <v>6025</v>
       </c>
       <c r="D17" s="1">
-        <v>6195</v>
+        <v>6010</v>
       </c>
       <c r="E17" s="1">
-        <v>6155</v>
+        <v>6100</v>
       </c>
       <c r="F17" s="1">
-        <v>6010</v>
+        <v>5995</v>
       </c>
       <c r="G17" s="1">
-        <v>6075</v>
+        <v>6110</v>
       </c>
       <c r="H17" s="1">
+        <v>6025</v>
+      </c>
+      <c r="I17" s="7">
         <v>6070</v>
       </c>
-      <c r="I17" s="1">
-        <v>6055</v>
-      </c>
-      <c r="J17" s="1">
-        <v>5930</v>
-      </c>
-      <c r="K17" s="1">
-        <v>5940</v>
-      </c>
-      <c r="L17" s="1">
-        <v>6120</v>
-      </c>
-      <c r="M17" s="1">
-        <v>5945</v>
+      <c r="J17" s="8">
+        <v>6190</v>
+      </c>
+      <c r="K17" s="8">
+        <v>6070</v>
+      </c>
+      <c r="L17" s="8">
+        <v>5950</v>
+      </c>
+      <c r="M17" s="5">
+        <v>6100</v>
       </c>
       <c r="N17" s="12">
         <f t="shared" si="1"/>
-        <v>5930</v>
+        <v>5950</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="2"/>
-        <v>5930</v>
+        <v>5940</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
@@ -2050,48 +2047,48 @@
         <v>2995</v>
       </c>
       <c r="B18" s="1">
-        <v>3040</v>
+        <v>3125</v>
       </c>
       <c r="C18" s="1">
-        <v>3105</v>
+        <v>3120</v>
       </c>
       <c r="D18" s="1">
+        <v>3015</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3255</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2995</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3075</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3110</v>
+      </c>
+      <c r="I18" s="7">
         <v>3030</v>
       </c>
-      <c r="E18" s="1">
-        <v>2930</v>
-      </c>
-      <c r="F18" s="1">
-        <v>3070</v>
-      </c>
-      <c r="G18" s="1">
-        <v>3100</v>
-      </c>
-      <c r="H18" s="1">
-        <v>3010</v>
-      </c>
-      <c r="I18" s="1">
-        <v>2965</v>
-      </c>
-      <c r="J18" s="1">
-        <v>3095</v>
-      </c>
-      <c r="K18" s="1">
-        <v>3040</v>
-      </c>
-      <c r="L18" s="1">
-        <v>3150</v>
-      </c>
-      <c r="M18" s="1">
-        <v>3070</v>
+      <c r="J18" s="8">
+        <v>3065</v>
+      </c>
+      <c r="K18" s="8">
+        <v>3015</v>
+      </c>
+      <c r="L18" s="8">
+        <v>3025</v>
+      </c>
+      <c r="M18" s="5">
+        <v>2990</v>
       </c>
       <c r="N18" s="12">
         <f t="shared" si="1"/>
-        <v>2930</v>
+        <v>2990</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="2"/>
-        <v>2930</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
@@ -2099,48 +2096,48 @@
         <v>5060</v>
       </c>
       <c r="B19" s="1">
-        <v>5285</v>
+        <v>5525</v>
       </c>
       <c r="C19" s="1">
-        <v>5150</v>
+        <v>5145</v>
       </c>
       <c r="D19" s="1">
-        <v>5390</v>
+        <v>5170</v>
       </c>
       <c r="E19" s="1">
-        <v>5305</v>
+        <v>5315</v>
       </c>
       <c r="F19" s="1">
-        <v>5105</v>
+        <v>5175</v>
       </c>
       <c r="G19" s="1">
-        <v>5190</v>
+        <v>5160</v>
       </c>
       <c r="H19" s="1">
-        <v>5370</v>
-      </c>
-      <c r="I19" s="1">
-        <v>5055</v>
-      </c>
-      <c r="J19" s="1">
-        <v>5255</v>
-      </c>
-      <c r="K19" s="1">
-        <v>5170</v>
-      </c>
-      <c r="L19" s="1">
-        <v>5220</v>
-      </c>
-      <c r="M19" s="1">
-        <v>5140</v>
+        <v>5180</v>
+      </c>
+      <c r="I19" s="7">
+        <v>5095</v>
+      </c>
+      <c r="J19" s="8">
+        <v>5185</v>
+      </c>
+      <c r="K19" s="8">
+        <v>5165</v>
+      </c>
+      <c r="L19" s="8">
+        <v>5060</v>
+      </c>
+      <c r="M19" s="5">
+        <v>5355</v>
       </c>
       <c r="N19" s="12">
         <f t="shared" si="1"/>
-        <v>5055</v>
+        <v>5060</v>
       </c>
       <c r="O19" s="3">
         <f t="shared" si="2"/>
-        <v>5055</v>
+        <v>5060</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
@@ -2148,48 +2145,48 @@
         <v>2925</v>
       </c>
       <c r="B20" s="1">
-        <v>2985</v>
+        <v>2980</v>
       </c>
       <c r="C20" s="1">
-        <v>2960</v>
+        <v>2885</v>
       </c>
       <c r="D20" s="1">
-        <v>2845</v>
+        <v>2945</v>
       </c>
       <c r="E20" s="1">
-        <v>2935</v>
+        <v>3050</v>
       </c>
       <c r="F20" s="1">
-        <v>3060</v>
+        <v>3000</v>
       </c>
       <c r="G20" s="1">
-        <v>2835</v>
+        <v>2885</v>
       </c>
       <c r="H20" s="1">
-        <v>2925</v>
-      </c>
-      <c r="I20" s="1">
-        <v>2970</v>
-      </c>
-      <c r="J20" s="1">
-        <v>3000</v>
-      </c>
-      <c r="K20" s="1">
-        <v>2815</v>
-      </c>
-      <c r="L20" s="1">
-        <v>2960</v>
-      </c>
-      <c r="M20" s="1">
-        <v>2765</v>
+        <v>2915</v>
+      </c>
+      <c r="I20" s="7">
+        <v>2995</v>
+      </c>
+      <c r="J20" s="8">
+        <v>2990</v>
+      </c>
+      <c r="K20" s="8">
+        <v>3045</v>
+      </c>
+      <c r="L20" s="8">
+        <v>3015</v>
+      </c>
+      <c r="M20" s="5">
+        <v>2980</v>
       </c>
       <c r="N20" s="12">
         <f t="shared" si="1"/>
-        <v>2765</v>
+        <v>2885</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" si="2"/>
-        <v>2765</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
@@ -2197,48 +2194,48 @@
         <v>5315</v>
       </c>
       <c r="B21" s="1">
-        <v>5235</v>
+        <v>5405</v>
       </c>
       <c r="C21" s="1">
-        <v>5460</v>
+        <v>5595</v>
       </c>
       <c r="D21" s="1">
-        <v>5490</v>
+        <v>5425</v>
       </c>
       <c r="E21" s="1">
-        <v>5420</v>
+        <v>5375</v>
       </c>
       <c r="F21" s="1">
-        <v>5565</v>
+        <v>5685</v>
       </c>
       <c r="G21" s="1">
-        <v>5190</v>
+        <v>5150</v>
       </c>
       <c r="H21" s="1">
-        <v>5440</v>
-      </c>
-      <c r="I21" s="1">
-        <v>5475</v>
-      </c>
-      <c r="J21" s="1">
-        <v>5360</v>
-      </c>
-      <c r="K21" s="1">
-        <v>5410</v>
-      </c>
-      <c r="L21" s="1">
-        <v>5340</v>
-      </c>
-      <c r="M21" s="1">
-        <v>5335</v>
+        <v>5355</v>
+      </c>
+      <c r="I21" s="7">
+        <v>5305</v>
+      </c>
+      <c r="J21" s="8">
+        <v>5705</v>
+      </c>
+      <c r="K21" s="8">
+        <v>5600</v>
+      </c>
+      <c r="L21" s="8">
+        <v>5365</v>
+      </c>
+      <c r="M21" s="5">
+        <v>5305</v>
       </c>
       <c r="N21" s="12">
         <f t="shared" si="1"/>
-        <v>5190</v>
+        <v>5150</v>
       </c>
       <c r="O21" s="3">
         <f t="shared" si="2"/>
-        <v>5190</v>
+        <v>5150</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
@@ -2443,8 +2440,9 @@
       <c r="G88" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:N1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:M1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:Z128">

</xml_diff>

<commit_message>
new implementation for swap chain. bug fix on swap chain. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="36720" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="37890" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>TSR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;w1,w1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -45,11 +41,39 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>0.5;w1,w1</t>
+    <t>ACEBR_BNP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_FNF</t>
+    <t>ACEBR_BNR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACEBR_BAO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACEBR_BNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACEBR_FNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACEBR_FAO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BAO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_FAO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -57,35 +81,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_BAF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_BAP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_BNO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ACBR_BNP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_FAO</t>
+    <t>ACBR_BNR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_FWF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_FWO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_BNR</t>
+    <t>1.5;w1,w1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -96,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,14 +257,6 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -784,7 +780,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -824,12 +820,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -847,6 +846,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1216,7 +1221,7 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1236,58 +1241,56 @@
   <sheetData>
     <row r="1" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
-      <c r="B1" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="20"/>
-      <c r="I1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="14"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>7</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>15</v>
@@ -1296,18 +1299,18 @@
         <v>16</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1319,10 +1322,10 @@
       <c r="F3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -1331,13 +1334,13 @@
       <c r="J3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="6" t="s">
@@ -1345,64 +1348,65 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
-        <v>3501.7647058823532</v>
+      <c r="A4" s="9">
+        <f>AVERAGE(A5:A128)</f>
+        <v>3475.8823529411766</v>
       </c>
       <c r="B4" s="9">
         <f>AVERAGE(B5:B128)</f>
-        <v>3640.294117647059</v>
+        <v>3664.1176470588234</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ref="C4:O4" si="0">AVERAGE(C5:C128)</f>
-        <v>3593.5294117647059</v>
+        <v>3690.294117647059</v>
       </c>
       <c r="D4" s="4">
         <f>AVERAGE(D5:D128)</f>
-        <v>3585</v>
+        <v>3639.705882352941</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>3614.1176470588234</v>
+        <v>3669.1176470588234</v>
       </c>
       <c r="F4" s="4">
         <f>AVERAGE(F5:F128)</f>
-        <v>3577.9411764705883</v>
+        <v>3667.9411764705883</v>
       </c>
       <c r="G4" s="11">
         <f t="shared" si="0"/>
-        <v>3562.6470588235293</v>
+        <v>3684.4117647058824</v>
       </c>
       <c r="H4" s="10">
         <f t="shared" si="0"/>
-        <v>3575.294117647059</v>
+        <v>3567.6470588235293</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="0"/>
-        <v>3584.1176470588234</v>
+        <v>3541.1764705882351</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
-        <v>3613.5294117647059</v>
+        <v>3597.0588235294117</v>
       </c>
       <c r="K4" s="10">
         <f t="shared" si="0"/>
-        <v>3589.4117647058824</v>
+        <v>3579.4117647058824</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>3563.2352941176468</v>
+        <v>3580.294117647059</v>
       </c>
       <c r="M4" s="9">
         <f t="shared" si="0"/>
-        <v>3582.0588235294117</v>
+        <v>3575</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
-        <v>3488.8235294117649</v>
+        <v>3473.8235294117649</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>3475.8823529411766</v>
+        <v>3446.7647058823532</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
@@ -1410,44 +1414,44 @@
         <v>1560</v>
       </c>
       <c r="B5" s="1">
-        <v>1560</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1610</v>
+        <v>1585</v>
+      </c>
+      <c r="C5">
+        <v>1630</v>
       </c>
       <c r="D5" s="1">
         <v>1630</v>
       </c>
-      <c r="E5" s="1">
-        <v>1600</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1560</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1560</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1585</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="E5">
         <v>1630</v>
       </c>
-      <c r="J5" s="8">
+      <c r="F5">
+        <v>1605</v>
+      </c>
+      <c r="G5">
+        <v>1630</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1635</v>
+      </c>
+      <c r="I5" s="22">
         <v>1610</v>
       </c>
-      <c r="K5" s="8">
+      <c r="J5" s="22">
         <v>1660</v>
       </c>
-      <c r="L5" s="8">
-        <v>1615</v>
-      </c>
-      <c r="M5" s="5">
-        <v>1560</v>
+      <c r="K5" s="22">
+        <v>1640</v>
+      </c>
+      <c r="L5" s="22">
+        <v>1570</v>
+      </c>
+      <c r="M5" s="23">
+        <v>1630</v>
       </c>
       <c r="N5" s="12">
         <f>MIN(B5:M5)</f>
-        <v>1560</v>
+        <v>1570</v>
       </c>
       <c r="O5" s="3">
         <f>MIN(A5,N5)</f>
@@ -1456,47 +1460,47 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>3075</v>
+        <v>2945</v>
       </c>
       <c r="B6" s="1">
-        <v>3070</v>
-      </c>
-      <c r="C6" s="1">
         <v>3115</v>
       </c>
+      <c r="C6">
+        <v>3100</v>
+      </c>
       <c r="D6" s="1">
+        <v>3045</v>
+      </c>
+      <c r="E6">
+        <v>3100</v>
+      </c>
+      <c r="F6">
+        <v>3090</v>
+      </c>
+      <c r="G6">
+        <v>3165</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3065</v>
+      </c>
+      <c r="I6" s="22">
+        <v>3085</v>
+      </c>
+      <c r="J6" s="22">
+        <v>3140</v>
+      </c>
+      <c r="K6" s="22">
         <v>3080</v>
       </c>
-      <c r="E6" s="1">
-        <v>3170</v>
-      </c>
-      <c r="F6" s="1">
-        <v>3090</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3015</v>
-      </c>
-      <c r="H6" s="1">
-        <v>3115</v>
-      </c>
-      <c r="I6" s="7">
-        <v>3025</v>
-      </c>
-      <c r="J6" s="8">
-        <v>3060</v>
-      </c>
-      <c r="K6" s="8">
-        <v>3080</v>
-      </c>
-      <c r="L6" s="8">
-        <v>2945</v>
-      </c>
-      <c r="M6" s="5">
-        <v>3135</v>
+      <c r="L6" s="22">
+        <v>3045</v>
+      </c>
+      <c r="M6" s="23">
+        <v>3055</v>
       </c>
       <c r="N6" s="12">
         <f t="shared" ref="N6:N21" si="1">MIN(B6:M6)</f>
-        <v>2945</v>
+        <v>3045</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" ref="O6:O21" si="2">MIN(A6,N6)</f>
@@ -1508,44 +1512,44 @@
         <v>1965</v>
       </c>
       <c r="B7" s="1">
+        <v>2040</v>
+      </c>
+      <c r="C7">
+        <v>2035</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2060</v>
+      </c>
+      <c r="E7">
         <v>2045</v>
       </c>
-      <c r="C7" s="1">
-        <v>2050</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="F7">
+        <v>2065</v>
+      </c>
+      <c r="G7">
+        <v>2025</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2005</v>
+      </c>
+      <c r="I7" s="22">
+        <v>2015</v>
+      </c>
+      <c r="J7" s="22">
+        <v>2010</v>
+      </c>
+      <c r="K7" s="22">
         <v>2020</v>
       </c>
-      <c r="F7" s="1">
-        <v>1990</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1990</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1985</v>
-      </c>
-      <c r="I7" s="7">
-        <v>2020</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1995</v>
-      </c>
-      <c r="K7" s="8">
+      <c r="L7" s="22">
         <v>2015</v>
       </c>
-      <c r="L7" s="8">
-        <v>2035</v>
-      </c>
-      <c r="M7" s="5">
-        <v>2035</v>
+      <c r="M7" s="23">
+        <v>2015</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" si="1"/>
-        <v>1985</v>
+        <v>2005</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="2"/>
@@ -1554,47 +1558,47 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
+        <v>2270</v>
+      </c>
+      <c r="B8" s="1">
         <v>2310</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8">
+        <v>2365</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2325</v>
+      </c>
+      <c r="E8">
+        <v>2365</v>
+      </c>
+      <c r="F8">
+        <v>2340</v>
+      </c>
+      <c r="G8">
         <v>2345</v>
       </c>
-      <c r="C8" s="1">
-        <v>2370</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="H8" s="7">
         <v>2335</v>
       </c>
-      <c r="E8" s="1">
-        <v>2380</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2295</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2320</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="I8" s="22">
+        <v>2355</v>
+      </c>
+      <c r="J8" s="22">
+        <v>2285</v>
+      </c>
+      <c r="K8" s="22">
+        <v>2350</v>
+      </c>
+      <c r="L8" s="22">
+        <v>2340</v>
+      </c>
+      <c r="M8" s="23">
         <v>2325</v>
-      </c>
-      <c r="I8" s="7">
-        <v>2270</v>
-      </c>
-      <c r="J8" s="8">
-        <v>2365</v>
-      </c>
-      <c r="K8" s="8">
-        <v>2305</v>
-      </c>
-      <c r="L8" s="8">
-        <v>2380</v>
-      </c>
-      <c r="M8" s="5">
-        <v>2330</v>
       </c>
       <c r="N8" s="12">
         <f t="shared" si="1"/>
-        <v>2270</v>
+        <v>2285</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="2"/>
@@ -1606,48 +1610,48 @@
         <v>3195</v>
       </c>
       <c r="B9" s="1">
+        <v>3260</v>
+      </c>
+      <c r="C9">
+        <v>3410</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3365</v>
+      </c>
+      <c r="E9">
+        <v>3370</v>
+      </c>
+      <c r="F9">
+        <v>3275</v>
+      </c>
+      <c r="G9">
+        <v>3550</v>
+      </c>
+      <c r="H9" s="7">
+        <v>3305</v>
+      </c>
+      <c r="I9" s="22">
+        <v>3280</v>
+      </c>
+      <c r="J9" s="22">
+        <v>3455</v>
+      </c>
+      <c r="K9" s="22">
+        <v>3265</v>
+      </c>
+      <c r="L9" s="22">
         <v>3360</v>
       </c>
-      <c r="C9" s="1">
-        <v>3210</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3310</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3245</v>
-      </c>
-      <c r="F9" s="1">
-        <v>3380</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3295</v>
-      </c>
-      <c r="H9" s="1">
-        <v>3330</v>
-      </c>
-      <c r="I9" s="7">
-        <v>3330</v>
-      </c>
-      <c r="J9" s="8">
-        <v>3330</v>
-      </c>
-      <c r="K9" s="8">
-        <v>3215</v>
-      </c>
-      <c r="L9" s="8">
-        <v>3390</v>
-      </c>
-      <c r="M9" s="5">
-        <v>3285</v>
+      <c r="M9" s="23">
+        <v>3185</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="1"/>
-        <v>3210</v>
+        <v>3185</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="2"/>
-        <v>3195</v>
+        <v>3185</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
@@ -1655,44 +1659,44 @@
         <v>2065</v>
       </c>
       <c r="B10" s="1">
-        <v>2110</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2245</v>
+        <v>2185</v>
+      </c>
+      <c r="C10">
+        <v>2145</v>
       </c>
       <c r="D10" s="1">
-        <v>2150</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2115</v>
-      </c>
-      <c r="F10" s="1">
+        <v>2130</v>
+      </c>
+      <c r="E10">
+        <v>2100</v>
+      </c>
+      <c r="F10">
         <v>2190</v>
       </c>
-      <c r="G10" s="1">
-        <v>2145</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="G10">
+        <v>2200</v>
+      </c>
+      <c r="H10" s="7">
+        <v>2130</v>
+      </c>
+      <c r="I10" s="22">
         <v>2165</v>
       </c>
-      <c r="I10" s="7">
-        <v>2215</v>
-      </c>
-      <c r="J10" s="8">
-        <v>2210</v>
-      </c>
-      <c r="K10" s="8">
-        <v>2115</v>
-      </c>
-      <c r="L10" s="8">
-        <v>2185</v>
-      </c>
-      <c r="M10" s="5">
-        <v>2130</v>
+      <c r="J10" s="22">
+        <v>2190</v>
+      </c>
+      <c r="K10" s="22">
+        <v>2135</v>
+      </c>
+      <c r="L10" s="22">
+        <v>2070</v>
+      </c>
+      <c r="M10" s="23">
+        <v>2070</v>
       </c>
       <c r="N10" s="12">
         <f t="shared" si="1"/>
-        <v>2110</v>
+        <v>2070</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="2"/>
@@ -1701,51 +1705,51 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>3545</v>
+        <v>3525</v>
       </c>
       <c r="B11" s="1">
-        <v>3790</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3525</v>
+        <v>3465</v>
+      </c>
+      <c r="C11">
+        <v>3825</v>
       </c>
       <c r="D11" s="1">
-        <v>3620</v>
-      </c>
-      <c r="E11" s="1">
-        <v>3670</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3525</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3625</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3535</v>
-      </c>
-      <c r="I11" s="7">
-        <v>3640</v>
-      </c>
-      <c r="J11" s="8">
-        <v>3525</v>
-      </c>
-      <c r="K11" s="8">
-        <v>3555</v>
-      </c>
-      <c r="L11" s="8">
-        <v>3620</v>
-      </c>
-      <c r="M11" s="5">
-        <v>3670</v>
+        <v>3590</v>
+      </c>
+      <c r="E11">
+        <v>3695</v>
+      </c>
+      <c r="F11">
+        <v>3660</v>
+      </c>
+      <c r="G11">
+        <v>3615</v>
+      </c>
+      <c r="H11" s="7">
+        <v>3645</v>
+      </c>
+      <c r="I11" s="22">
+        <v>3655</v>
+      </c>
+      <c r="J11" s="22">
+        <v>3665</v>
+      </c>
+      <c r="K11" s="22">
+        <v>3565</v>
+      </c>
+      <c r="L11" s="22">
+        <v>3585</v>
+      </c>
+      <c r="M11" s="23">
+        <v>3650</v>
       </c>
       <c r="N11" s="12">
         <f t="shared" si="1"/>
-        <v>3525</v>
+        <v>3465</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="2"/>
-        <v>3525</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
@@ -1753,44 +1757,44 @@
         <v>2250</v>
       </c>
       <c r="B12" s="1">
-        <v>2295</v>
-      </c>
-      <c r="C12" s="1">
+        <v>2425</v>
+      </c>
+      <c r="C12">
+        <v>2385</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2395</v>
+      </c>
+      <c r="E12">
+        <v>2435</v>
+      </c>
+      <c r="F12">
+        <v>2425</v>
+      </c>
+      <c r="G12">
+        <v>2345</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2260</v>
+      </c>
+      <c r="I12" s="22">
+        <v>2320</v>
+      </c>
+      <c r="J12" s="22">
+        <v>2380</v>
+      </c>
+      <c r="K12" s="22">
+        <v>2340</v>
+      </c>
+      <c r="L12" s="22">
         <v>2290</v>
       </c>
-      <c r="D12" s="1">
-        <v>2330</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2280</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2305</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2340</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="M12" s="23">
         <v>2300</v>
-      </c>
-      <c r="I12" s="7">
-        <v>2310</v>
-      </c>
-      <c r="J12" s="8">
-        <v>2335</v>
-      </c>
-      <c r="K12" s="8">
-        <v>2330</v>
-      </c>
-      <c r="L12" s="8">
-        <v>2285</v>
-      </c>
-      <c r="M12" s="5">
-        <v>2280</v>
       </c>
       <c r="N12" s="12">
         <f t="shared" si="1"/>
-        <v>2280</v>
+        <v>2260</v>
       </c>
       <c r="O12" s="3">
         <f t="shared" si="2"/>
@@ -1802,44 +1806,44 @@
         <v>6800</v>
       </c>
       <c r="B13" s="1">
-        <v>7080</v>
-      </c>
-      <c r="C13" s="1">
-        <v>6850</v>
+        <v>7170</v>
+      </c>
+      <c r="C13">
+        <v>7270</v>
       </c>
       <c r="D13" s="1">
-        <v>6950</v>
-      </c>
-      <c r="E13" s="1">
-        <v>6930</v>
-      </c>
-      <c r="F13" s="1">
-        <v>6980</v>
-      </c>
-      <c r="G13" s="1">
-        <v>6990</v>
-      </c>
-      <c r="H13" s="1">
-        <v>7030</v>
-      </c>
-      <c r="I13" s="7">
-        <v>6980</v>
-      </c>
-      <c r="J13" s="8">
-        <v>7000</v>
-      </c>
-      <c r="K13" s="8">
-        <v>6945</v>
-      </c>
-      <c r="L13" s="8">
-        <v>6860</v>
-      </c>
-      <c r="M13" s="5">
-        <v>7010</v>
+        <v>7005</v>
+      </c>
+      <c r="E13">
+        <v>7110</v>
+      </c>
+      <c r="F13">
+        <v>7300</v>
+      </c>
+      <c r="G13">
+        <v>7225</v>
+      </c>
+      <c r="H13" s="7">
+        <v>7025</v>
+      </c>
+      <c r="I13" s="22">
+        <v>6890</v>
+      </c>
+      <c r="J13" s="22">
+        <v>7015</v>
+      </c>
+      <c r="K13" s="22">
+        <v>6935</v>
+      </c>
+      <c r="L13" s="22">
+        <v>7070</v>
+      </c>
+      <c r="M13" s="23">
+        <v>7100</v>
       </c>
       <c r="N13" s="12">
         <f t="shared" si="1"/>
-        <v>6850</v>
+        <v>6890</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" si="2"/>
@@ -1848,47 +1852,47 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>2800</v>
+        <v>2770</v>
       </c>
       <c r="B14" s="1">
-        <v>2955</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2905</v>
+        <v>3075</v>
+      </c>
+      <c r="C14">
+        <v>3040</v>
       </c>
       <c r="D14" s="1">
-        <v>2930</v>
-      </c>
-      <c r="E14" s="1">
-        <v>2960</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2770</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2895</v>
-      </c>
-      <c r="H14" s="1">
-        <v>2850</v>
-      </c>
-      <c r="I14" s="7">
+        <v>3095</v>
+      </c>
+      <c r="E14">
+        <v>2980</v>
+      </c>
+      <c r="F14">
+        <v>3060</v>
+      </c>
+      <c r="G14">
+        <v>3000</v>
+      </c>
+      <c r="H14" s="7">
+        <v>2840</v>
+      </c>
+      <c r="I14" s="22">
+        <v>2840</v>
+      </c>
+      <c r="J14" s="22">
         <v>2910</v>
       </c>
-      <c r="J14" s="8">
-        <v>2850</v>
-      </c>
-      <c r="K14" s="8">
-        <v>2900</v>
-      </c>
-      <c r="L14" s="8">
-        <v>2945</v>
-      </c>
-      <c r="M14" s="5">
-        <v>2825</v>
+      <c r="K14" s="22">
+        <v>2820</v>
+      </c>
+      <c r="L14" s="22">
+        <v>2875</v>
+      </c>
+      <c r="M14" s="23">
+        <v>2860</v>
       </c>
       <c r="N14" s="12">
         <f t="shared" si="1"/>
-        <v>2770</v>
+        <v>2820</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="2"/>
@@ -1900,93 +1904,93 @@
         <v>3780</v>
       </c>
       <c r="B15" s="1">
-        <v>3920</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4015</v>
+        <v>3835</v>
+      </c>
+      <c r="C15">
+        <v>4105</v>
       </c>
       <c r="D15" s="1">
-        <v>3920</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3830</v>
-      </c>
-      <c r="F15" s="1">
-        <v>3950</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3985</v>
-      </c>
-      <c r="H15" s="1">
-        <v>3885</v>
-      </c>
-      <c r="I15" s="7">
-        <v>4005</v>
-      </c>
-      <c r="J15" s="8">
-        <v>3935</v>
-      </c>
-      <c r="K15" s="8">
-        <v>4045</v>
-      </c>
-      <c r="L15" s="8">
-        <v>3845</v>
-      </c>
-      <c r="M15" s="5">
-        <v>3830</v>
+        <v>4040</v>
+      </c>
+      <c r="E15">
+        <v>4035</v>
+      </c>
+      <c r="F15">
+        <v>3975</v>
+      </c>
+      <c r="G15">
+        <v>3990</v>
+      </c>
+      <c r="H15" s="7">
+        <v>3875</v>
+      </c>
+      <c r="I15" s="22">
+        <v>3600</v>
+      </c>
+      <c r="J15" s="22">
+        <v>3875</v>
+      </c>
+      <c r="K15" s="22">
+        <v>3900</v>
+      </c>
+      <c r="L15" s="22">
+        <v>3965</v>
+      </c>
+      <c r="M15" s="23">
+        <v>3875</v>
       </c>
       <c r="N15" s="12">
         <f t="shared" si="1"/>
-        <v>3830</v>
+        <v>3600</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="2"/>
-        <v>3780</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>3950</v>
+        <v>3940</v>
       </c>
       <c r="B16" s="1">
-        <v>4200</v>
-      </c>
-      <c r="C16" s="1">
+        <v>4185</v>
+      </c>
+      <c r="C16">
+        <v>4140</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4075</v>
+      </c>
+      <c r="E16">
+        <v>4100</v>
+      </c>
+      <c r="F16">
+        <v>4015</v>
+      </c>
+      <c r="G16">
+        <v>4165</v>
+      </c>
+      <c r="H16" s="7">
+        <v>4070</v>
+      </c>
+      <c r="I16" s="22">
+        <v>4045</v>
+      </c>
+      <c r="J16" s="22">
+        <v>4105</v>
+      </c>
+      <c r="K16" s="22">
+        <v>4070</v>
+      </c>
+      <c r="L16" s="22">
         <v>4135</v>
       </c>
-      <c r="D16" s="1">
-        <v>4125</v>
-      </c>
-      <c r="E16" s="1">
-        <v>4145</v>
-      </c>
-      <c r="F16" s="1">
-        <v>3940</v>
-      </c>
-      <c r="G16" s="1">
-        <v>4025</v>
-      </c>
-      <c r="H16" s="1">
-        <v>4090</v>
-      </c>
-      <c r="I16" s="7">
-        <v>4100</v>
-      </c>
-      <c r="J16" s="8">
-        <v>4080</v>
-      </c>
-      <c r="K16" s="8">
-        <v>3960</v>
-      </c>
-      <c r="L16" s="8">
-        <v>4055</v>
-      </c>
-      <c r="M16" s="5">
-        <v>4075</v>
+      <c r="M16" s="23">
+        <v>4105</v>
       </c>
       <c r="N16" s="12">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>4015</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="2"/>
@@ -1998,44 +2002,44 @@
         <v>5940</v>
       </c>
       <c r="B17" s="1">
-        <v>6120</v>
-      </c>
-      <c r="C17" s="1">
-        <v>6025</v>
+        <v>6195</v>
+      </c>
+      <c r="C17">
+        <v>6255</v>
       </c>
       <c r="D17" s="1">
-        <v>6010</v>
-      </c>
-      <c r="E17" s="1">
-        <v>6100</v>
-      </c>
-      <c r="F17" s="1">
-        <v>5995</v>
-      </c>
-      <c r="G17" s="1">
-        <v>6110</v>
-      </c>
-      <c r="H17" s="1">
-        <v>6025</v>
-      </c>
-      <c r="I17" s="7">
-        <v>6070</v>
-      </c>
-      <c r="J17" s="8">
-        <v>6190</v>
-      </c>
-      <c r="K17" s="8">
-        <v>6070</v>
-      </c>
-      <c r="L17" s="8">
-        <v>5950</v>
-      </c>
-      <c r="M17" s="5">
-        <v>6100</v>
+        <v>5975</v>
+      </c>
+      <c r="E17">
+        <v>6185</v>
+      </c>
+      <c r="F17">
+        <v>6170</v>
+      </c>
+      <c r="G17">
+        <v>6295</v>
+      </c>
+      <c r="H17" s="7">
+        <v>5945</v>
+      </c>
+      <c r="I17" s="22">
+        <v>6090</v>
+      </c>
+      <c r="J17" s="22">
+        <v>6055</v>
+      </c>
+      <c r="K17" s="22">
+        <v>6115</v>
+      </c>
+      <c r="L17" s="22">
+        <v>6080</v>
+      </c>
+      <c r="M17" s="23">
+        <v>6040</v>
       </c>
       <c r="N17" s="12">
         <f t="shared" si="1"/>
-        <v>5950</v>
+        <v>5945</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="2"/>
@@ -2044,51 +2048,51 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>2995</v>
+        <v>2990</v>
       </c>
       <c r="B18" s="1">
-        <v>3125</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3120</v>
+        <v>3260</v>
+      </c>
+      <c r="C18">
+        <v>3025</v>
       </c>
       <c r="D18" s="1">
-        <v>3015</v>
-      </c>
-      <c r="E18" s="1">
-        <v>3255</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2995</v>
-      </c>
-      <c r="G18" s="1">
+        <v>3150</v>
+      </c>
+      <c r="E18">
+        <v>3130</v>
+      </c>
+      <c r="F18">
+        <v>3090</v>
+      </c>
+      <c r="G18">
+        <v>3045</v>
+      </c>
+      <c r="H18" s="7">
+        <v>3115</v>
+      </c>
+      <c r="I18" s="22">
         <v>3075</v>
       </c>
-      <c r="H18" s="1">
-        <v>3110</v>
-      </c>
-      <c r="I18" s="7">
-        <v>3030</v>
-      </c>
-      <c r="J18" s="8">
-        <v>3065</v>
-      </c>
-      <c r="K18" s="8">
-        <v>3015</v>
-      </c>
-      <c r="L18" s="8">
-        <v>3025</v>
-      </c>
-      <c r="M18" s="5">
-        <v>2990</v>
+      <c r="J18" s="22">
+        <v>3070</v>
+      </c>
+      <c r="K18" s="22">
+        <v>2890</v>
+      </c>
+      <c r="L18" s="22">
+        <v>3035</v>
+      </c>
+      <c r="M18" s="23">
+        <v>3010</v>
       </c>
       <c r="N18" s="12">
         <f t="shared" si="1"/>
-        <v>2990</v>
+        <v>2890</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="2"/>
-        <v>2990</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
@@ -2096,142 +2100,142 @@
         <v>5060</v>
       </c>
       <c r="B19" s="1">
-        <v>5525</v>
-      </c>
-      <c r="C19" s="1">
-        <v>5145</v>
+        <v>5365</v>
+      </c>
+      <c r="C19">
+        <v>5535</v>
       </c>
       <c r="D19" s="1">
-        <v>5170</v>
-      </c>
-      <c r="E19" s="1">
-        <v>5315</v>
-      </c>
-      <c r="F19" s="1">
-        <v>5175</v>
-      </c>
-      <c r="G19" s="1">
-        <v>5160</v>
-      </c>
-      <c r="H19" s="1">
-        <v>5180</v>
-      </c>
-      <c r="I19" s="7">
-        <v>5095</v>
-      </c>
-      <c r="J19" s="8">
-        <v>5185</v>
-      </c>
-      <c r="K19" s="8">
-        <v>5165</v>
-      </c>
-      <c r="L19" s="8">
-        <v>5060</v>
-      </c>
-      <c r="M19" s="5">
-        <v>5355</v>
+        <v>5290</v>
+      </c>
+      <c r="E19">
+        <v>5300</v>
+      </c>
+      <c r="F19">
+        <v>5270</v>
+      </c>
+      <c r="G19">
+        <v>5265</v>
+      </c>
+      <c r="H19" s="7">
+        <v>5115</v>
+      </c>
+      <c r="I19" s="22">
+        <v>5125</v>
+      </c>
+      <c r="J19" s="22">
+        <v>4960</v>
+      </c>
+      <c r="K19" s="22">
+        <v>5155</v>
+      </c>
+      <c r="L19" s="22">
+        <v>5205</v>
+      </c>
+      <c r="M19" s="23">
+        <v>5300</v>
       </c>
       <c r="N19" s="12">
         <f t="shared" si="1"/>
-        <v>5060</v>
+        <v>4960</v>
       </c>
       <c r="O19" s="3">
         <f t="shared" si="2"/>
-        <v>5060</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>2925</v>
+        <v>2885</v>
       </c>
       <c r="B20" s="1">
-        <v>2980</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2885</v>
+        <v>3220</v>
+      </c>
+      <c r="C20">
+        <v>2910</v>
       </c>
       <c r="D20" s="1">
-        <v>2945</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3050</v>
-      </c>
-      <c r="F20" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G20" s="1">
-        <v>2885</v>
-      </c>
-      <c r="H20" s="1">
-        <v>2915</v>
-      </c>
-      <c r="I20" s="7">
-        <v>2995</v>
-      </c>
-      <c r="J20" s="8">
-        <v>2990</v>
-      </c>
-      <c r="K20" s="8">
-        <v>3045</v>
-      </c>
-      <c r="L20" s="8">
-        <v>3015</v>
-      </c>
-      <c r="M20" s="5">
-        <v>2980</v>
+        <v>3120</v>
+      </c>
+      <c r="E20">
+        <v>3250</v>
+      </c>
+      <c r="F20">
+        <v>3150</v>
+      </c>
+      <c r="G20">
+        <v>3085</v>
+      </c>
+      <c r="H20" s="7">
+        <v>2910</v>
+      </c>
+      <c r="I20" s="22">
+        <v>2840</v>
+      </c>
+      <c r="J20" s="22">
+        <v>2970</v>
+      </c>
+      <c r="K20" s="22">
+        <v>3100</v>
+      </c>
+      <c r="L20" s="22">
+        <v>2890</v>
+      </c>
+      <c r="M20" s="23">
+        <v>2880</v>
       </c>
       <c r="N20" s="12">
         <f t="shared" si="1"/>
-        <v>2885</v>
+        <v>2840</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" si="2"/>
-        <v>2885</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>5315</v>
+        <v>5150</v>
       </c>
       <c r="B21" s="1">
+        <v>5600</v>
+      </c>
+      <c r="C21">
+        <v>5560</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5585</v>
+      </c>
+      <c r="E21">
+        <v>5545</v>
+      </c>
+      <c r="F21">
+        <v>5675</v>
+      </c>
+      <c r="G21">
+        <v>5690</v>
+      </c>
+      <c r="H21" s="7">
+        <v>5375</v>
+      </c>
+      <c r="I21" s="22">
+        <v>5210</v>
+      </c>
+      <c r="J21" s="22">
         <v>5405</v>
       </c>
-      <c r="C21" s="1">
-        <v>5595</v>
-      </c>
-      <c r="D21" s="1">
-        <v>5425</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="K21" s="22">
+        <v>5470</v>
+      </c>
+      <c r="L21" s="22">
+        <v>5335</v>
+      </c>
+      <c r="M21" s="23">
         <v>5375</v>
-      </c>
-      <c r="F21" s="1">
-        <v>5685</v>
-      </c>
-      <c r="G21" s="1">
-        <v>5150</v>
-      </c>
-      <c r="H21" s="1">
-        <v>5355</v>
-      </c>
-      <c r="I21" s="7">
-        <v>5305</v>
-      </c>
-      <c r="J21" s="8">
-        <v>5705</v>
-      </c>
-      <c r="K21" s="8">
-        <v>5600</v>
-      </c>
-      <c r="L21" s="8">
-        <v>5365</v>
-      </c>
-      <c r="M21" s="5">
-        <v>5305</v>
       </c>
       <c r="N21" s="12">
         <f t="shared" si="1"/>
-        <v>5150</v>
+        <v>5210</v>
       </c>
       <c r="O21" s="3">
         <f t="shared" si="2"/>
@@ -2440,9 +2444,8 @@
       <c r="G88" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:M1"/>
+  <mergeCells count="1">
+    <mergeCell ref="B1:M1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:Z128">

</xml_diff>

<commit_message>
batch test update. bug fix on swap chain. instance sequence update.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37890" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="39060" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="19">
   <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -89,7 +89,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1.5;w1,w1</t>
+    <t>1;w1,n0.5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -780,7 +784,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -846,12 +850,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -898,7 +896,182 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1221,7 +1394,7 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1241,15 +1414,15 @@
   <sheetData>
     <row r="1" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
-      <c r="B1" s="19" t="s">
-        <v>17</v>
-      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -1350,31 +1523,31 @@
     <row r="4" spans="1:15" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <f>AVERAGE(A5:A128)</f>
-        <v>3475.8823529411766</v>
+        <v>3450.294117647059</v>
       </c>
       <c r="B4" s="9">
         <f>AVERAGE(B5:B128)</f>
-        <v>3664.1176470588234</v>
+        <v>9999</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ref="C4:O4" si="0">AVERAGE(C5:C128)</f>
-        <v>3690.294117647059</v>
+        <v>9999</v>
       </c>
       <c r="D4" s="4">
         <f>AVERAGE(D5:D128)</f>
-        <v>3639.705882352941</v>
+        <v>9999</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>3669.1176470588234</v>
+        <v>9999</v>
       </c>
       <c r="F4" s="4">
         <f>AVERAGE(F5:F128)</f>
-        <v>3667.9411764705883</v>
+        <v>9999</v>
       </c>
       <c r="G4" s="11">
         <f t="shared" si="0"/>
-        <v>3684.4117647058824</v>
+        <v>9999</v>
       </c>
       <c r="H4" s="10">
         <f t="shared" si="0"/>
@@ -1382,72 +1555,72 @@
       </c>
       <c r="I4" s="4">
         <f t="shared" si="0"/>
-        <v>3541.1764705882351</v>
+        <v>3546.4705882352941</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
-        <v>3597.0588235294117</v>
+        <v>3588.5294117647059</v>
       </c>
       <c r="K4" s="10">
         <f t="shared" si="0"/>
-        <v>3579.4117647058824</v>
+        <v>3619.1176470588234</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>3580.294117647059</v>
+        <v>3606.1764705882351</v>
       </c>
       <c r="M4" s="9">
         <f t="shared" si="0"/>
-        <v>3575</v>
+        <v>3601.7647058823532</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
-        <v>3473.8235294117649</v>
+        <v>3492.3529411764707</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>3446.7647058823532</v>
+        <v>3444.705882352941</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>1560</v>
       </c>
-      <c r="B5" s="1">
-        <v>1585</v>
+      <c r="B5">
+        <v>9999</v>
       </c>
       <c r="C5">
-        <v>1630</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1630</v>
+        <v>9999</v>
+      </c>
+      <c r="D5">
+        <v>9999</v>
       </c>
       <c r="E5">
-        <v>1630</v>
+        <v>9999</v>
       </c>
       <c r="F5">
-        <v>1605</v>
+        <v>9999</v>
       </c>
       <c r="G5">
-        <v>1630</v>
+        <v>9999</v>
       </c>
       <c r="H5" s="7">
         <v>1635</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5">
+        <v>1570</v>
+      </c>
+      <c r="J5">
         <v>1610</v>
       </c>
-      <c r="J5" s="22">
-        <v>1660</v>
-      </c>
-      <c r="K5" s="22">
-        <v>1640</v>
-      </c>
-      <c r="L5" s="22">
+      <c r="K5">
+        <v>1585</v>
+      </c>
+      <c r="L5">
+        <v>1630</v>
+      </c>
+      <c r="M5">
         <v>1570</v>
-      </c>
-      <c r="M5" s="23">
-        <v>1630</v>
       </c>
       <c r="N5" s="12">
         <f>MIN(B5:M5)</f>
@@ -1462,94 +1635,94 @@
       <c r="A6" s="3">
         <v>2945</v>
       </c>
-      <c r="B6" s="1">
-        <v>3115</v>
-      </c>
-      <c r="C6">
-        <v>3100</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3045</v>
-      </c>
-      <c r="E6">
-        <v>3100</v>
-      </c>
-      <c r="F6">
-        <v>3090</v>
-      </c>
-      <c r="G6">
-        <v>3165</v>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
       </c>
       <c r="H6" s="7">
         <v>3065</v>
       </c>
-      <c r="I6" s="22">
-        <v>3085</v>
-      </c>
-      <c r="J6" s="22">
-        <v>3140</v>
-      </c>
-      <c r="K6" s="22">
-        <v>3080</v>
-      </c>
-      <c r="L6" s="22">
-        <v>3045</v>
-      </c>
-      <c r="M6" s="23">
-        <v>3055</v>
+      <c r="I6">
+        <v>3185</v>
+      </c>
+      <c r="J6">
+        <v>3025</v>
+      </c>
+      <c r="K6">
+        <v>3115</v>
+      </c>
+      <c r="L6">
+        <v>2910</v>
+      </c>
+      <c r="M6">
+        <v>3090</v>
       </c>
       <c r="N6" s="12">
         <f t="shared" ref="N6:N21" si="1">MIN(B6:M6)</f>
-        <v>3045</v>
+        <v>2910</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" ref="O6:O21" si="2">MIN(A6,N6)</f>
-        <v>2945</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>1965</v>
       </c>
-      <c r="B7" s="1">
-        <v>2040</v>
-      </c>
-      <c r="C7">
-        <v>2035</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2060</v>
-      </c>
-      <c r="E7">
-        <v>2045</v>
-      </c>
-      <c r="F7">
-        <v>2065</v>
-      </c>
-      <c r="G7">
-        <v>2025</v>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
       </c>
       <c r="H7" s="7">
         <v>2005</v>
       </c>
-      <c r="I7" s="22">
-        <v>2015</v>
-      </c>
-      <c r="J7" s="22">
-        <v>2010</v>
-      </c>
-      <c r="K7" s="22">
-        <v>2020</v>
-      </c>
-      <c r="L7" s="22">
-        <v>2015</v>
-      </c>
-      <c r="M7" s="23">
-        <v>2015</v>
+      <c r="I7">
+        <v>1990</v>
+      </c>
+      <c r="J7">
+        <v>2000</v>
+      </c>
+      <c r="K7">
+        <v>1975</v>
+      </c>
+      <c r="L7">
+        <v>2030</v>
+      </c>
+      <c r="M7">
+        <v>2000</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" si="1"/>
-        <v>2005</v>
+        <v>1975</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="2"/>
@@ -1560,45 +1733,45 @@
       <c r="A8" s="3">
         <v>2270</v>
       </c>
-      <c r="B8" s="1">
-        <v>2310</v>
-      </c>
-      <c r="C8">
-        <v>2365</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2325</v>
-      </c>
-      <c r="E8">
-        <v>2365</v>
-      </c>
-      <c r="F8">
-        <v>2340</v>
-      </c>
-      <c r="G8">
-        <v>2345</v>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
       </c>
       <c r="H8" s="7">
         <v>2335</v>
       </c>
-      <c r="I8" s="22">
-        <v>2355</v>
-      </c>
-      <c r="J8" s="22">
-        <v>2285</v>
-      </c>
-      <c r="K8" s="22">
-        <v>2350</v>
-      </c>
-      <c r="L8" s="22">
+      <c r="I8">
+        <v>2315</v>
+      </c>
+      <c r="J8">
+        <v>2330</v>
+      </c>
+      <c r="K8">
+        <v>2320</v>
+      </c>
+      <c r="L8">
         <v>2340</v>
       </c>
-      <c r="M8" s="23">
-        <v>2325</v>
+      <c r="M8">
+        <v>2315</v>
       </c>
       <c r="N8" s="12">
         <f t="shared" si="1"/>
-        <v>2285</v>
+        <v>2315</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="2"/>
@@ -1607,96 +1780,96 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>3195</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3260</v>
-      </c>
-      <c r="C9">
-        <v>3410</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3365</v>
-      </c>
-      <c r="E9">
-        <v>3370</v>
-      </c>
-      <c r="F9">
-        <v>3275</v>
-      </c>
-      <c r="G9">
-        <v>3550</v>
+        <v>3185</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
       </c>
       <c r="H9" s="7">
         <v>3305</v>
       </c>
-      <c r="I9" s="22">
-        <v>3280</v>
-      </c>
-      <c r="J9" s="22">
-        <v>3455</v>
-      </c>
-      <c r="K9" s="22">
+      <c r="I9">
+        <v>3150</v>
+      </c>
+      <c r="J9">
         <v>3265</v>
       </c>
-      <c r="L9" s="22">
-        <v>3360</v>
-      </c>
-      <c r="M9" s="23">
-        <v>3185</v>
+      <c r="K9">
+        <v>3415</v>
+      </c>
+      <c r="L9">
+        <v>3345</v>
+      </c>
+      <c r="M9">
+        <v>3355</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="1"/>
-        <v>3185</v>
+        <v>3150</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="2"/>
-        <v>3185</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>2065</v>
       </c>
-      <c r="B10" s="1">
-        <v>2185</v>
-      </c>
-      <c r="C10">
-        <v>2145</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2130</v>
-      </c>
-      <c r="E10">
-        <v>2100</v>
-      </c>
-      <c r="F10">
-        <v>2190</v>
-      </c>
-      <c r="G10">
-        <v>2200</v>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
       </c>
       <c r="H10" s="7">
         <v>2130</v>
       </c>
-      <c r="I10" s="22">
-        <v>2165</v>
-      </c>
-      <c r="J10" s="22">
-        <v>2190</v>
-      </c>
-      <c r="K10" s="22">
-        <v>2135</v>
-      </c>
-      <c r="L10" s="22">
-        <v>2070</v>
-      </c>
-      <c r="M10" s="23">
-        <v>2070</v>
+      <c r="I10">
+        <v>2130</v>
+      </c>
+      <c r="J10">
+        <v>2230</v>
+      </c>
+      <c r="K10">
+        <v>2140</v>
+      </c>
+      <c r="L10">
+        <v>2115</v>
+      </c>
+      <c r="M10">
+        <v>2160</v>
       </c>
       <c r="N10" s="12">
         <f t="shared" si="1"/>
-        <v>2070</v>
+        <v>2115</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="2"/>
@@ -1707,90 +1880,90 @@
       <c r="A11" s="3">
         <v>3525</v>
       </c>
-      <c r="B11" s="1">
-        <v>3465</v>
-      </c>
-      <c r="C11">
-        <v>3825</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3590</v>
-      </c>
-      <c r="E11">
-        <v>3695</v>
-      </c>
-      <c r="F11">
-        <v>3660</v>
-      </c>
-      <c r="G11">
-        <v>3615</v>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
       </c>
       <c r="H11" s="7">
         <v>3645</v>
       </c>
-      <c r="I11" s="22">
-        <v>3655</v>
-      </c>
-      <c r="J11" s="22">
-        <v>3665</v>
-      </c>
-      <c r="K11" s="22">
-        <v>3565</v>
-      </c>
-      <c r="L11" s="22">
-        <v>3585</v>
-      </c>
-      <c r="M11" s="23">
-        <v>3650</v>
+      <c r="I11">
+        <v>3695</v>
+      </c>
+      <c r="J11">
+        <v>3680</v>
+      </c>
+      <c r="K11">
+        <v>3620</v>
+      </c>
+      <c r="L11">
+        <v>3550</v>
+      </c>
+      <c r="M11">
+        <v>3610</v>
       </c>
       <c r="N11" s="12">
         <f t="shared" si="1"/>
-        <v>3465</v>
+        <v>3550</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="2"/>
-        <v>3465</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>2250</v>
       </c>
-      <c r="B12" s="1">
-        <v>2425</v>
-      </c>
-      <c r="C12">
-        <v>2385</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2395</v>
-      </c>
-      <c r="E12">
-        <v>2435</v>
-      </c>
-      <c r="F12">
-        <v>2425</v>
-      </c>
-      <c r="G12">
-        <v>2345</v>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
       </c>
       <c r="H12" s="7">
         <v>2260</v>
       </c>
-      <c r="I12" s="22">
-        <v>2320</v>
-      </c>
-      <c r="J12" s="22">
-        <v>2380</v>
-      </c>
-      <c r="K12" s="22">
-        <v>2340</v>
-      </c>
-      <c r="L12" s="22">
+      <c r="I12">
+        <v>2280</v>
+      </c>
+      <c r="J12">
+        <v>2310</v>
+      </c>
+      <c r="K12">
+        <v>2350</v>
+      </c>
+      <c r="L12">
+        <v>2355</v>
+      </c>
+      <c r="M12">
         <v>2290</v>
-      </c>
-      <c r="M12" s="23">
-        <v>2300</v>
       </c>
       <c r="N12" s="12">
         <f t="shared" si="1"/>
@@ -1805,45 +1978,45 @@
       <c r="A13" s="3">
         <v>6800</v>
       </c>
-      <c r="B13" s="1">
-        <v>7170</v>
-      </c>
-      <c r="C13">
-        <v>7270</v>
-      </c>
-      <c r="D13" s="1">
-        <v>7005</v>
-      </c>
-      <c r="E13">
-        <v>7110</v>
-      </c>
-      <c r="F13">
-        <v>7300</v>
-      </c>
-      <c r="G13">
-        <v>7225</v>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
       </c>
       <c r="H13" s="7">
         <v>7025</v>
       </c>
-      <c r="I13" s="22">
-        <v>6890</v>
-      </c>
-      <c r="J13" s="22">
-        <v>7015</v>
-      </c>
-      <c r="K13" s="22">
-        <v>6935</v>
-      </c>
-      <c r="L13" s="22">
-        <v>7070</v>
-      </c>
-      <c r="M13" s="23">
-        <v>7100</v>
+      <c r="I13">
+        <v>6870</v>
+      </c>
+      <c r="J13">
+        <v>7020</v>
+      </c>
+      <c r="K13">
+        <v>7035</v>
+      </c>
+      <c r="L13">
+        <v>7065</v>
+      </c>
+      <c r="M13">
+        <v>7030</v>
       </c>
       <c r="N13" s="12">
         <f t="shared" si="1"/>
-        <v>6890</v>
+        <v>6870</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" si="2"/>
@@ -1854,94 +2027,94 @@
       <c r="A14" s="3">
         <v>2770</v>
       </c>
-      <c r="B14" s="1">
-        <v>3075</v>
-      </c>
-      <c r="C14">
-        <v>3040</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3095</v>
-      </c>
-      <c r="E14">
-        <v>2980</v>
-      </c>
-      <c r="F14">
-        <v>3060</v>
-      </c>
-      <c r="G14">
-        <v>3000</v>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
       </c>
       <c r="H14" s="7">
         <v>2840</v>
       </c>
-      <c r="I14" s="22">
-        <v>2840</v>
-      </c>
-      <c r="J14" s="22">
-        <v>2910</v>
-      </c>
-      <c r="K14" s="22">
-        <v>2820</v>
-      </c>
-      <c r="L14" s="22">
-        <v>2875</v>
-      </c>
-      <c r="M14" s="23">
+      <c r="I14">
         <v>2860</v>
+      </c>
+      <c r="J14">
+        <v>2765</v>
+      </c>
+      <c r="K14">
+        <v>2880</v>
+      </c>
+      <c r="L14">
+        <v>2870</v>
+      </c>
+      <c r="M14">
+        <v>2865</v>
       </c>
       <c r="N14" s="12">
         <f t="shared" si="1"/>
-        <v>2820</v>
+        <v>2765</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="2"/>
-        <v>2770</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>3780</v>
-      </c>
-      <c r="B15" s="1">
-        <v>3835</v>
-      </c>
-      <c r="C15">
-        <v>4105</v>
-      </c>
-      <c r="D15" s="1">
-        <v>4040</v>
-      </c>
-      <c r="E15">
-        <v>4035</v>
-      </c>
-      <c r="F15">
-        <v>3975</v>
-      </c>
-      <c r="G15">
-        <v>3990</v>
+        <v>3600</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
       </c>
       <c r="H15" s="7">
         <v>3875</v>
       </c>
-      <c r="I15" s="22">
-        <v>3600</v>
-      </c>
-      <c r="J15" s="22">
-        <v>3875</v>
-      </c>
-      <c r="K15" s="22">
-        <v>3900</v>
-      </c>
-      <c r="L15" s="22">
-        <v>3965</v>
-      </c>
-      <c r="M15" s="23">
-        <v>3875</v>
+      <c r="I15">
+        <v>3910</v>
+      </c>
+      <c r="J15">
+        <v>4105</v>
+      </c>
+      <c r="K15">
+        <v>3810</v>
+      </c>
+      <c r="L15">
+        <v>3840</v>
+      </c>
+      <c r="M15">
+        <v>4020</v>
       </c>
       <c r="N15" s="12">
         <f t="shared" si="1"/>
-        <v>3600</v>
+        <v>3810</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="2"/>
@@ -1952,45 +2125,45 @@
       <c r="A16" s="3">
         <v>3940</v>
       </c>
-      <c r="B16" s="1">
-        <v>4185</v>
-      </c>
-      <c r="C16">
-        <v>4140</v>
-      </c>
-      <c r="D16" s="1">
-        <v>4075</v>
-      </c>
-      <c r="E16">
-        <v>4100</v>
-      </c>
-      <c r="F16">
-        <v>4015</v>
-      </c>
-      <c r="G16">
-        <v>4165</v>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
       </c>
       <c r="H16" s="7">
         <v>4070</v>
       </c>
-      <c r="I16" s="22">
-        <v>4045</v>
-      </c>
-      <c r="J16" s="22">
-        <v>4105</v>
-      </c>
-      <c r="K16" s="22">
-        <v>4070</v>
-      </c>
-      <c r="L16" s="22">
-        <v>4135</v>
-      </c>
-      <c r="M16" s="23">
-        <v>4105</v>
+      <c r="I16">
+        <v>4130</v>
+      </c>
+      <c r="J16">
+        <v>3975</v>
+      </c>
+      <c r="K16">
+        <v>4120</v>
+      </c>
+      <c r="L16">
+        <v>4075</v>
+      </c>
+      <c r="M16">
+        <v>4035</v>
       </c>
       <c r="N16" s="12">
         <f t="shared" si="1"/>
-        <v>4015</v>
+        <v>3975</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="2"/>
@@ -2001,41 +2174,41 @@
       <c r="A17" s="3">
         <v>5940</v>
       </c>
-      <c r="B17" s="1">
-        <v>6195</v>
-      </c>
-      <c r="C17">
-        <v>6255</v>
-      </c>
-      <c r="D17" s="1">
-        <v>5975</v>
-      </c>
-      <c r="E17">
-        <v>6185</v>
-      </c>
-      <c r="F17">
-        <v>6170</v>
-      </c>
-      <c r="G17">
-        <v>6295</v>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
       </c>
       <c r="H17" s="7">
         <v>5945</v>
       </c>
-      <c r="I17" s="22">
-        <v>6090</v>
-      </c>
-      <c r="J17" s="22">
-        <v>6055</v>
-      </c>
-      <c r="K17" s="22">
-        <v>6115</v>
-      </c>
-      <c r="L17" s="22">
-        <v>6080</v>
-      </c>
-      <c r="M17" s="23">
-        <v>6040</v>
+      <c r="I17">
+        <v>5975</v>
+      </c>
+      <c r="J17">
+        <v>5955</v>
+      </c>
+      <c r="K17">
+        <v>6105</v>
+      </c>
+      <c r="L17">
+        <v>6300</v>
+      </c>
+      <c r="M17">
+        <v>6110</v>
       </c>
       <c r="N17" s="12">
         <f t="shared" si="1"/>
@@ -2048,47 +2221,47 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>2990</v>
-      </c>
-      <c r="B18" s="1">
-        <v>3260</v>
-      </c>
-      <c r="C18">
-        <v>3025</v>
-      </c>
-      <c r="D18" s="1">
-        <v>3150</v>
-      </c>
-      <c r="E18">
-        <v>3130</v>
-      </c>
-      <c r="F18">
-        <v>3090</v>
-      </c>
-      <c r="G18">
-        <v>3045</v>
+        <v>2890</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
       </c>
       <c r="H18" s="7">
         <v>3115</v>
       </c>
-      <c r="I18" s="22">
-        <v>3075</v>
-      </c>
-      <c r="J18" s="22">
-        <v>3070</v>
-      </c>
-      <c r="K18" s="22">
-        <v>2890</v>
-      </c>
-      <c r="L18" s="22">
-        <v>3035</v>
-      </c>
-      <c r="M18" s="23">
-        <v>3010</v>
+      <c r="I18">
+        <v>3005</v>
+      </c>
+      <c r="J18">
+        <v>3085</v>
+      </c>
+      <c r="K18">
+        <v>3160</v>
+      </c>
+      <c r="L18">
+        <v>3230</v>
+      </c>
+      <c r="M18">
+        <v>3125</v>
       </c>
       <c r="N18" s="12">
         <f t="shared" si="1"/>
-        <v>2890</v>
+        <v>3005</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="2"/>
@@ -2097,47 +2270,47 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>5060</v>
-      </c>
-      <c r="B19" s="1">
-        <v>5365</v>
-      </c>
-      <c r="C19">
-        <v>5535</v>
-      </c>
-      <c r="D19" s="1">
-        <v>5290</v>
-      </c>
-      <c r="E19">
-        <v>5300</v>
-      </c>
-      <c r="F19">
-        <v>5270</v>
-      </c>
-      <c r="G19">
-        <v>5265</v>
+        <v>4960</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
       </c>
       <c r="H19" s="7">
         <v>5115</v>
       </c>
-      <c r="I19" s="22">
-        <v>5125</v>
-      </c>
-      <c r="J19" s="22">
-        <v>4960</v>
-      </c>
-      <c r="K19" s="22">
-        <v>5155</v>
-      </c>
-      <c r="L19" s="22">
-        <v>5205</v>
-      </c>
-      <c r="M19" s="23">
-        <v>5300</v>
+      <c r="I19">
+        <v>5185</v>
+      </c>
+      <c r="J19">
+        <v>5135</v>
+      </c>
+      <c r="K19">
+        <v>5270</v>
+      </c>
+      <c r="L19">
+        <v>5220</v>
+      </c>
+      <c r="M19">
+        <v>5260</v>
       </c>
       <c r="N19" s="12">
         <f t="shared" si="1"/>
-        <v>4960</v>
+        <v>5115</v>
       </c>
       <c r="O19" s="3">
         <f t="shared" si="2"/>
@@ -2146,47 +2319,47 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>2885</v>
-      </c>
-      <c r="B20" s="1">
-        <v>3220</v>
-      </c>
-      <c r="C20">
-        <v>2910</v>
-      </c>
-      <c r="D20" s="1">
-        <v>3120</v>
-      </c>
-      <c r="E20">
-        <v>3250</v>
-      </c>
-      <c r="F20">
-        <v>3150</v>
-      </c>
-      <c r="G20">
-        <v>3085</v>
+        <v>2840</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
       </c>
       <c r="H20" s="7">
         <v>2910</v>
       </c>
-      <c r="I20" s="22">
-        <v>2840</v>
-      </c>
-      <c r="J20" s="22">
-        <v>2970</v>
-      </c>
-      <c r="K20" s="22">
-        <v>3100</v>
-      </c>
-      <c r="L20" s="22">
-        <v>2890</v>
-      </c>
-      <c r="M20" s="23">
-        <v>2880</v>
+      <c r="I20">
+        <v>2910</v>
+      </c>
+      <c r="J20">
+        <v>2925</v>
+      </c>
+      <c r="K20">
+        <v>2985</v>
+      </c>
+      <c r="L20">
+        <v>3000</v>
+      </c>
+      <c r="M20">
+        <v>3015</v>
       </c>
       <c r="N20" s="12">
         <f t="shared" si="1"/>
-        <v>2840</v>
+        <v>2910</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" si="2"/>
@@ -2197,49 +2370,49 @@
       <c r="A21" s="3">
         <v>5150</v>
       </c>
-      <c r="B21" s="1">
-        <v>5600</v>
-      </c>
-      <c r="C21">
-        <v>5560</v>
-      </c>
-      <c r="D21" s="1">
-        <v>5585</v>
-      </c>
-      <c r="E21">
-        <v>5545</v>
-      </c>
-      <c r="F21">
-        <v>5675</v>
-      </c>
-      <c r="G21">
-        <v>5690</v>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
       </c>
       <c r="H21" s="7">
         <v>5375</v>
       </c>
-      <c r="I21" s="22">
-        <v>5210</v>
-      </c>
-      <c r="J21" s="22">
-        <v>5405</v>
-      </c>
-      <c r="K21" s="22">
-        <v>5470</v>
-      </c>
-      <c r="L21" s="22">
-        <v>5335</v>
-      </c>
-      <c r="M21" s="23">
-        <v>5375</v>
+      <c r="I21">
+        <v>5130</v>
+      </c>
+      <c r="J21">
+        <v>5590</v>
+      </c>
+      <c r="K21">
+        <v>5640</v>
+      </c>
+      <c r="L21">
+        <v>5430</v>
+      </c>
+      <c r="M21">
+        <v>5380</v>
       </c>
       <c r="N21" s="12">
         <f t="shared" si="1"/>
-        <v>5210</v>
+        <v>5130</v>
       </c>
       <c r="O21" s="3">
         <f t="shared" si="2"/>
-        <v>5150</v>
+        <v>5130</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
@@ -2444,24 +2617,25 @@
       <c r="G88" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:M1"/>
+  <mergeCells count="2">
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:Z128">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>A4=SMALL($A4:$Z4,1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>A4=SMALL($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="27" priority="4">
       <formula>A4=LARGE($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="26" priority="5">
       <formula>A4=LARGE($A4:$Z4,1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="25" priority="3">
       <formula>A4=SMALL($A4:$Z4,3)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
bug fix on total assign.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="42570" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="43740" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -904,7 +904,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -938,6 +938,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -956,50 +995,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1046,182 +1049,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1544,7 +1372,8 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1554,46 +1383,46 @@
     <col min="8" max="12" width="8.5" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="9.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" style="14" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="17"/>
+      <c r="I1" s="11"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
       <c r="M1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1620,12 +1449,12 @@
       <c r="M2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="20"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="31"/>
     </row>
     <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
@@ -1662,148 +1491,152 @@
       <c r="M3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="20"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="31"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="e">
+      <c r="A4" s="18" t="e">
         <f>AVERAGE(A6:A129)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="19">
         <f>AVERAGE(B6:B19,B21:B34)</f>
         <v>3845.1785714285716</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="19">
         <f t="shared" ref="C4:O4" si="0">AVERAGE(C6:C19,C21:C34)</f>
         <v>3876.25</v>
       </c>
-      <c r="D4" s="27" t="e">
+      <c r="D4" s="19">
+        <f t="shared" si="0"/>
+        <v>3854.8214285714284</v>
+      </c>
+      <c r="E4" s="19">
+        <f t="shared" si="0"/>
+        <v>3898.5714285714284</v>
+      </c>
+      <c r="F4" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E4" s="27" t="e">
+      <c r="G4" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F4" s="27" t="e">
+      <c r="H4" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G4" s="27" t="e">
+      <c r="I4" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H4" s="27" t="e">
+      <c r="J4" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I4" s="27" t="e">
+      <c r="K4" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="27" t="e">
+      <c r="L4" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4" s="27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" s="27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" s="27">
+      <c r="M4" s="19">
         <f t="shared" si="0"/>
         <v>3775.7142857142858</v>
       </c>
-      <c r="N4" s="27">
+      <c r="N4" s="19">
         <f t="shared" si="0"/>
-        <v>3801.25</v>
-      </c>
-      <c r="O4" s="27">
+        <v>3776.0714285714284</v>
+      </c>
+      <c r="O4" s="19">
         <f t="shared" si="0"/>
-        <v>3801.25</v>
-      </c>
-      <c r="P4" s="21"/>
+        <v>3776.0714285714284</v>
+      </c>
+      <c r="P4" s="13"/>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="28" t="e">
+      <c r="A5" s="20" t="e">
         <f>AVERAGE(A6:A19)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="20">
         <f>AVERAGE(B6:B19)</f>
         <v>3800</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="20">
         <f t="shared" ref="C5:O5" si="1">AVERAGE(C6:C19)</f>
         <v>3832.5</v>
       </c>
-      <c r="D5" s="28" t="e">
+      <c r="D5" s="20">
+        <f t="shared" si="1"/>
+        <v>3777.1428571428573</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="1"/>
+        <v>3828.9285714285716</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E5" s="28" t="e">
+      <c r="G5" s="20" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="28" t="e">
+      <c r="H5" s="20" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G5" s="28" t="e">
+      <c r="I5" s="20" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="28" t="e">
+      <c r="J5" s="20" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="28" t="e">
+      <c r="K5" s="20" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5" s="28" t="e">
+      <c r="L5" s="20" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="28" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="28" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="28">
+      <c r="M5" s="20">
         <f t="shared" si="1"/>
         <v>3775.7142857142858</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="20">
         <f t="shared" si="1"/>
-        <v>3731.0714285714284</v>
-      </c>
-      <c r="O5" s="28">
+        <v>3702.5</v>
+      </c>
+      <c r="O5" s="20">
         <f t="shared" si="1"/>
-        <v>3731.0714285714284</v>
-      </c>
-      <c r="P5" s="24">
+        <v>3702.5</v>
+      </c>
+      <c r="P5" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="29"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="9">
         <v>5440</v>
       </c>
       <c r="C6" s="9">
         <v>5515</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6">
+        <v>5515</v>
+      </c>
+      <c r="E6">
+        <v>5555</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -1811,7 +1644,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="22">
+      <c r="M6" s="14">
         <v>5290</v>
       </c>
       <c r="N6" s="3">
@@ -1827,15 +1660,19 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="29"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="9">
         <v>4585</v>
       </c>
       <c r="C7" s="9">
         <v>4750</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7">
+        <v>4645</v>
+      </c>
+      <c r="E7">
+        <v>4830</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -1843,7 +1680,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="22">
+      <c r="M7" s="14">
         <v>4610</v>
       </c>
       <c r="N7" s="3">
@@ -1859,15 +1696,19 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" s="29"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="9">
         <v>3150</v>
       </c>
       <c r="C8" s="9">
         <v>3265</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="D8">
+        <v>3310</v>
+      </c>
+      <c r="E8">
+        <v>3360</v>
+      </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -1875,7 +1716,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="22">
+      <c r="M8" s="14">
         <v>3200</v>
       </c>
       <c r="N8" s="3">
@@ -1891,15 +1732,19 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="29"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="9">
         <v>6000</v>
       </c>
       <c r="C9" s="9">
         <v>5950</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="D9">
+        <v>5860</v>
+      </c>
+      <c r="E9">
+        <v>5890</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -1907,31 +1752,35 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="22">
+      <c r="M9" s="14">
         <v>5880</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="2"/>
-        <v>5880</v>
+        <v>5860</v>
       </c>
       <c r="O9" s="9">
         <f t="shared" si="3"/>
-        <v>5880</v>
+        <v>5860</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="29"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="9">
         <v>2150</v>
       </c>
       <c r="C10" s="9">
         <v>2280</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="D10">
+        <v>2160</v>
+      </c>
+      <c r="E10">
+        <v>2200</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -1939,7 +1788,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="22">
+      <c r="M10" s="14">
         <v>2190</v>
       </c>
       <c r="N10" s="3">
@@ -1955,15 +1804,19 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A11" s="29"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="9">
         <v>4100</v>
       </c>
       <c r="C11" s="9">
         <v>4070</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11">
+        <v>4085</v>
+      </c>
+      <c r="E11">
+        <v>4145</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -1971,7 +1824,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="22">
+      <c r="M11" s="14">
         <v>3985</v>
       </c>
       <c r="N11" s="3">
@@ -1987,15 +1840,19 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="29"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="9">
         <v>4245</v>
       </c>
       <c r="C12" s="9">
         <v>4195</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="D12">
+        <v>4235</v>
+      </c>
+      <c r="E12">
+        <v>4215</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -2003,7 +1860,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="22">
+      <c r="M12" s="14">
         <v>4185</v>
       </c>
       <c r="N12" s="3">
@@ -2019,15 +1876,19 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A13" s="29"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="9">
         <v>7100</v>
       </c>
       <c r="C13" s="9">
         <v>7435</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="D13">
+        <v>6850</v>
+      </c>
+      <c r="E13">
+        <v>7245</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -2035,31 +1896,35 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="22">
+      <c r="M13" s="14">
         <v>7190</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="2"/>
-        <v>7100</v>
+        <v>6850</v>
       </c>
       <c r="O13" s="9">
         <f t="shared" si="3"/>
-        <v>7100</v>
+        <v>6850</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A14" s="29"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="9">
         <v>3135</v>
       </c>
       <c r="C14" s="9">
         <v>3185</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="D14">
+        <v>3085</v>
+      </c>
+      <c r="E14">
+        <v>3035</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -2067,31 +1932,35 @@
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="22">
+      <c r="M14" s="14">
         <v>3135</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="2"/>
-        <v>3135</v>
+        <v>3035</v>
       </c>
       <c r="O14" s="9">
         <f t="shared" si="3"/>
-        <v>3135</v>
+        <v>3035</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A15" s="29"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="9">
         <v>4300</v>
       </c>
       <c r="C15" s="9">
         <v>4035</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="D15">
+        <v>4010</v>
+      </c>
+      <c r="E15">
+        <v>4030</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -2099,31 +1968,35 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="22">
+      <c r="M15" s="14">
         <v>4155</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="2"/>
-        <v>4035</v>
+        <v>4010</v>
       </c>
       <c r="O15" s="9">
         <f t="shared" si="3"/>
-        <v>4035</v>
+        <v>4010</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A16" s="29"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="9">
         <v>1835</v>
       </c>
       <c r="C16" s="9">
         <v>1945</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="D16">
+        <v>1925</v>
+      </c>
+      <c r="E16">
+        <v>1965</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -2131,7 +2004,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="22">
+      <c r="M16" s="14">
         <v>1930</v>
       </c>
       <c r="N16" s="3">
@@ -2147,15 +2020,19 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A17" s="29"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="9">
         <v>3085</v>
       </c>
       <c r="C17" s="9">
         <v>2910</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="D17">
+        <v>3070</v>
+      </c>
+      <c r="E17">
+        <v>3100</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -2163,7 +2040,7 @@
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
-      <c r="M17" s="22">
+      <c r="M17" s="14">
         <v>3115</v>
       </c>
       <c r="N17" s="3">
@@ -2179,15 +2056,19 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A18" s="29"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="9">
         <v>2010</v>
       </c>
       <c r="C18" s="9">
         <v>2020</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="D18">
+        <v>1990</v>
+      </c>
+      <c r="E18">
+        <v>1980</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -2195,7 +2076,7 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
-      <c r="M18" s="22">
+      <c r="M18" s="14">
         <v>1935</v>
       </c>
       <c r="N18" s="3">
@@ -2211,15 +2092,19 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A19" s="29"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="9">
         <v>2065</v>
       </c>
       <c r="C19" s="9">
         <v>2100</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="D19">
+        <v>2140</v>
+      </c>
+      <c r="E19">
+        <v>2055</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -2227,96 +2112,100 @@
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
-      <c r="M19" s="22">
+      <c r="M19" s="14">
         <v>2060</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="2"/>
-        <v>2060</v>
+        <v>2055</v>
       </c>
       <c r="O19" s="9">
         <f t="shared" si="3"/>
-        <v>2060</v>
+        <v>2055</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A20" s="30" t="e">
+      <c r="A20" s="22" t="e">
         <f>AVERAGE(A21:A34)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="22">
         <f>AVERAGE(B21:B34)</f>
         <v>3890.3571428571427</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="22">
         <f t="shared" ref="C20:O20" si="4">AVERAGE(C21:C34)</f>
         <v>3920</v>
       </c>
-      <c r="D20" s="30" t="e">
+      <c r="D20" s="22">
+        <f t="shared" si="4"/>
+        <v>3932.5</v>
+      </c>
+      <c r="E20" s="22">
+        <f t="shared" si="4"/>
+        <v>3968.2142857142858</v>
+      </c>
+      <c r="F20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E20" s="30" t="e">
+      <c r="G20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" s="30" t="e">
+      <c r="H20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="30" t="e">
+      <c r="I20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H20" s="30" t="e">
+      <c r="J20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I20" s="30" t="e">
+      <c r="K20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J20" s="30" t="e">
+      <c r="L20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K20" s="30" t="e">
+      <c r="M20" s="22" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L20" s="30" t="e">
+      <c r="N20" s="22">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="30" t="e">
+        <v>3849.6428571428573</v>
+      </c>
+      <c r="O20" s="22">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" s="30">
-        <f t="shared" si="4"/>
-        <v>3871.4285714285716</v>
-      </c>
-      <c r="O20" s="30">
-        <f t="shared" si="4"/>
-        <v>3871.4285714285716</v>
-      </c>
-      <c r="P20" s="23">
+        <v>3849.6428571428573</v>
+      </c>
+      <c r="P20" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A21" s="29"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="9">
         <v>5755</v>
       </c>
       <c r="C21" s="9">
         <v>5900</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="D21">
+        <v>5920</v>
+      </c>
+      <c r="E21">
+        <v>6080</v>
+      </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -2338,15 +2227,19 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A22" s="29"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="9">
         <v>4820</v>
       </c>
       <c r="C22" s="9">
         <v>4885</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="D22">
+        <v>4680</v>
+      </c>
+      <c r="E22">
+        <v>4805</v>
+      </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -2357,26 +2250,30 @@
       <c r="M22" s="9"/>
       <c r="N22" s="3">
         <f t="shared" si="2"/>
-        <v>4820</v>
+        <v>4680</v>
       </c>
       <c r="O22" s="9">
         <f t="shared" si="3"/>
-        <v>4820</v>
+        <v>4680</v>
       </c>
       <c r="P22" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A23" s="29"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="9">
         <v>3310</v>
       </c>
       <c r="C23" s="9">
         <v>3265</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="D23">
+        <v>3245</v>
+      </c>
+      <c r="E23">
+        <v>3215</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2387,26 +2284,30 @@
       <c r="M23" s="9"/>
       <c r="N23" s="3">
         <f t="shared" si="2"/>
-        <v>3265</v>
+        <v>3215</v>
       </c>
       <c r="O23" s="9">
         <f t="shared" si="3"/>
-        <v>3265</v>
+        <v>3215</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A24" s="29"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="9">
         <v>6160</v>
       </c>
       <c r="C24" s="9">
         <v>6470</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="D24">
+        <v>6445</v>
+      </c>
+      <c r="E24">
+        <v>6360</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -2428,15 +2329,19 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A25" s="29"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="9">
         <v>2825</v>
       </c>
       <c r="C25" s="9">
         <v>2805</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="D25">
+        <v>2745</v>
+      </c>
+      <c r="E25">
+        <v>2870</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -2447,26 +2352,30 @@
       <c r="M25" s="9"/>
       <c r="N25" s="3">
         <f t="shared" si="2"/>
-        <v>2805</v>
+        <v>2745</v>
       </c>
       <c r="O25" s="9">
         <f t="shared" si="3"/>
-        <v>2805</v>
+        <v>2745</v>
       </c>
       <c r="P25" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A26" s="29"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="9">
         <v>4715</v>
       </c>
       <c r="C26" s="9">
         <v>4595</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
+      <c r="D26">
+        <v>4790</v>
+      </c>
+      <c r="E26">
+        <v>4765</v>
+      </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -2488,15 +2397,19 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A27" s="29"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="9">
         <v>4145</v>
       </c>
       <c r="C27" s="9">
         <v>4130</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="D27">
+        <v>4130</v>
+      </c>
+      <c r="E27">
+        <v>4190</v>
+      </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -2518,15 +2431,19 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A28" s="29"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="9">
         <v>6910</v>
       </c>
       <c r="C28" s="9">
         <v>6970</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
+      <c r="D28">
+        <v>7065</v>
+      </c>
+      <c r="E28">
+        <v>7105</v>
+      </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -2548,15 +2465,19 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A29" s="29"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="9">
         <v>3300</v>
       </c>
       <c r="C29" s="9">
         <v>3295</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="D29">
+        <v>3240</v>
+      </c>
+      <c r="E29">
+        <v>3340</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -2567,26 +2488,30 @@
       <c r="M29" s="9"/>
       <c r="N29" s="3">
         <f t="shared" si="2"/>
-        <v>3295</v>
+        <v>3240</v>
       </c>
       <c r="O29" s="9">
         <f t="shared" si="3"/>
-        <v>3295</v>
+        <v>3240</v>
       </c>
       <c r="P29" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A30" s="29"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="9">
         <v>3665</v>
       </c>
       <c r="C30" s="9">
         <v>3705</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
+      <c r="D30">
+        <v>3770</v>
+      </c>
+      <c r="E30">
+        <v>3770</v>
+      </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -2608,15 +2533,19 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A31" s="29"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="9">
         <v>1905</v>
       </c>
       <c r="C31" s="9">
         <v>1935</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="D31">
+        <v>1965</v>
+      </c>
+      <c r="E31">
+        <v>1910</v>
+      </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -2638,15 +2567,19 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A32" s="29"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="9">
         <v>2615</v>
       </c>
       <c r="C32" s="9">
         <v>2590</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="D32">
+        <v>2685</v>
+      </c>
+      <c r="E32">
+        <v>2680</v>
+      </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -2668,15 +2601,19 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A33" s="29"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="9">
         <v>2170</v>
       </c>
       <c r="C33" s="9">
         <v>2135</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
+      <c r="D33">
+        <v>2195</v>
+      </c>
+      <c r="E33">
+        <v>2215</v>
+      </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -2698,28 +2635,32 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="31"/>
-      <c r="B34" s="25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="17">
         <v>2170</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="17">
         <v>2200</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
+      <c r="D34" s="32">
+        <v>2180</v>
+      </c>
+      <c r="E34" s="32">
+        <v>2250</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
       <c r="N34" s="7">
         <f t="shared" si="2"/>
         <v>2170</v>
       </c>
-      <c r="O34" s="25">
+      <c r="O34" s="17">
         <f t="shared" si="3"/>
         <v>2170</v>
       </c>
@@ -2742,19 +2683,19 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:O34">
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>A4=SMALL($A4:$Z4,1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>A4=SMALL($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>A4=SMALL($A4:$Z4,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>A4=LARGE($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="10">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>A4=LARGE($A4:$Z4,1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
reconstruct evaluateObjValue(). project configure change. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="47250" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="49590" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>OldMin</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -103,38 +103,42 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>ACBR_iFAO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>1;w1,w1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>1;w1,w1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_iBNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>ACBR_iFAO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>TSR_LS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>ACBR_iFAO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TSR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SCS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SCS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;w1,w1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;w1,w1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ACBR_iBNO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -143,11 +147,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TSR_LS</t>
+    <t>TSR_RM</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TSR</t>
+    <t>TSR_RMIE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -501,7 +505,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -722,17 +726,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -913,7 +906,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -935,21 +928,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -959,13 +949,13 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1385,63 +1375,63 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="10.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="10.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="24" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="32" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="23"/>
+      <c r="L1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="32"/>
+      <c r="N1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="24"/>
+      <c r="B2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -1450,201 +1440,207 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="L2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="31"/>
+      <c r="M2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="24"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26"/>
-      <c r="B3" s="23" t="s">
-        <v>27</v>
+      <c r="A3" s="25"/>
+      <c r="B3" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="L3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="26"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="31"/>
+        <v>36</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="25"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="30"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="e">
+      <c r="A4" s="12">
         <f>AVERAGE(A6:A129)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B4" s="14">
+        <v>9999</v>
+      </c>
+      <c r="B4" s="13">
         <f>AVERAGE(B6:B19,B21:B34)</f>
         <v>3845.1785714285716</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <f t="shared" ref="C4:O4" si="0">AVERAGE(C6:C19,C21:C34)</f>
         <v>3876.25</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <f t="shared" si="0"/>
         <v>3854.8214285714284</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <f t="shared" si="0"/>
         <v>3898.5714285714284</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <f t="shared" si="0"/>
         <v>3851.4285714285716</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <f t="shared" si="0"/>
         <v>3861.9642857142858</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <f t="shared" si="0"/>
         <v>3823.75</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <f t="shared" si="0"/>
         <v>3860.7142857142858</v>
       </c>
-      <c r="J4" s="14" t="e">
+      <c r="J4" s="13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" s="14" t="e">
+        <v>3831.4285714285716</v>
+      </c>
+      <c r="K4" s="13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" s="14">
+        <v>3833.0357142857142</v>
+      </c>
+      <c r="L4" s="13">
         <f t="shared" si="0"/>
-        <v>3795</v>
-      </c>
-      <c r="M4" s="14">
+        <v>3810.3571428571427</v>
+      </c>
+      <c r="M4" s="13">
         <f t="shared" si="0"/>
-        <v>3775.7142857142858</v>
-      </c>
-      <c r="N4" s="14">
+        <v>3846.6071428571427</v>
+      </c>
+      <c r="N4" s="13">
         <f t="shared" si="0"/>
-        <v>3730.1785714285716</v>
-      </c>
-      <c r="O4" s="14">
+        <v>3698.0357142857142</v>
+      </c>
+      <c r="O4" s="13">
         <f t="shared" si="0"/>
-        <v>3730.1785714285716</v>
-      </c>
-      <c r="P4" s="8"/>
+        <v>3698.0357142857142</v>
+      </c>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15" t="e">
+      <c r="A5" s="14">
         <f>AVERAGE(A6:A19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B5" s="15">
+        <v>9999</v>
+      </c>
+      <c r="B5" s="14">
         <f>AVERAGE(B6:B19)</f>
         <v>3800</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <f t="shared" ref="C5:O5" si="1">AVERAGE(C6:C19)</f>
         <v>3832.5</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <f t="shared" si="1"/>
         <v>3777.1428571428573</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <f t="shared" si="1"/>
         <v>3828.9285714285716</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <f t="shared" si="1"/>
         <v>3797.5</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <f t="shared" si="1"/>
         <v>3791.7857142857142</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <f t="shared" si="1"/>
         <v>3770.3571428571427</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <f t="shared" si="1"/>
         <v>3781.7857142857142</v>
       </c>
-      <c r="J5" s="15" t="e">
+      <c r="J5" s="14">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K5" s="15" t="e">
+        <v>3747.8571428571427</v>
+      </c>
+      <c r="K5" s="14">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="15">
+        <v>3766.0714285714284</v>
+      </c>
+      <c r="L5" s="14">
         <f t="shared" si="1"/>
-        <v>3795</v>
-      </c>
-      <c r="M5" s="15">
+        <v>3748.2142857142858</v>
+      </c>
+      <c r="M5" s="14">
         <f t="shared" si="1"/>
-        <v>3775.7142857142858</v>
-      </c>
-      <c r="N5" s="15">
+        <v>3808.9285714285716</v>
+      </c>
+      <c r="N5" s="14">
         <f t="shared" si="1"/>
-        <v>3668.5714285714284</v>
-      </c>
-      <c r="O5" s="15">
+        <v>3644.2857142857142</v>
+      </c>
+      <c r="O5" s="14">
         <f t="shared" si="1"/>
-        <v>3668.5714285714284</v>
-      </c>
-      <c r="P5" s="11">
+        <v>3644.2857142857142</v>
+      </c>
+      <c r="P5" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15">
+        <v>9999</v>
+      </c>
       <c r="B6" s="6">
         <v>5440</v>
       </c>
@@ -1669,28 +1665,32 @@
       <c r="I6" s="1">
         <v>5240</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="J6" s="6">
+        <v>5190</v>
+      </c>
+      <c r="K6" s="6">
+        <v>5235</v>
+      </c>
       <c r="L6" s="1">
-        <v>5430</v>
-      </c>
-      <c r="M6" s="9">
-        <v>5290</v>
-      </c>
-      <c r="N6" s="21">
+        <v>5225</v>
+      </c>
+      <c r="M6" s="8">
+        <v>5280</v>
+      </c>
+      <c r="N6" s="20">
         <f>MIN(B6:M6)</f>
-        <v>5240</v>
+        <v>5190</v>
       </c>
       <c r="O6" s="6">
         <f>MIN(B6:N6)</f>
-        <v>5240</v>
-      </c>
-      <c r="P6" s="21" t="s">
+        <v>5190</v>
+      </c>
+      <c r="P6" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="6">
         <v>4585</v>
       </c>
@@ -1715,28 +1715,32 @@
       <c r="I7" s="1">
         <v>4660</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="J7" s="6">
+        <v>4610</v>
+      </c>
+      <c r="K7" s="6">
+        <v>4460</v>
+      </c>
       <c r="L7" s="1">
-        <v>4675</v>
-      </c>
-      <c r="M7" s="9">
-        <v>4610</v>
-      </c>
-      <c r="N7" s="21">
+        <v>4550</v>
+      </c>
+      <c r="M7" s="8">
+        <v>4615</v>
+      </c>
+      <c r="N7" s="20">
         <f t="shared" ref="N7:N34" si="2">MIN(B7:M7)</f>
-        <v>4555</v>
+        <v>4460</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" ref="O7:O34" si="3">MIN(B7:N7)</f>
-        <v>4555</v>
-      </c>
-      <c r="P7" s="21" t="s">
+        <v>4460</v>
+      </c>
+      <c r="P7" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" s="16"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="6">
         <v>3150</v>
       </c>
@@ -1761,28 +1765,32 @@
       <c r="I8" s="1">
         <v>3180</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="J8" s="6">
+        <v>3140</v>
+      </c>
+      <c r="K8" s="6">
+        <v>3225</v>
+      </c>
       <c r="L8" s="1">
-        <v>3215</v>
-      </c>
-      <c r="M8" s="9">
-        <v>3200</v>
-      </c>
-      <c r="N8" s="21">
+        <v>3070</v>
+      </c>
+      <c r="M8" s="8">
+        <v>3230</v>
+      </c>
+      <c r="N8" s="20">
         <f t="shared" si="2"/>
-        <v>3150</v>
+        <v>3070</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="3"/>
-        <v>3150</v>
-      </c>
-      <c r="P8" s="21" t="s">
+        <v>3070</v>
+      </c>
+      <c r="P8" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="6">
         <v>6000</v>
       </c>
@@ -1807,28 +1815,32 @@
       <c r="I9" s="1">
         <v>5905</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="J9" s="6">
+        <v>5600</v>
+      </c>
+      <c r="K9" s="6">
+        <v>5750</v>
+      </c>
       <c r="L9" s="1">
-        <v>5925</v>
-      </c>
-      <c r="M9" s="9">
-        <v>5880</v>
-      </c>
-      <c r="N9" s="21">
+        <v>5750</v>
+      </c>
+      <c r="M9" s="8">
+        <v>5835</v>
+      </c>
+      <c r="N9" s="20">
         <f t="shared" si="2"/>
-        <v>5670</v>
+        <v>5600</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="3"/>
-        <v>5670</v>
-      </c>
-      <c r="P9" s="21" t="s">
+        <v>5600</v>
+      </c>
+      <c r="P9" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="6">
         <v>2150</v>
       </c>
@@ -1853,28 +1865,32 @@
       <c r="I10" s="1">
         <v>2105</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="J10" s="6">
+        <v>2195</v>
+      </c>
+      <c r="K10" s="6">
+        <v>2075</v>
+      </c>
       <c r="L10" s="1">
+        <v>2210</v>
+      </c>
+      <c r="M10" s="8">
         <v>2245</v>
       </c>
-      <c r="M10" s="9">
-        <v>2190</v>
-      </c>
-      <c r="N10" s="21">
+      <c r="N10" s="20">
         <f t="shared" si="2"/>
-        <v>2105</v>
+        <v>2075</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="3"/>
-        <v>2105</v>
-      </c>
-      <c r="P10" s="21" t="s">
+        <v>2075</v>
+      </c>
+      <c r="P10" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="6">
         <v>4100</v>
       </c>
@@ -1899,15 +1915,19 @@
       <c r="I11" s="1">
         <v>3980</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="J11" s="6">
+        <v>4100</v>
+      </c>
+      <c r="K11" s="6">
+        <v>4095</v>
+      </c>
       <c r="L11" s="1">
-        <v>4020</v>
-      </c>
-      <c r="M11" s="9">
-        <v>3985</v>
-      </c>
-      <c r="N11" s="21">
+        <v>4005</v>
+      </c>
+      <c r="M11" s="8">
+        <v>4040</v>
+      </c>
+      <c r="N11" s="20">
         <f t="shared" si="2"/>
         <v>3980</v>
       </c>
@@ -1915,12 +1935,12 @@
         <f t="shared" si="3"/>
         <v>3980</v>
       </c>
-      <c r="P11" s="21" t="s">
+      <c r="P11" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="16"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="6">
         <v>4245</v>
       </c>
@@ -1945,15 +1965,19 @@
       <c r="I12" s="1">
         <v>4280</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="J12" s="6">
+        <v>4285</v>
+      </c>
+      <c r="K12" s="6">
+        <v>4370</v>
+      </c>
       <c r="L12" s="1">
-        <v>4250</v>
-      </c>
-      <c r="M12" s="9">
-        <v>4185</v>
-      </c>
-      <c r="N12" s="21">
+        <v>4195</v>
+      </c>
+      <c r="M12" s="8">
+        <v>4345</v>
+      </c>
+      <c r="N12" s="20">
         <f t="shared" si="2"/>
         <v>4140</v>
       </c>
@@ -1961,12 +1985,12 @@
         <f t="shared" si="3"/>
         <v>4140</v>
       </c>
-      <c r="P12" s="21" t="s">
+      <c r="P12" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="6">
         <v>7100</v>
       </c>
@@ -1991,15 +2015,19 @@
       <c r="I13" s="1">
         <v>7405</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="J13" s="6">
+        <v>7105</v>
+      </c>
+      <c r="K13" s="6">
+        <v>7080</v>
+      </c>
       <c r="L13" s="1">
-        <v>7160</v>
-      </c>
-      <c r="M13" s="9">
-        <v>7190</v>
-      </c>
-      <c r="N13" s="21">
+        <v>7065</v>
+      </c>
+      <c r="M13" s="8">
+        <v>7285</v>
+      </c>
+      <c r="N13" s="20">
         <f t="shared" si="2"/>
         <v>6850</v>
       </c>
@@ -2007,12 +2035,12 @@
         <f t="shared" si="3"/>
         <v>6850</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A14" s="16"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="6">
         <v>3135</v>
       </c>
@@ -2037,15 +2065,19 @@
       <c r="I14" s="1">
         <v>3140</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="J14" s="6">
+        <v>3115</v>
+      </c>
+      <c r="K14" s="6">
+        <v>3270</v>
+      </c>
       <c r="L14" s="1">
-        <v>3060</v>
-      </c>
-      <c r="M14" s="9">
-        <v>3135</v>
-      </c>
-      <c r="N14" s="21">
+        <v>3240</v>
+      </c>
+      <c r="M14" s="8">
+        <v>3215</v>
+      </c>
+      <c r="N14" s="20">
         <f t="shared" si="2"/>
         <v>2980</v>
       </c>
@@ -2053,12 +2085,12 @@
         <f t="shared" si="3"/>
         <v>2980</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="6">
         <v>4300</v>
       </c>
@@ -2083,15 +2115,19 @@
       <c r="I15" s="1">
         <v>4175</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="J15" s="6">
+        <v>4085</v>
+      </c>
+      <c r="K15" s="6">
+        <v>4080</v>
+      </c>
       <c r="L15" s="1">
-        <v>4110</v>
-      </c>
-      <c r="M15" s="9">
-        <v>4155</v>
-      </c>
-      <c r="N15" s="21">
+        <v>4090</v>
+      </c>
+      <c r="M15" s="8">
+        <v>4205</v>
+      </c>
+      <c r="N15" s="20">
         <f t="shared" si="2"/>
         <v>4010</v>
       </c>
@@ -2099,12 +2135,12 @@
         <f t="shared" si="3"/>
         <v>4010</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A16" s="16"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="6">
         <v>1835</v>
       </c>
@@ -2129,15 +2165,19 @@
       <c r="I16" s="1">
         <v>1865</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="J16" s="6">
+        <v>1890</v>
+      </c>
+      <c r="K16" s="6">
+        <v>1915</v>
+      </c>
       <c r="L16" s="1">
-        <v>1955</v>
-      </c>
-      <c r="M16" s="9">
-        <v>1930</v>
-      </c>
-      <c r="N16" s="21">
+        <v>1895</v>
+      </c>
+      <c r="M16" s="8">
+        <v>1890</v>
+      </c>
+      <c r="N16" s="20">
         <f t="shared" si="2"/>
         <v>1835</v>
       </c>
@@ -2145,12 +2185,12 @@
         <f t="shared" si="3"/>
         <v>1835</v>
       </c>
-      <c r="P16" s="21" t="s">
+      <c r="P16" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A17" s="16"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="6">
         <v>3085</v>
       </c>
@@ -2175,15 +2215,19 @@
       <c r="I17" s="1">
         <v>2900</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="J17" s="6">
+        <v>3170</v>
+      </c>
+      <c r="K17" s="6">
+        <v>3065</v>
+      </c>
       <c r="L17" s="1">
-        <v>2975</v>
-      </c>
-      <c r="M17" s="9">
-        <v>3115</v>
-      </c>
-      <c r="N17" s="21">
+        <v>2995</v>
+      </c>
+      <c r="M17" s="8">
+        <v>3170</v>
+      </c>
+      <c r="N17" s="20">
         <f t="shared" si="2"/>
         <v>2900</v>
       </c>
@@ -2191,12 +2235,12 @@
         <f t="shared" si="3"/>
         <v>2900</v>
       </c>
-      <c r="P17" s="21" t="s">
+      <c r="P17" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A18" s="16"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="6">
         <v>2010</v>
       </c>
@@ -2221,28 +2265,32 @@
       <c r="I18" s="1">
         <v>1990</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="J18" s="6">
+        <v>1930</v>
+      </c>
+      <c r="K18" s="6">
+        <v>2030</v>
+      </c>
       <c r="L18" s="1">
-        <v>2005</v>
-      </c>
-      <c r="M18" s="9">
-        <v>1935</v>
-      </c>
-      <c r="N18" s="21">
+        <v>2080</v>
+      </c>
+      <c r="M18" s="8">
+        <v>1920</v>
+      </c>
+      <c r="N18" s="20">
         <f t="shared" si="2"/>
-        <v>1935</v>
+        <v>1920</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="3"/>
-        <v>1935</v>
-      </c>
-      <c r="P18" s="21" t="s">
+        <v>1920</v>
+      </c>
+      <c r="P18" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A19" s="16"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="6">
         <v>2065</v>
       </c>
@@ -2267,15 +2315,19 @@
       <c r="I19" s="1">
         <v>2120</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="J19" s="6">
+        <v>2055</v>
+      </c>
+      <c r="K19" s="6">
+        <v>2075</v>
+      </c>
       <c r="L19" s="1">
         <v>2105</v>
       </c>
-      <c r="M19" s="9">
-        <v>2060</v>
-      </c>
-      <c r="N19" s="21">
+      <c r="M19" s="8">
+        <v>2050</v>
+      </c>
+      <c r="N19" s="20">
         <f t="shared" si="2"/>
         <v>2010</v>
       </c>
@@ -2283,77 +2335,79 @@
         <f t="shared" si="3"/>
         <v>2010</v>
       </c>
-      <c r="P19" s="21" t="s">
+      <c r="P19" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A20" s="17" t="e">
+      <c r="A20" s="16">
         <f>AVERAGE(A21:A34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B20" s="17">
+        <v>9999</v>
+      </c>
+      <c r="B20" s="16">
         <f>AVERAGE(B21:B34)</f>
         <v>3890.3571428571427</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="16">
         <f t="shared" ref="C20:O20" si="4">AVERAGE(C21:C34)</f>
         <v>3920</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <f t="shared" si="4"/>
         <v>3932.5</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <f t="shared" si="4"/>
         <v>3968.2142857142858</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="16">
         <f t="shared" si="4"/>
         <v>3905.3571428571427</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="16">
         <f t="shared" si="4"/>
         <v>3932.1428571428573</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="16">
         <f t="shared" si="4"/>
         <v>3877.1428571428573</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="16">
         <f t="shared" si="4"/>
         <v>3939.6428571428573</v>
       </c>
-      <c r="J20" s="17" t="e">
+      <c r="J20" s="16">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="17" t="e">
+        <v>3915</v>
+      </c>
+      <c r="K20" s="16">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="17" t="e">
+        <v>3900</v>
+      </c>
+      <c r="L20" s="16">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="17" t="e">
+        <v>3872.5</v>
+      </c>
+      <c r="M20" s="16">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" s="17">
+        <v>3884.2857142857142</v>
+      </c>
+      <c r="N20" s="16">
         <f t="shared" si="4"/>
-        <v>3791.7857142857142</v>
-      </c>
-      <c r="O20" s="17">
+        <v>3751.7857142857142</v>
+      </c>
+      <c r="O20" s="16">
         <f t="shared" si="4"/>
-        <v>3791.7857142857142</v>
-      </c>
-      <c r="P20" s="10">
+        <v>3751.7857142857142</v>
+      </c>
+      <c r="P20" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A21" s="16"/>
+      <c r="A21" s="15">
+        <v>9999</v>
+      </c>
       <c r="B21" s="6">
         <v>5755</v>
       </c>
@@ -2378,24 +2432,32 @@
       <c r="I21" s="6">
         <v>5950</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="21">
+      <c r="J21" s="6">
+        <v>5190</v>
+      </c>
+      <c r="K21" s="6">
+        <v>5600</v>
+      </c>
+      <c r="L21" s="6">
+        <v>5655</v>
+      </c>
+      <c r="M21" s="6">
+        <v>5355</v>
+      </c>
+      <c r="N21" s="20">
         <f t="shared" si="2"/>
-        <v>5695</v>
+        <v>5190</v>
       </c>
       <c r="O21" s="6">
         <f t="shared" si="3"/>
-        <v>5695</v>
-      </c>
-      <c r="P21" s="21" t="s">
+        <v>5190</v>
+      </c>
+      <c r="P21" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="6">
         <v>4820</v>
       </c>
@@ -2420,11 +2482,19 @@
       <c r="I22" s="6">
         <v>4735</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="21">
+      <c r="J22" s="6">
+        <v>5090</v>
+      </c>
+      <c r="K22" s="6">
+        <v>5055</v>
+      </c>
+      <c r="L22" s="6">
+        <v>4820</v>
+      </c>
+      <c r="M22" s="6">
+        <v>4870</v>
+      </c>
+      <c r="N22" s="20">
         <f t="shared" si="2"/>
         <v>4585</v>
       </c>
@@ -2432,12 +2502,12 @@
         <f t="shared" si="3"/>
         <v>4585</v>
       </c>
-      <c r="P22" s="21" t="s">
+      <c r="P22" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="6">
         <v>3310</v>
       </c>
@@ -2462,11 +2532,19 @@
       <c r="I23" s="6">
         <v>3330</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="21">
+      <c r="J23" s="6">
+        <v>3380</v>
+      </c>
+      <c r="K23" s="6">
+        <v>3290</v>
+      </c>
+      <c r="L23" s="6">
+        <v>3250</v>
+      </c>
+      <c r="M23" s="6">
+        <v>3280</v>
+      </c>
+      <c r="N23" s="20">
         <f t="shared" si="2"/>
         <v>3195</v>
       </c>
@@ -2474,12 +2552,12 @@
         <f t="shared" si="3"/>
         <v>3195</v>
       </c>
-      <c r="P23" s="21" t="s">
+      <c r="P23" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="6">
         <v>6160</v>
       </c>
@@ -2504,11 +2582,19 @@
       <c r="I24" s="6">
         <v>6555</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="21">
+      <c r="J24" s="6">
+        <v>6220</v>
+      </c>
+      <c r="K24" s="6">
+        <v>6225</v>
+      </c>
+      <c r="L24" s="6">
+        <v>6275</v>
+      </c>
+      <c r="M24" s="6">
+        <v>6290</v>
+      </c>
+      <c r="N24" s="20">
         <f t="shared" si="2"/>
         <v>6160</v>
       </c>
@@ -2516,12 +2602,12 @@
         <f t="shared" si="3"/>
         <v>6160</v>
       </c>
-      <c r="P24" s="21" t="s">
+      <c r="P24" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="6">
         <v>2825</v>
       </c>
@@ -2546,11 +2632,19 @@
       <c r="I25" s="6">
         <v>2685</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="21">
+      <c r="J25" s="6">
+        <v>2750</v>
+      </c>
+      <c r="K25" s="6">
+        <v>2650</v>
+      </c>
+      <c r="L25" s="6">
+        <v>2625</v>
+      </c>
+      <c r="M25" s="6">
+        <v>2615</v>
+      </c>
+      <c r="N25" s="20">
         <f t="shared" si="2"/>
         <v>2580</v>
       </c>
@@ -2558,12 +2652,12 @@
         <f t="shared" si="3"/>
         <v>2580</v>
       </c>
-      <c r="P25" s="21" t="s">
+      <c r="P25" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="6">
         <v>4715</v>
       </c>
@@ -2588,11 +2682,19 @@
       <c r="I26" s="6">
         <v>4485</v>
       </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="21">
+      <c r="J26" s="6">
+        <v>4850</v>
+      </c>
+      <c r="K26" s="6">
+        <v>4445</v>
+      </c>
+      <c r="L26" s="6">
+        <v>4555</v>
+      </c>
+      <c r="M26" s="6">
+        <v>4675</v>
+      </c>
+      <c r="N26" s="20">
         <f t="shared" si="2"/>
         <v>4435</v>
       </c>
@@ -2600,12 +2702,12 @@
         <f t="shared" si="3"/>
         <v>4435</v>
       </c>
-      <c r="P26" s="21" t="s">
+      <c r="P26" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="6">
         <v>4145</v>
       </c>
@@ -2630,24 +2732,32 @@
       <c r="I27" s="6">
         <v>4135</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="21">
+      <c r="J27" s="6">
+        <v>4165</v>
+      </c>
+      <c r="K27" s="6">
+        <v>4135</v>
+      </c>
+      <c r="L27" s="6">
+        <v>4170</v>
+      </c>
+      <c r="M27" s="6">
+        <v>4075</v>
+      </c>
+      <c r="N27" s="20">
         <f t="shared" si="2"/>
-        <v>4085</v>
+        <v>4075</v>
       </c>
       <c r="O27" s="6">
         <f t="shared" si="3"/>
-        <v>4085</v>
-      </c>
-      <c r="P27" s="21" t="s">
+        <v>4075</v>
+      </c>
+      <c r="P27" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A28" s="16"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="6">
         <v>6910</v>
       </c>
@@ -2672,11 +2782,19 @@
       <c r="I28" s="6">
         <v>7120</v>
       </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="21">
+      <c r="J28" s="6">
+        <v>7035</v>
+      </c>
+      <c r="K28" s="6">
+        <v>7040</v>
+      </c>
+      <c r="L28" s="6">
+        <v>6830</v>
+      </c>
+      <c r="M28" s="6">
+        <v>6985</v>
+      </c>
+      <c r="N28" s="20">
         <f t="shared" si="2"/>
         <v>6780</v>
       </c>
@@ -2684,12 +2802,12 @@
         <f t="shared" si="3"/>
         <v>6780</v>
       </c>
-      <c r="P28" s="21" t="s">
+      <c r="P28" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A29" s="16"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="6">
         <v>3300</v>
       </c>
@@ -2714,11 +2832,19 @@
       <c r="I29" s="6">
         <v>3425</v>
       </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="21">
+      <c r="J29" s="6">
+        <v>3390</v>
+      </c>
+      <c r="K29" s="6">
+        <v>3425</v>
+      </c>
+      <c r="L29" s="6">
+        <v>3340</v>
+      </c>
+      <c r="M29" s="6">
+        <v>3470</v>
+      </c>
+      <c r="N29" s="20">
         <f t="shared" si="2"/>
         <v>3240</v>
       </c>
@@ -2726,12 +2852,12 @@
         <f t="shared" si="3"/>
         <v>3240</v>
       </c>
-      <c r="P29" s="21" t="s">
+      <c r="P29" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A30" s="16"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="6">
         <v>3665</v>
       </c>
@@ -2756,11 +2882,19 @@
       <c r="I30" s="6">
         <v>3720</v>
       </c>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="21">
+      <c r="J30" s="6">
+        <v>3710</v>
+      </c>
+      <c r="K30" s="6">
+        <v>3785</v>
+      </c>
+      <c r="L30" s="6">
+        <v>3815</v>
+      </c>
+      <c r="M30" s="6">
+        <v>3860</v>
+      </c>
+      <c r="N30" s="20">
         <f t="shared" si="2"/>
         <v>3595</v>
       </c>
@@ -2768,12 +2902,12 @@
         <f t="shared" si="3"/>
         <v>3595</v>
       </c>
-      <c r="P30" s="21" t="s">
+      <c r="P30" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="6">
         <v>1905</v>
       </c>
@@ -2798,24 +2932,32 @@
       <c r="I31" s="6">
         <v>1920</v>
       </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="21">
+      <c r="J31" s="6">
+        <v>1915</v>
+      </c>
+      <c r="K31" s="6">
+        <v>1910</v>
+      </c>
+      <c r="L31" s="6">
+        <v>1830</v>
+      </c>
+      <c r="M31" s="6">
+        <v>1865</v>
+      </c>
+      <c r="N31" s="20">
         <f t="shared" si="2"/>
-        <v>1840</v>
+        <v>1830</v>
       </c>
       <c r="O31" s="6">
         <f t="shared" si="3"/>
-        <v>1840</v>
-      </c>
-      <c r="P31" s="21" t="s">
+        <v>1830</v>
+      </c>
+      <c r="P31" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A32" s="16"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="6">
         <v>2615</v>
       </c>
@@ -2840,11 +2982,19 @@
       <c r="I32" s="6">
         <v>2705</v>
       </c>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="21">
+      <c r="J32" s="6">
+        <v>2730</v>
+      </c>
+      <c r="K32" s="6">
+        <v>2670</v>
+      </c>
+      <c r="L32" s="6">
+        <v>2635</v>
+      </c>
+      <c r="M32" s="6">
+        <v>2665</v>
+      </c>
+      <c r="N32" s="20">
         <f t="shared" si="2"/>
         <v>2590</v>
       </c>
@@ -2852,12 +3002,12 @@
         <f t="shared" si="3"/>
         <v>2590</v>
       </c>
-      <c r="P32" s="21" t="s">
+      <c r="P32" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A33" s="16"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="6">
         <v>2170</v>
       </c>
@@ -2882,11 +3032,19 @@
       <c r="I33" s="6">
         <v>2185</v>
       </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="21">
+      <c r="J33" s="6">
+        <v>2205</v>
+      </c>
+      <c r="K33" s="6">
+        <v>2235</v>
+      </c>
+      <c r="L33" s="6">
+        <v>2220</v>
+      </c>
+      <c r="M33" s="6">
+        <v>2150</v>
+      </c>
+      <c r="N33" s="20">
         <f t="shared" si="2"/>
         <v>2135</v>
       </c>
@@ -2894,47 +3052,55 @@
         <f t="shared" si="3"/>
         <v>2135</v>
       </c>
-      <c r="P33" s="21" t="s">
+      <c r="P33" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="12">
+      <c r="A34" s="17"/>
+      <c r="B34" s="11">
         <v>2170</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="11">
         <v>2200</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="19">
         <v>2180</v>
       </c>
-      <c r="E34" s="20">
+      <c r="E34" s="19">
         <v>2250</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="11">
         <v>2215</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="11">
         <v>2180</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="11">
         <v>2190</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="11">
         <v>2205</v>
       </c>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
+      <c r="J34" s="11">
+        <v>2180</v>
+      </c>
+      <c r="K34" s="11">
+        <v>2135</v>
+      </c>
+      <c r="L34" s="11">
+        <v>2195</v>
+      </c>
+      <c r="M34" s="11">
+        <v>2225</v>
+      </c>
       <c r="N34" s="4">
         <f t="shared" si="2"/>
-        <v>2170</v>
-      </c>
-      <c r="O34" s="12">
+        <v>2135</v>
+      </c>
+      <c r="O34" s="11">
         <f t="shared" si="3"/>
-        <v>2170</v>
+        <v>2135</v>
       </c>
       <c r="P34" s="4" t="s">
         <v>21</v>
@@ -2944,7 +3110,7 @@
       <c r="N35" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="N1:N3"/>
     <mergeCell ref="O1:O3"/>
     <mergeCell ref="P1:P3"/>
@@ -2954,6 +3120,7 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:O34">

</xml_diff>

<commit_message>
bug fix on BiasTabuSearch. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="49590" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="51930" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;w1,n0.25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>1;w1,w1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -152,6 +148,10 @@
   </si>
   <si>
     <t>TSR_RMIE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTS</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -906,7 +906,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -952,13 +952,7 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1375,63 +1369,63 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="10.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="10.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.5" style="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="21"/>
+      <c r="L1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="30"/>
+      <c r="N1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22"/>
+      <c r="B2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -1440,87 +1434,86 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="M2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="22"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="28"/>
+    </row>
+    <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23"/>
+      <c r="B3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="30"/>
-    </row>
-    <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="30"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
-        <f>AVERAGE(A6:A129)</f>
-        <v>9999</v>
+        <v>3701.7857142857142</v>
       </c>
       <c r="B4" s="13">
         <f>AVERAGE(B6:B19,B21:B34)</f>
-        <v>3845.1785714285716</v>
+        <v>3803.75</v>
       </c>
       <c r="C4" s="13">
         <f t="shared" ref="C4:O4" si="0">AVERAGE(C6:C19,C21:C34)</f>
-        <v>3876.25</v>
+        <v>3846.7857142857142</v>
       </c>
       <c r="D4" s="13">
         <f t="shared" si="0"/>
@@ -1548,11 +1541,11 @@
       </c>
       <c r="J4" s="13">
         <f t="shared" si="0"/>
-        <v>3831.4285714285716</v>
+        <v>3823.9285714285716</v>
       </c>
       <c r="K4" s="13">
         <f t="shared" si="0"/>
-        <v>3833.0357142857142</v>
+        <v>3837.3214285714284</v>
       </c>
       <c r="L4" s="13">
         <f t="shared" si="0"/>
@@ -1564,26 +1557,25 @@
       </c>
       <c r="N4" s="13">
         <f t="shared" si="0"/>
-        <v>3698.0357142857142</v>
+        <v>3702.8571428571427</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" si="0"/>
-        <v>3698.0357142857142</v>
+        <v>3699.2857142857142</v>
       </c>
       <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="14">
-        <f>AVERAGE(A6:A19)</f>
-        <v>9999</v>
+        <v>3641.7857142857142</v>
       </c>
       <c r="B5" s="14">
         <f>AVERAGE(B6:B19)</f>
-        <v>3800</v>
+        <v>3729.2857142857142</v>
       </c>
       <c r="C5" s="14">
         <f t="shared" ref="C5:O5" si="1">AVERAGE(C6:C19)</f>
-        <v>3832.5</v>
+        <v>3786.4285714285716</v>
       </c>
       <c r="D5" s="14">
         <f t="shared" si="1"/>
@@ -1611,11 +1603,11 @@
       </c>
       <c r="J5" s="14">
         <f t="shared" si="1"/>
-        <v>3747.8571428571427</v>
+        <v>3757.1428571428573</v>
       </c>
       <c r="K5" s="14">
         <f t="shared" si="1"/>
-        <v>3766.0714285714284</v>
+        <v>3793.5714285714284</v>
       </c>
       <c r="L5" s="14">
         <f t="shared" si="1"/>
@@ -1627,25 +1619,25 @@
       </c>
       <c r="N5" s="14">
         <f t="shared" si="1"/>
-        <v>3644.2857142857142</v>
+        <v>3636.7857142857142</v>
       </c>
       <c r="O5" s="14">
         <f t="shared" si="1"/>
-        <v>3644.2857142857142</v>
+        <v>3636.7857142857142</v>
       </c>
       <c r="P5" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="15">
-        <v>9999</v>
+      <c r="A6" s="18">
+        <v>5035</v>
       </c>
       <c r="B6" s="6">
-        <v>5440</v>
+        <v>5125</v>
       </c>
       <c r="C6" s="6">
-        <v>5515</v>
+        <v>5405</v>
       </c>
       <c r="D6" s="1">
         <v>5515</v>
@@ -1666,10 +1658,10 @@
         <v>5240</v>
       </c>
       <c r="J6" s="6">
-        <v>5190</v>
+        <v>5035</v>
       </c>
       <c r="K6" s="6">
-        <v>5235</v>
+        <v>5320</v>
       </c>
       <c r="L6" s="1">
         <v>5225</v>
@@ -1677,25 +1669,27 @@
       <c r="M6" s="8">
         <v>5280</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="18">
         <f>MIN(B6:M6)</f>
-        <v>5190</v>
+        <v>5035</v>
       </c>
       <c r="O6" s="6">
-        <f>MIN(B6:N6)</f>
-        <v>5190</v>
-      </c>
-      <c r="P6" s="20" t="s">
+        <f>MIN(A6:N6)</f>
+        <v>5035</v>
+      </c>
+      <c r="P6" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="15"/>
+      <c r="A7" s="18">
+        <v>4550</v>
+      </c>
       <c r="B7" s="6">
-        <v>4585</v>
+        <v>4520</v>
       </c>
       <c r="C7" s="6">
-        <v>4750</v>
+        <v>4505</v>
       </c>
       <c r="D7" s="1">
         <v>4645</v>
@@ -1716,10 +1710,10 @@
         <v>4660</v>
       </c>
       <c r="J7" s="6">
-        <v>4610</v>
+        <v>4750</v>
       </c>
       <c r="K7" s="6">
-        <v>4460</v>
+        <v>4745</v>
       </c>
       <c r="L7" s="1">
         <v>4550</v>
@@ -1727,25 +1721,27 @@
       <c r="M7" s="8">
         <v>4615</v>
       </c>
-      <c r="N7" s="20">
+      <c r="N7" s="18">
         <f t="shared" ref="N7:N34" si="2">MIN(B7:M7)</f>
-        <v>4460</v>
+        <v>4505</v>
       </c>
       <c r="O7" s="6">
-        <f t="shared" ref="O7:O34" si="3">MIN(B7:N7)</f>
-        <v>4460</v>
-      </c>
-      <c r="P7" s="20" t="s">
+        <f t="shared" ref="O7:O19" si="3">MIN(A7:N7)</f>
+        <v>4505</v>
+      </c>
+      <c r="P7" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" s="15"/>
+      <c r="A8" s="18">
+        <v>3070</v>
+      </c>
       <c r="B8" s="6">
-        <v>3150</v>
+        <v>3265</v>
       </c>
       <c r="C8" s="6">
-        <v>3265</v>
+        <v>3205</v>
       </c>
       <c r="D8" s="1">
         <v>3310</v>
@@ -1766,10 +1762,10 @@
         <v>3180</v>
       </c>
       <c r="J8" s="6">
-        <v>3140</v>
+        <v>3145</v>
       </c>
       <c r="K8" s="6">
-        <v>3225</v>
+        <v>3245</v>
       </c>
       <c r="L8" s="1">
         <v>3070</v>
@@ -1777,7 +1773,7 @@
       <c r="M8" s="8">
         <v>3230</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="18">
         <f t="shared" si="2"/>
         <v>3070</v>
       </c>
@@ -1785,17 +1781,19 @@
         <f t="shared" si="3"/>
         <v>3070</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
+      <c r="A9" s="18">
+        <v>5670</v>
+      </c>
       <c r="B9" s="6">
-        <v>6000</v>
+        <v>5760</v>
       </c>
       <c r="C9" s="6">
-        <v>5950</v>
+        <v>5740</v>
       </c>
       <c r="D9" s="1">
         <v>5860</v>
@@ -1816,10 +1814,10 @@
         <v>5905</v>
       </c>
       <c r="J9" s="6">
-        <v>5600</v>
+        <v>5795</v>
       </c>
       <c r="K9" s="6">
-        <v>5750</v>
+        <v>5775</v>
       </c>
       <c r="L9" s="1">
         <v>5750</v>
@@ -1827,25 +1825,27 @@
       <c r="M9" s="8">
         <v>5835</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="18">
         <f t="shared" si="2"/>
-        <v>5600</v>
+        <v>5670</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="3"/>
-        <v>5600</v>
-      </c>
-      <c r="P9" s="20" t="s">
+        <v>5670</v>
+      </c>
+      <c r="P9" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="15"/>
+      <c r="A10" s="18">
+        <v>2085</v>
+      </c>
       <c r="B10" s="6">
-        <v>2150</v>
+        <v>2170</v>
       </c>
       <c r="C10" s="6">
-        <v>2280</v>
+        <v>2220</v>
       </c>
       <c r="D10" s="1">
         <v>2160</v>
@@ -1866,10 +1866,10 @@
         <v>2105</v>
       </c>
       <c r="J10" s="6">
-        <v>2195</v>
+        <v>2205</v>
       </c>
       <c r="K10" s="6">
-        <v>2075</v>
+        <v>2085</v>
       </c>
       <c r="L10" s="1">
         <v>2210</v>
@@ -1877,25 +1877,27 @@
       <c r="M10" s="8">
         <v>2245</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="18">
         <f t="shared" si="2"/>
-        <v>2075</v>
+        <v>2085</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="3"/>
-        <v>2075</v>
-      </c>
-      <c r="P10" s="20" t="s">
+        <v>2085</v>
+      </c>
+      <c r="P10" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A11" s="15"/>
+      <c r="A11" s="18">
+        <v>3970</v>
+      </c>
       <c r="B11" s="6">
-        <v>4100</v>
+        <v>3980</v>
       </c>
       <c r="C11" s="6">
-        <v>4070</v>
+        <v>4045</v>
       </c>
       <c r="D11" s="1">
         <v>4085</v>
@@ -1916,10 +1918,10 @@
         <v>3980</v>
       </c>
       <c r="J11" s="6">
-        <v>4100</v>
+        <v>4120</v>
       </c>
       <c r="K11" s="6">
-        <v>4095</v>
+        <v>3970</v>
       </c>
       <c r="L11" s="1">
         <v>4005</v>
@@ -1927,25 +1929,27 @@
       <c r="M11" s="8">
         <v>4040</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="18">
         <f t="shared" si="2"/>
-        <v>3980</v>
+        <v>3970</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="3"/>
-        <v>3980</v>
-      </c>
-      <c r="P11" s="20" t="s">
+        <v>3970</v>
+      </c>
+      <c r="P11" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="15"/>
+      <c r="A12" s="18">
+        <v>4140</v>
+      </c>
       <c r="B12" s="6">
         <v>4245</v>
       </c>
       <c r="C12" s="6">
-        <v>4195</v>
+        <v>4210</v>
       </c>
       <c r="D12" s="1">
         <v>4235</v>
@@ -1966,10 +1970,10 @@
         <v>4280</v>
       </c>
       <c r="J12" s="6">
-        <v>4285</v>
+        <v>4245</v>
       </c>
       <c r="K12" s="6">
-        <v>4370</v>
+        <v>4210</v>
       </c>
       <c r="L12" s="1">
         <v>4195</v>
@@ -1977,7 +1981,7 @@
       <c r="M12" s="8">
         <v>4345</v>
       </c>
-      <c r="N12" s="20">
+      <c r="N12" s="18">
         <f t="shared" si="2"/>
         <v>4140</v>
       </c>
@@ -1985,17 +1989,19 @@
         <f t="shared" si="3"/>
         <v>4140</v>
       </c>
-      <c r="P12" s="20" t="s">
+      <c r="P12" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A13" s="15"/>
+      <c r="A13" s="18">
+        <v>6850</v>
+      </c>
       <c r="B13" s="6">
-        <v>7100</v>
+        <v>7170</v>
       </c>
       <c r="C13" s="6">
-        <v>7435</v>
+        <v>7380</v>
       </c>
       <c r="D13" s="1">
         <v>6850</v>
@@ -2016,10 +2022,10 @@
         <v>7405</v>
       </c>
       <c r="J13" s="6">
-        <v>7105</v>
+        <v>7035</v>
       </c>
       <c r="K13" s="6">
-        <v>7080</v>
+        <v>7215</v>
       </c>
       <c r="L13" s="1">
         <v>7065</v>
@@ -2027,7 +2033,7 @@
       <c r="M13" s="8">
         <v>7285</v>
       </c>
-      <c r="N13" s="20">
+      <c r="N13" s="18">
         <f t="shared" si="2"/>
         <v>6850</v>
       </c>
@@ -2035,17 +2041,19 @@
         <f t="shared" si="3"/>
         <v>6850</v>
       </c>
-      <c r="P13" s="20" t="s">
+      <c r="P13" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A14" s="15"/>
+      <c r="A14" s="18">
+        <v>2980</v>
+      </c>
       <c r="B14" s="6">
-        <v>3135</v>
+        <v>3225</v>
       </c>
       <c r="C14" s="6">
-        <v>3185</v>
+        <v>3195</v>
       </c>
       <c r="D14" s="1">
         <v>3085</v>
@@ -2066,10 +2074,10 @@
         <v>3140</v>
       </c>
       <c r="J14" s="6">
-        <v>3115</v>
+        <v>3165</v>
       </c>
       <c r="K14" s="6">
-        <v>3270</v>
+        <v>3215</v>
       </c>
       <c r="L14" s="1">
         <v>3240</v>
@@ -2077,7 +2085,7 @@
       <c r="M14" s="8">
         <v>3215</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="18">
         <f t="shared" si="2"/>
         <v>2980</v>
       </c>
@@ -2085,17 +2093,19 @@
         <f t="shared" si="3"/>
         <v>2980</v>
       </c>
-      <c r="P14" s="20" t="s">
+      <c r="P14" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
+      <c r="A15" s="18">
+        <v>4010</v>
+      </c>
       <c r="B15" s="6">
-        <v>4300</v>
+        <v>3985</v>
       </c>
       <c r="C15" s="6">
-        <v>4035</v>
+        <v>4065</v>
       </c>
       <c r="D15" s="1">
         <v>4010</v>
@@ -2116,10 +2126,10 @@
         <v>4175</v>
       </c>
       <c r="J15" s="6">
-        <v>4085</v>
+        <v>4100</v>
       </c>
       <c r="K15" s="6">
-        <v>4080</v>
+        <v>4210</v>
       </c>
       <c r="L15" s="1">
         <v>4090</v>
@@ -2127,25 +2137,27 @@
       <c r="M15" s="8">
         <v>4205</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="18">
         <f t="shared" si="2"/>
-        <v>4010</v>
+        <v>3985</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="3"/>
-        <v>4010</v>
-      </c>
-      <c r="P15" s="20" t="s">
+        <v>3985</v>
+      </c>
+      <c r="P15" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A16" s="15"/>
+      <c r="A16" s="18">
+        <v>1795</v>
+      </c>
       <c r="B16" s="6">
-        <v>1835</v>
+        <v>1850</v>
       </c>
       <c r="C16" s="6">
-        <v>1945</v>
+        <v>1930</v>
       </c>
       <c r="D16" s="1">
         <v>1925</v>
@@ -2166,10 +2178,10 @@
         <v>1865</v>
       </c>
       <c r="J16" s="6">
-        <v>1890</v>
+        <v>1795</v>
       </c>
       <c r="K16" s="6">
-        <v>1915</v>
+        <v>1895</v>
       </c>
       <c r="L16" s="1">
         <v>1895</v>
@@ -2177,25 +2189,27 @@
       <c r="M16" s="8">
         <v>1890</v>
       </c>
-      <c r="N16" s="20">
+      <c r="N16" s="18">
         <f t="shared" si="2"/>
-        <v>1835</v>
+        <v>1795</v>
       </c>
       <c r="O16" s="6">
         <f t="shared" si="3"/>
-        <v>1835</v>
-      </c>
-      <c r="P16" s="20" t="s">
+        <v>1795</v>
+      </c>
+      <c r="P16" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
+      <c r="A17" s="18">
+        <v>2900</v>
+      </c>
       <c r="B17" s="6">
-        <v>3085</v>
+        <v>2935</v>
       </c>
       <c r="C17" s="6">
-        <v>2910</v>
+        <v>3050</v>
       </c>
       <c r="D17" s="1">
         <v>3070</v>
@@ -2216,10 +2230,10 @@
         <v>2900</v>
       </c>
       <c r="J17" s="6">
-        <v>3170</v>
+        <v>3105</v>
       </c>
       <c r="K17" s="6">
-        <v>3065</v>
+        <v>3145</v>
       </c>
       <c r="L17" s="1">
         <v>2995</v>
@@ -2227,7 +2241,7 @@
       <c r="M17" s="8">
         <v>3170</v>
       </c>
-      <c r="N17" s="20">
+      <c r="N17" s="18">
         <f t="shared" si="2"/>
         <v>2900</v>
       </c>
@@ -2235,17 +2249,19 @@
         <f t="shared" si="3"/>
         <v>2900</v>
       </c>
-      <c r="P17" s="20" t="s">
+      <c r="P17" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A18" s="15"/>
+      <c r="A18" s="18">
+        <v>1920</v>
+      </c>
       <c r="B18" s="6">
-        <v>2010</v>
+        <v>1925</v>
       </c>
       <c r="C18" s="6">
-        <v>2020</v>
+        <v>1940</v>
       </c>
       <c r="D18" s="1">
         <v>1990</v>
@@ -2266,10 +2282,10 @@
         <v>1990</v>
       </c>
       <c r="J18" s="6">
-        <v>1930</v>
+        <v>2010</v>
       </c>
       <c r="K18" s="6">
-        <v>2030</v>
+        <v>1970</v>
       </c>
       <c r="L18" s="1">
         <v>2080</v>
@@ -2277,7 +2293,7 @@
       <c r="M18" s="8">
         <v>1920</v>
       </c>
-      <c r="N18" s="20">
+      <c r="N18" s="18">
         <f t="shared" si="2"/>
         <v>1920</v>
       </c>
@@ -2285,17 +2301,19 @@
         <f t="shared" si="3"/>
         <v>1920</v>
       </c>
-      <c r="P18" s="20" t="s">
+      <c r="P18" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
+      <c r="A19" s="18">
+        <v>2010</v>
+      </c>
       <c r="B19" s="6">
-        <v>2065</v>
+        <v>2055</v>
       </c>
       <c r="C19" s="6">
-        <v>2100</v>
+        <v>2120</v>
       </c>
       <c r="D19" s="1">
         <v>2140</v>
@@ -2316,10 +2334,10 @@
         <v>2120</v>
       </c>
       <c r="J19" s="6">
-        <v>2055</v>
+        <v>2095</v>
       </c>
       <c r="K19" s="6">
-        <v>2075</v>
+        <v>2110</v>
       </c>
       <c r="L19" s="1">
         <v>2105</v>
@@ -2327,7 +2345,7 @@
       <c r="M19" s="8">
         <v>2050</v>
       </c>
-      <c r="N19" s="20">
+      <c r="N19" s="18">
         <f t="shared" si="2"/>
         <v>2010</v>
       </c>
@@ -2335,84 +2353,83 @@
         <f t="shared" si="3"/>
         <v>2010</v>
       </c>
-      <c r="P19" s="20" t="s">
+      <c r="P19" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A20" s="16">
-        <f>AVERAGE(A21:A34)</f>
-        <v>9999</v>
-      </c>
-      <c r="B20" s="16">
+      <c r="A20" s="15">
+        <v>3761.7857142857142</v>
+      </c>
+      <c r="B20" s="15">
         <f>AVERAGE(B21:B34)</f>
-        <v>3890.3571428571427</v>
-      </c>
-      <c r="C20" s="16">
+        <v>3878.2142857142858</v>
+      </c>
+      <c r="C20" s="15">
         <f t="shared" ref="C20:O20" si="4">AVERAGE(C21:C34)</f>
-        <v>3920</v>
-      </c>
-      <c r="D20" s="16">
+        <v>3907.1428571428573</v>
+      </c>
+      <c r="D20" s="15">
         <f t="shared" si="4"/>
         <v>3932.5</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="15">
         <f t="shared" si="4"/>
         <v>3968.2142857142858</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="15">
         <f t="shared" si="4"/>
         <v>3905.3571428571427</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="15">
         <f t="shared" si="4"/>
         <v>3932.1428571428573</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="15">
         <f t="shared" si="4"/>
         <v>3877.1428571428573</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="15">
         <f t="shared" si="4"/>
         <v>3939.6428571428573</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J20" s="15">
         <f t="shared" si="4"/>
-        <v>3915</v>
-      </c>
-      <c r="K20" s="16">
+        <v>3890.7142857142858</v>
+      </c>
+      <c r="K20" s="15">
         <f t="shared" si="4"/>
-        <v>3900</v>
-      </c>
-      <c r="L20" s="16">
+        <v>3881.0714285714284</v>
+      </c>
+      <c r="L20" s="15">
         <f t="shared" si="4"/>
         <v>3872.5</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="15">
         <f t="shared" si="4"/>
         <v>3884.2857142857142</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N20" s="15">
         <f t="shared" si="4"/>
-        <v>3751.7857142857142</v>
-      </c>
-      <c r="O20" s="16">
+        <v>3768.9285714285716</v>
+      </c>
+      <c r="O20" s="15">
         <f t="shared" si="4"/>
-        <v>3751.7857142857142</v>
+        <v>3761.7857142857142</v>
       </c>
       <c r="P20" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A21" s="15">
-        <v>9999</v>
+      <c r="A21" s="18">
+        <v>5355</v>
       </c>
       <c r="B21" s="6">
-        <v>5755</v>
+        <v>5675</v>
       </c>
       <c r="C21" s="6">
-        <v>5900</v>
+        <v>5785</v>
       </c>
       <c r="D21" s="1">
         <v>5920</v>
@@ -2433,10 +2450,10 @@
         <v>5950</v>
       </c>
       <c r="J21" s="6">
-        <v>5190</v>
+        <v>5425</v>
       </c>
       <c r="K21" s="6">
-        <v>5600</v>
+        <v>5505</v>
       </c>
       <c r="L21" s="6">
         <v>5655</v>
@@ -2444,25 +2461,27 @@
       <c r="M21" s="6">
         <v>5355</v>
       </c>
-      <c r="N21" s="20">
+      <c r="N21" s="18">
         <f t="shared" si="2"/>
-        <v>5190</v>
+        <v>5355</v>
       </c>
       <c r="O21" s="6">
-        <f t="shared" si="3"/>
-        <v>5190</v>
-      </c>
-      <c r="P21" s="20" t="s">
+        <f>MIN(A21:N21)</f>
+        <v>5355</v>
+      </c>
+      <c r="P21" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A22" s="15"/>
+      <c r="A22" s="18">
+        <v>4585</v>
+      </c>
       <c r="B22" s="6">
-        <v>4820</v>
+        <v>4590</v>
       </c>
       <c r="C22" s="6">
-        <v>4885</v>
+        <v>4655</v>
       </c>
       <c r="D22" s="1">
         <v>4680</v>
@@ -2483,10 +2502,10 @@
         <v>4735</v>
       </c>
       <c r="J22" s="6">
-        <v>5090</v>
+        <v>4950</v>
       </c>
       <c r="K22" s="6">
-        <v>5055</v>
+        <v>4905</v>
       </c>
       <c r="L22" s="6">
         <v>4820</v>
@@ -2494,25 +2513,27 @@
       <c r="M22" s="6">
         <v>4870</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="18">
         <f t="shared" si="2"/>
         <v>4585</v>
       </c>
       <c r="O22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="O22:O34" si="5">MIN(A22:N22)</f>
         <v>4585</v>
       </c>
-      <c r="P22" s="20" t="s">
+      <c r="P22" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
+      <c r="A23" s="18">
+        <v>3195</v>
+      </c>
       <c r="B23" s="6">
-        <v>3310</v>
+        <v>3275</v>
       </c>
       <c r="C23" s="6">
-        <v>3265</v>
+        <v>3305</v>
       </c>
       <c r="D23" s="1">
         <v>3245</v>
@@ -2533,10 +2554,10 @@
         <v>3330</v>
       </c>
       <c r="J23" s="6">
-        <v>3380</v>
+        <v>3295</v>
       </c>
       <c r="K23" s="6">
-        <v>3290</v>
+        <v>3220</v>
       </c>
       <c r="L23" s="6">
         <v>3250</v>
@@ -2544,25 +2565,27 @@
       <c r="M23" s="6">
         <v>3280</v>
       </c>
-      <c r="N23" s="20">
+      <c r="N23" s="18">
         <f t="shared" si="2"/>
         <v>3195</v>
       </c>
       <c r="O23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3195</v>
       </c>
-      <c r="P23" s="20" t="s">
+      <c r="P23" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A24" s="15"/>
+      <c r="A24" s="18">
+        <v>6160</v>
+      </c>
       <c r="B24" s="6">
-        <v>6160</v>
+        <v>6275</v>
       </c>
       <c r="C24" s="6">
-        <v>6470</v>
+        <v>6510</v>
       </c>
       <c r="D24" s="1">
         <v>6445</v>
@@ -2583,10 +2606,10 @@
         <v>6555</v>
       </c>
       <c r="J24" s="6">
-        <v>6220</v>
+        <v>6385</v>
       </c>
       <c r="K24" s="6">
-        <v>6225</v>
+        <v>6205</v>
       </c>
       <c r="L24" s="6">
         <v>6275</v>
@@ -2594,25 +2617,27 @@
       <c r="M24" s="6">
         <v>6290</v>
       </c>
-      <c r="N24" s="20">
+      <c r="N24" s="18">
         <f t="shared" si="2"/>
+        <v>6205</v>
+      </c>
+      <c r="O24" s="6">
+        <f t="shared" si="5"/>
         <v>6160</v>
       </c>
-      <c r="O24" s="6">
-        <f t="shared" si="3"/>
-        <v>6160</v>
-      </c>
-      <c r="P24" s="20" t="s">
+      <c r="P24" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A25" s="15"/>
+      <c r="A25" s="18">
+        <v>2580</v>
+      </c>
       <c r="B25" s="6">
-        <v>2825</v>
+        <v>2790</v>
       </c>
       <c r="C25" s="6">
-        <v>2805</v>
+        <v>2635</v>
       </c>
       <c r="D25" s="1">
         <v>2745</v>
@@ -2633,10 +2658,10 @@
         <v>2685</v>
       </c>
       <c r="J25" s="6">
-        <v>2750</v>
+        <v>2690</v>
       </c>
       <c r="K25" s="6">
-        <v>2650</v>
+        <v>2845</v>
       </c>
       <c r="L25" s="6">
         <v>2625</v>
@@ -2644,25 +2669,27 @@
       <c r="M25" s="6">
         <v>2615</v>
       </c>
-      <c r="N25" s="20">
+      <c r="N25" s="18">
         <f t="shared" si="2"/>
         <v>2580</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2580</v>
       </c>
-      <c r="P25" s="20" t="s">
+      <c r="P25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A26" s="15"/>
+      <c r="A26" s="18">
+        <v>4435</v>
+      </c>
       <c r="B26" s="6">
-        <v>4715</v>
+        <v>4460</v>
       </c>
       <c r="C26" s="6">
-        <v>4595</v>
+        <v>4580</v>
       </c>
       <c r="D26" s="1">
         <v>4790</v>
@@ -2683,10 +2710,10 @@
         <v>4485</v>
       </c>
       <c r="J26" s="6">
-        <v>4850</v>
+        <v>4585</v>
       </c>
       <c r="K26" s="6">
-        <v>4445</v>
+        <v>4585</v>
       </c>
       <c r="L26" s="6">
         <v>4555</v>
@@ -2694,25 +2721,27 @@
       <c r="M26" s="6">
         <v>4675</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="18">
         <f t="shared" si="2"/>
         <v>4435</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4435</v>
       </c>
-      <c r="P26" s="20" t="s">
+      <c r="P26" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A27" s="15"/>
+      <c r="A27" s="18">
+        <v>4075</v>
+      </c>
       <c r="B27" s="6">
-        <v>4145</v>
+        <v>4210</v>
       </c>
       <c r="C27" s="6">
-        <v>4130</v>
+        <v>4165</v>
       </c>
       <c r="D27" s="1">
         <v>4130</v>
@@ -2733,10 +2762,10 @@
         <v>4135</v>
       </c>
       <c r="J27" s="6">
-        <v>4165</v>
+        <v>4170</v>
       </c>
       <c r="K27" s="6">
-        <v>4135</v>
+        <v>4260</v>
       </c>
       <c r="L27" s="6">
         <v>4170</v>
@@ -2744,25 +2773,27 @@
       <c r="M27" s="6">
         <v>4075</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="18">
         <f t="shared" si="2"/>
         <v>4075</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4075</v>
       </c>
-      <c r="P27" s="20" t="s">
+      <c r="P27" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A28" s="15"/>
+      <c r="A28" s="18">
+        <v>6780</v>
+      </c>
       <c r="B28" s="6">
         <v>6910</v>
       </c>
       <c r="C28" s="6">
-        <v>6970</v>
+        <v>6895</v>
       </c>
       <c r="D28" s="1">
         <v>7065</v>
@@ -2783,10 +2814,10 @@
         <v>7120</v>
       </c>
       <c r="J28" s="6">
-        <v>7035</v>
+        <v>6815</v>
       </c>
       <c r="K28" s="6">
-        <v>7040</v>
+        <v>6915</v>
       </c>
       <c r="L28" s="6">
         <v>6830</v>
@@ -2794,25 +2825,27 @@
       <c r="M28" s="6">
         <v>6985</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="18">
         <f t="shared" si="2"/>
         <v>6780</v>
       </c>
       <c r="O28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6780</v>
       </c>
-      <c r="P28" s="20" t="s">
+      <c r="P28" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A29" s="15"/>
+      <c r="A29" s="18">
+        <v>3240</v>
+      </c>
       <c r="B29" s="6">
-        <v>3300</v>
+        <v>3245</v>
       </c>
       <c r="C29" s="6">
-        <v>3295</v>
+        <v>3315</v>
       </c>
       <c r="D29" s="1">
         <v>3240</v>
@@ -2833,10 +2866,10 @@
         <v>3425</v>
       </c>
       <c r="J29" s="6">
-        <v>3390</v>
+        <v>3410</v>
       </c>
       <c r="K29" s="6">
-        <v>3425</v>
+        <v>3450</v>
       </c>
       <c r="L29" s="6">
         <v>3340</v>
@@ -2844,25 +2877,27 @@
       <c r="M29" s="6">
         <v>3470</v>
       </c>
-      <c r="N29" s="20">
+      <c r="N29" s="18">
         <f t="shared" si="2"/>
         <v>3240</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3240</v>
       </c>
-      <c r="P29" s="20" t="s">
+      <c r="P29" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A30" s="15"/>
+      <c r="A30" s="18">
+        <v>3595</v>
+      </c>
       <c r="B30" s="6">
-        <v>3665</v>
+        <v>3720</v>
       </c>
       <c r="C30" s="6">
-        <v>3705</v>
+        <v>3775</v>
       </c>
       <c r="D30" s="1">
         <v>3770</v>
@@ -2883,10 +2918,10 @@
         <v>3720</v>
       </c>
       <c r="J30" s="6">
-        <v>3710</v>
+        <v>3855</v>
       </c>
       <c r="K30" s="6">
-        <v>3785</v>
+        <v>3635</v>
       </c>
       <c r="L30" s="6">
         <v>3815</v>
@@ -2894,25 +2929,27 @@
       <c r="M30" s="6">
         <v>3860</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N30" s="18">
         <f t="shared" si="2"/>
         <v>3595</v>
       </c>
       <c r="O30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3595</v>
       </c>
-      <c r="P30" s="20" t="s">
+      <c r="P30" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A31" s="15"/>
+      <c r="A31" s="18">
+        <v>1830</v>
+      </c>
       <c r="B31" s="6">
-        <v>1905</v>
+        <v>1930</v>
       </c>
       <c r="C31" s="6">
-        <v>1935</v>
+        <v>1925</v>
       </c>
       <c r="D31" s="1">
         <v>1965</v>
@@ -2933,10 +2970,10 @@
         <v>1920</v>
       </c>
       <c r="J31" s="6">
-        <v>1915</v>
+        <v>1865</v>
       </c>
       <c r="K31" s="6">
-        <v>1910</v>
+        <v>1880</v>
       </c>
       <c r="L31" s="6">
         <v>1830</v>
@@ -2944,25 +2981,27 @@
       <c r="M31" s="6">
         <v>1865</v>
       </c>
-      <c r="N31" s="20">
+      <c r="N31" s="18">
         <f t="shared" si="2"/>
         <v>1830</v>
       </c>
       <c r="O31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1830</v>
       </c>
-      <c r="P31" s="20" t="s">
+      <c r="P31" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A32" s="15"/>
+      <c r="A32" s="18">
+        <v>2590</v>
+      </c>
       <c r="B32" s="6">
-        <v>2615</v>
+        <v>2745</v>
       </c>
       <c r="C32" s="6">
-        <v>2590</v>
+        <v>2675</v>
       </c>
       <c r="D32" s="1">
         <v>2685</v>
@@ -2983,10 +3022,10 @@
         <v>2705</v>
       </c>
       <c r="J32" s="6">
-        <v>2730</v>
+        <v>2695</v>
       </c>
       <c r="K32" s="6">
-        <v>2670</v>
+        <v>2635</v>
       </c>
       <c r="L32" s="6">
         <v>2635</v>
@@ -2994,25 +3033,27 @@
       <c r="M32" s="6">
         <v>2665</v>
       </c>
-      <c r="N32" s="20">
+      <c r="N32" s="18">
         <f t="shared" si="2"/>
+        <v>2635</v>
+      </c>
+      <c r="O32" s="6">
+        <f t="shared" si="5"/>
         <v>2590</v>
       </c>
-      <c r="O32" s="6">
-        <f t="shared" si="3"/>
-        <v>2590</v>
-      </c>
-      <c r="P32" s="20" t="s">
+      <c r="P32" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A33" s="15"/>
+      <c r="A33" s="18">
+        <v>2135</v>
+      </c>
       <c r="B33" s="6">
-        <v>2170</v>
+        <v>2210</v>
       </c>
       <c r="C33" s="6">
-        <v>2135</v>
+        <v>2240</v>
       </c>
       <c r="D33" s="1">
         <v>2195</v>
@@ -3033,10 +3074,10 @@
         <v>2185</v>
       </c>
       <c r="J33" s="6">
-        <v>2205</v>
+        <v>2145</v>
       </c>
       <c r="K33" s="6">
-        <v>2235</v>
+        <v>2185</v>
       </c>
       <c r="L33" s="6">
         <v>2220</v>
@@ -3044,30 +3085,32 @@
       <c r="M33" s="6">
         <v>2150</v>
       </c>
-      <c r="N33" s="20">
+      <c r="N33" s="18">
         <f t="shared" si="2"/>
+        <v>2145</v>
+      </c>
+      <c r="O33" s="6">
+        <f t="shared" si="5"/>
         <v>2135</v>
       </c>
-      <c r="O33" s="6">
-        <f t="shared" si="3"/>
-        <v>2135</v>
-      </c>
-      <c r="P33" s="20" t="s">
+      <c r="P33" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
+      <c r="A34" s="4">
+        <v>2110</v>
+      </c>
       <c r="B34" s="11">
-        <v>2170</v>
+        <v>2260</v>
       </c>
       <c r="C34" s="11">
-        <v>2200</v>
-      </c>
-      <c r="D34" s="19">
+        <v>2240</v>
+      </c>
+      <c r="D34" s="17">
         <v>2180</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="17">
         <v>2250</v>
       </c>
       <c r="F34" s="11">
@@ -3083,10 +3126,10 @@
         <v>2205</v>
       </c>
       <c r="J34" s="11">
-        <v>2180</v>
+        <v>2185</v>
       </c>
       <c r="K34" s="11">
-        <v>2135</v>
+        <v>2110</v>
       </c>
       <c r="L34" s="11">
         <v>2195</v>
@@ -3096,11 +3139,11 @@
       </c>
       <c r="N34" s="4">
         <f t="shared" si="2"/>
-        <v>2135</v>
-      </c>
-      <c r="O34" s="11">
-        <f t="shared" si="3"/>
-        <v>2135</v>
+        <v>2110</v>
+      </c>
+      <c r="O34" s="4">
+        <f t="shared" si="5"/>
+        <v>2110</v>
       </c>
       <c r="P34" s="4" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
bug fix on cached block swap. make it configurable for max working weekend penalty counting. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51930" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="54270" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_fBNO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_fFAO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>n120w8</t>
   </si>
   <si>
@@ -103,15 +95,31 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>1;w1,w1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;w1,w1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_iBNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_iFAO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSR_LS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;w1,w1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;w1,w1</t>
+    <t>ACBR_iFAO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -123,15 +131,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TSR_LS</t>
+    <t>TSR_RM</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TSR</t>
+    <t>TSR_RMIE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_iFAO</t>
+    <t>BTS</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -139,19 +147,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_iFAO</t>
+    <t>BTS</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TSR_RM</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSR_RMIE</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BTS</t>
+    <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -906,7 +906,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -965,6 +965,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1369,7 +1372,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1382,126 +1385,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="30"/>
-      <c r="N1" s="21" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="31"/>
+      <c r="N1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="27" t="s">
-        <v>20</v>
+      <c r="P1" s="28" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>34</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="23"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="29"/>
+    </row>
+    <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="K3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="28"/>
-    </row>
-    <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="M3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="28"/>
+        <v>32</v>
+      </c>
+      <c r="N3" s="24"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
@@ -1517,23 +1520,23 @@
       </c>
       <c r="D4" s="13">
         <f t="shared" si="0"/>
-        <v>3854.8214285714284</v>
+        <v>3811.7857142857142</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="0"/>
-        <v>3898.5714285714284</v>
+        <v>3808.9285714285716</v>
       </c>
       <c r="F4" s="13">
         <f t="shared" si="0"/>
-        <v>3851.4285714285716</v>
+        <v>3887.8571428571427</v>
       </c>
       <c r="G4" s="13">
         <f t="shared" si="0"/>
-        <v>3861.9642857142858</v>
+        <v>3875.1785714285716</v>
       </c>
       <c r="H4" s="13">
         <f t="shared" si="0"/>
-        <v>3823.75</v>
+        <v>3869.2857142857142</v>
       </c>
       <c r="I4" s="13">
         <f t="shared" si="0"/>
@@ -1557,11 +1560,11 @@
       </c>
       <c r="N4" s="13">
         <f t="shared" si="0"/>
-        <v>3702.8571428571427</v>
+        <v>3693.3928571428573</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" si="0"/>
-        <v>3699.2857142857142</v>
+        <v>3678.9285714285716</v>
       </c>
       <c r="P4" s="7"/>
     </row>
@@ -1579,23 +1582,23 @@
       </c>
       <c r="D5" s="14">
         <f t="shared" si="1"/>
-        <v>3777.1428571428573</v>
+        <v>3751.4285714285716</v>
       </c>
       <c r="E5" s="14">
         <f t="shared" si="1"/>
-        <v>3828.9285714285716</v>
+        <v>3738.5714285714284</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>3797.5</v>
+        <v>3816.4285714285716</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="1"/>
-        <v>3791.7857142857142</v>
+        <v>3760.3571428571427</v>
       </c>
       <c r="H5" s="14">
         <f t="shared" si="1"/>
-        <v>3770.3571428571427</v>
+        <v>3772.8571428571427</v>
       </c>
       <c r="I5" s="14">
         <f t="shared" si="1"/>
@@ -1619,11 +1622,11 @@
       </c>
       <c r="N5" s="14">
         <f t="shared" si="1"/>
-        <v>3636.7857142857142</v>
+        <v>3636.0714285714284</v>
       </c>
       <c r="O5" s="14">
         <f t="shared" si="1"/>
-        <v>3636.7857142857142</v>
+        <v>3616.4285714285716</v>
       </c>
       <c r="P5" s="10">
         <v>1</v>
@@ -1640,19 +1643,19 @@
         <v>5405</v>
       </c>
       <c r="D6" s="1">
-        <v>5515</v>
+        <v>5360</v>
       </c>
       <c r="E6" s="1">
-        <v>5555</v>
+        <v>5250</v>
       </c>
       <c r="F6" s="1">
-        <v>5330</v>
+        <v>5140</v>
       </c>
       <c r="G6" s="1">
-        <v>5420</v>
+        <v>4855</v>
       </c>
       <c r="H6" s="6">
-        <v>5375</v>
+        <v>4945</v>
       </c>
       <c r="I6" s="1">
         <v>5240</v>
@@ -1671,14 +1674,14 @@
       </c>
       <c r="N6" s="18">
         <f>MIN(B6:M6)</f>
-        <v>5035</v>
+        <v>4855</v>
       </c>
       <c r="O6" s="6">
         <f>MIN(A6:N6)</f>
-        <v>5035</v>
+        <v>4855</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
@@ -1692,19 +1695,19 @@
         <v>4505</v>
       </c>
       <c r="D7" s="1">
-        <v>4645</v>
+        <v>4445</v>
       </c>
       <c r="E7" s="1">
-        <v>4830</v>
+        <v>4550</v>
       </c>
       <c r="F7" s="1">
-        <v>4625</v>
+        <v>5145</v>
       </c>
       <c r="G7" s="1">
-        <v>4665</v>
+        <v>4820</v>
       </c>
       <c r="H7" s="6">
-        <v>4555</v>
+        <v>4705</v>
       </c>
       <c r="I7" s="1">
         <v>4660</v>
@@ -1723,14 +1726,14 @@
       </c>
       <c r="N7" s="18">
         <f t="shared" ref="N7:N34" si="2">MIN(B7:M7)</f>
-        <v>4505</v>
+        <v>4445</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" ref="O7:O19" si="3">MIN(A7:N7)</f>
-        <v>4505</v>
+        <v>4445</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
@@ -1744,19 +1747,19 @@
         <v>3205</v>
       </c>
       <c r="D8" s="1">
-        <v>3310</v>
+        <v>3235</v>
       </c>
       <c r="E8" s="1">
-        <v>3360</v>
+        <v>3230</v>
       </c>
       <c r="F8" s="1">
-        <v>3330</v>
+        <v>3245</v>
       </c>
       <c r="G8" s="1">
-        <v>3335</v>
+        <v>3315</v>
       </c>
       <c r="H8" s="6">
-        <v>3165</v>
+        <v>3200</v>
       </c>
       <c r="I8" s="1">
         <v>3180</v>
@@ -1782,7 +1785,7 @@
         <v>3070</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
@@ -1796,19 +1799,19 @@
         <v>5740</v>
       </c>
       <c r="D9" s="1">
+        <v>5735</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5690</v>
+      </c>
+      <c r="F9" s="1">
         <v>5860</v>
       </c>
-      <c r="E9" s="1">
-        <v>5890</v>
-      </c>
-      <c r="F9" s="1">
-        <v>5835</v>
-      </c>
       <c r="G9" s="1">
-        <v>5820</v>
+        <v>5700</v>
       </c>
       <c r="H9" s="6">
-        <v>5670</v>
+        <v>5840</v>
       </c>
       <c r="I9" s="1">
         <v>5905</v>
@@ -1827,14 +1830,14 @@
       </c>
       <c r="N9" s="18">
         <f t="shared" si="2"/>
-        <v>5670</v>
+        <v>5690</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="3"/>
         <v>5670</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
@@ -1848,19 +1851,19 @@
         <v>2220</v>
       </c>
       <c r="D10" s="1">
-        <v>2160</v>
+        <v>2085</v>
       </c>
       <c r="E10" s="1">
-        <v>2200</v>
+        <v>2180</v>
       </c>
       <c r="F10" s="1">
-        <v>2225</v>
+        <v>2155</v>
       </c>
       <c r="G10" s="1">
-        <v>2205</v>
+        <v>2150</v>
       </c>
       <c r="H10" s="6">
-        <v>2120</v>
+        <v>2185</v>
       </c>
       <c r="I10" s="1">
         <v>2105</v>
@@ -1886,7 +1889,7 @@
         <v>2085</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
@@ -1900,19 +1903,19 @@
         <v>4045</v>
       </c>
       <c r="D11" s="1">
-        <v>4085</v>
+        <v>4035</v>
       </c>
       <c r="E11" s="1">
-        <v>4145</v>
+        <v>3925</v>
       </c>
       <c r="F11" s="1">
-        <v>4020</v>
+        <v>4105</v>
       </c>
       <c r="G11" s="1">
-        <v>4045</v>
+        <v>3965</v>
       </c>
       <c r="H11" s="6">
-        <v>4010</v>
+        <v>4080</v>
       </c>
       <c r="I11" s="1">
         <v>3980</v>
@@ -1931,14 +1934,14 @@
       </c>
       <c r="N11" s="18">
         <f t="shared" si="2"/>
-        <v>3970</v>
+        <v>3925</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="3"/>
-        <v>3970</v>
+        <v>3925</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
@@ -1952,19 +1955,19 @@
         <v>4210</v>
       </c>
       <c r="D12" s="1">
-        <v>4235</v>
+        <v>4260</v>
       </c>
       <c r="E12" s="1">
-        <v>4215</v>
+        <v>4180</v>
       </c>
       <c r="F12" s="1">
-        <v>4215</v>
+        <v>4300</v>
       </c>
       <c r="G12" s="1">
-        <v>4140</v>
+        <v>4325</v>
       </c>
       <c r="H12" s="6">
-        <v>4185</v>
+        <v>4310</v>
       </c>
       <c r="I12" s="1">
         <v>4280</v>
@@ -1983,14 +1986,14 @@
       </c>
       <c r="N12" s="18">
         <f t="shared" si="2"/>
-        <v>4140</v>
+        <v>4180</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="3"/>
         <v>4140</v>
       </c>
       <c r="P12" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
@@ -2004,19 +2007,19 @@
         <v>7380</v>
       </c>
       <c r="D13" s="1">
-        <v>6850</v>
+        <v>7155</v>
       </c>
       <c r="E13" s="1">
-        <v>7245</v>
+        <v>7005</v>
       </c>
       <c r="F13" s="1">
-        <v>7225</v>
+        <v>6995</v>
       </c>
       <c r="G13" s="1">
-        <v>7430</v>
+        <v>6900</v>
       </c>
       <c r="H13" s="6">
-        <v>7335</v>
+        <v>6925</v>
       </c>
       <c r="I13" s="1">
         <v>7405</v>
@@ -2035,14 +2038,14 @@
       </c>
       <c r="N13" s="18">
         <f t="shared" si="2"/>
-        <v>6850</v>
+        <v>6900</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" si="3"/>
         <v>6850</v>
       </c>
       <c r="P13" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
@@ -2056,19 +2059,19 @@
         <v>3195</v>
       </c>
       <c r="D14" s="1">
-        <v>3085</v>
+        <v>3195</v>
       </c>
       <c r="E14" s="1">
-        <v>3035</v>
+        <v>3155</v>
       </c>
       <c r="F14" s="1">
-        <v>3160</v>
+        <v>3225</v>
       </c>
       <c r="G14" s="1">
-        <v>2980</v>
+        <v>3210</v>
       </c>
       <c r="H14" s="6">
-        <v>3020</v>
+        <v>3225</v>
       </c>
       <c r="I14" s="1">
         <v>3140</v>
@@ -2087,14 +2090,14 @@
       </c>
       <c r="N14" s="18">
         <f t="shared" si="2"/>
-        <v>2980</v>
+        <v>3140</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" si="3"/>
         <v>2980</v>
       </c>
       <c r="P14" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
@@ -2108,19 +2111,19 @@
         <v>4065</v>
       </c>
       <c r="D15" s="1">
-        <v>4010</v>
+        <v>4120</v>
       </c>
       <c r="E15" s="1">
-        <v>4030</v>
+        <v>4090</v>
       </c>
       <c r="F15" s="1">
-        <v>4160</v>
+        <v>4230</v>
       </c>
       <c r="G15" s="1">
-        <v>4050</v>
+        <v>4270</v>
       </c>
       <c r="H15" s="6">
-        <v>4230</v>
+        <v>4305</v>
       </c>
       <c r="I15" s="1">
         <v>4175</v>
@@ -2146,7 +2149,7 @@
         <v>3985</v>
       </c>
       <c r="P15" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
@@ -2160,19 +2163,19 @@
         <v>1930</v>
       </c>
       <c r="D16" s="1">
-        <v>1925</v>
+        <v>1850</v>
       </c>
       <c r="E16" s="1">
-        <v>1965</v>
+        <v>1930</v>
       </c>
       <c r="F16" s="1">
-        <v>1860</v>
+        <v>1905</v>
       </c>
       <c r="G16" s="1">
-        <v>1970</v>
+        <v>1855</v>
       </c>
       <c r="H16" s="6">
-        <v>1925</v>
+        <v>1795</v>
       </c>
       <c r="I16" s="1">
         <v>1865</v>
@@ -2198,7 +2201,7 @@
         <v>1795</v>
       </c>
       <c r="P16" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
@@ -2212,19 +2215,19 @@
         <v>3050</v>
       </c>
       <c r="D17" s="1">
-        <v>3070</v>
+        <v>3005</v>
       </c>
       <c r="E17" s="1">
-        <v>3100</v>
+        <v>3125</v>
       </c>
       <c r="F17" s="1">
-        <v>3215</v>
+        <v>3130</v>
       </c>
       <c r="G17" s="1">
-        <v>2975</v>
+        <v>3195</v>
       </c>
       <c r="H17" s="6">
-        <v>3050</v>
+        <v>3275</v>
       </c>
       <c r="I17" s="1">
         <v>2900</v>
@@ -2250,7 +2253,7 @@
         <v>2900</v>
       </c>
       <c r="P17" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
@@ -2264,19 +2267,19 @@
         <v>1940</v>
       </c>
       <c r="D18" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1945</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1980</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H18" s="6">
         <v>1990</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1980</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1950</v>
-      </c>
-      <c r="G18" s="1">
-        <v>2040</v>
-      </c>
-      <c r="H18" s="6">
-        <v>2020</v>
       </c>
       <c r="I18" s="1">
         <v>1990</v>
@@ -2302,7 +2305,7 @@
         <v>1920</v>
       </c>
       <c r="P18" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
@@ -2316,19 +2319,19 @@
         <v>2120</v>
       </c>
       <c r="D19" s="1">
-        <v>2140</v>
+        <v>2025</v>
       </c>
       <c r="E19" s="1">
-        <v>2055</v>
+        <v>2085</v>
       </c>
       <c r="F19" s="1">
         <v>2015</v>
       </c>
       <c r="G19" s="1">
-        <v>2010</v>
+        <v>2085</v>
       </c>
       <c r="H19" s="6">
-        <v>2125</v>
+        <v>2040</v>
       </c>
       <c r="I19" s="1">
         <v>2120</v>
@@ -2347,14 +2350,14 @@
       </c>
       <c r="N19" s="18">
         <f t="shared" si="2"/>
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="O19" s="6">
         <f t="shared" si="3"/>
         <v>2010</v>
       </c>
       <c r="P19" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
@@ -2371,23 +2374,23 @@
       </c>
       <c r="D20" s="15">
         <f t="shared" si="4"/>
-        <v>3932.5</v>
+        <v>3872.1428571428573</v>
       </c>
       <c r="E20" s="15">
         <f t="shared" si="4"/>
-        <v>3968.2142857142858</v>
+        <v>3879.2857142857142</v>
       </c>
       <c r="F20" s="15">
         <f t="shared" si="4"/>
-        <v>3905.3571428571427</v>
+        <v>3959.2857142857142</v>
       </c>
       <c r="G20" s="15">
         <f t="shared" si="4"/>
-        <v>3932.1428571428573</v>
+        <v>3990</v>
       </c>
       <c r="H20" s="15">
         <f t="shared" si="4"/>
-        <v>3877.1428571428573</v>
+        <v>3965.7142857142858</v>
       </c>
       <c r="I20" s="15">
         <f t="shared" si="4"/>
@@ -2411,11 +2414,11 @@
       </c>
       <c r="N20" s="15">
         <f t="shared" si="4"/>
-        <v>3768.9285714285716</v>
+        <v>3750.7142857142858</v>
       </c>
       <c r="O20" s="15">
         <f t="shared" si="4"/>
-        <v>3761.7857142857142</v>
+        <v>3741.4285714285716</v>
       </c>
       <c r="P20" s="9">
         <v>0</v>
@@ -2432,19 +2435,19 @@
         <v>5785</v>
       </c>
       <c r="D21" s="1">
-        <v>5920</v>
+        <v>5880</v>
       </c>
       <c r="E21" s="1">
-        <v>6080</v>
+        <v>5675</v>
       </c>
       <c r="F21" s="6">
-        <v>5985</v>
+        <v>5390</v>
       </c>
       <c r="G21" s="6">
-        <v>6165</v>
+        <v>5630</v>
       </c>
       <c r="H21" s="6">
-        <v>5695</v>
+        <v>5575</v>
       </c>
       <c r="I21" s="6">
         <v>5950</v>
@@ -2470,7 +2473,7 @@
         <v>5355</v>
       </c>
       <c r="P21" s="18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
@@ -2484,19 +2487,19 @@
         <v>4655</v>
       </c>
       <c r="D22" s="1">
-        <v>4680</v>
+        <v>4695</v>
       </c>
       <c r="E22" s="1">
-        <v>4805</v>
+        <v>4750</v>
       </c>
       <c r="F22" s="6">
-        <v>4725</v>
+        <v>5345</v>
       </c>
       <c r="G22" s="6">
-        <v>4820</v>
+        <v>5295</v>
       </c>
       <c r="H22" s="6">
-        <v>4585</v>
+        <v>5255</v>
       </c>
       <c r="I22" s="6">
         <v>4735</v>
@@ -2515,14 +2518,14 @@
       </c>
       <c r="N22" s="18">
         <f t="shared" si="2"/>
-        <v>4585</v>
+        <v>4590</v>
       </c>
       <c r="O22" s="6">
         <f t="shared" ref="O22:O34" si="5">MIN(A22:N22)</f>
         <v>4585</v>
       </c>
       <c r="P22" s="18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
@@ -2536,19 +2539,19 @@
         <v>3305</v>
       </c>
       <c r="D23" s="1">
-        <v>3245</v>
+        <v>3340</v>
       </c>
       <c r="E23" s="1">
-        <v>3215</v>
+        <v>3335</v>
       </c>
       <c r="F23" s="6">
-        <v>3195</v>
+        <v>3170</v>
       </c>
       <c r="G23" s="6">
-        <v>3215</v>
+        <v>3290</v>
       </c>
       <c r="H23" s="6">
-        <v>3260</v>
+        <v>3220</v>
       </c>
       <c r="I23" s="6">
         <v>3330</v>
@@ -2567,14 +2570,14 @@
       </c>
       <c r="N23" s="18">
         <f t="shared" si="2"/>
-        <v>3195</v>
+        <v>3170</v>
       </c>
       <c r="O23" s="6">
         <f t="shared" si="5"/>
-        <v>3195</v>
+        <v>3170</v>
       </c>
       <c r="P23" s="18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
@@ -2588,19 +2591,19 @@
         <v>6510</v>
       </c>
       <c r="D24" s="1">
-        <v>6445</v>
+        <v>6185</v>
       </c>
       <c r="E24" s="1">
-        <v>6360</v>
+        <v>6310</v>
       </c>
       <c r="F24" s="6">
-        <v>6430</v>
+        <v>6395</v>
       </c>
       <c r="G24" s="6">
-        <v>6470</v>
+        <v>6350</v>
       </c>
       <c r="H24" s="6">
-        <v>6275</v>
+        <v>6295</v>
       </c>
       <c r="I24" s="6">
         <v>6555</v>
@@ -2619,14 +2622,14 @@
       </c>
       <c r="N24" s="18">
         <f t="shared" si="2"/>
-        <v>6205</v>
+        <v>6185</v>
       </c>
       <c r="O24" s="6">
         <f t="shared" si="5"/>
         <v>6160</v>
       </c>
       <c r="P24" s="18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
@@ -2640,19 +2643,19 @@
         <v>2635</v>
       </c>
       <c r="D25" s="1">
-        <v>2745</v>
+        <v>2710</v>
       </c>
       <c r="E25" s="1">
-        <v>2870</v>
+        <v>2690</v>
       </c>
       <c r="F25" s="6">
-        <v>2805</v>
+        <v>2945</v>
       </c>
       <c r="G25" s="6">
-        <v>2695</v>
+        <v>2980</v>
       </c>
       <c r="H25" s="6">
-        <v>2580</v>
+        <v>2860</v>
       </c>
       <c r="I25" s="6">
         <v>2685</v>
@@ -2671,14 +2674,14 @@
       </c>
       <c r="N25" s="18">
         <f t="shared" si="2"/>
-        <v>2580</v>
+        <v>2615</v>
       </c>
       <c r="O25" s="6">
         <f t="shared" si="5"/>
         <v>2580</v>
       </c>
       <c r="P25" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
@@ -2692,19 +2695,19 @@
         <v>4580</v>
       </c>
       <c r="D26" s="1">
-        <v>4790</v>
+        <v>4305</v>
       </c>
       <c r="E26" s="1">
-        <v>4765</v>
+        <v>4450</v>
       </c>
       <c r="F26" s="6">
-        <v>4680</v>
+        <v>4825</v>
       </c>
       <c r="G26" s="6">
-        <v>4435</v>
+        <v>4835</v>
       </c>
       <c r="H26" s="6">
-        <v>4765</v>
+        <v>4895</v>
       </c>
       <c r="I26" s="6">
         <v>4485</v>
@@ -2723,14 +2726,14 @@
       </c>
       <c r="N26" s="18">
         <f t="shared" si="2"/>
-        <v>4435</v>
+        <v>4305</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="5"/>
-        <v>4435</v>
+        <v>4305</v>
       </c>
       <c r="P26" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
@@ -2744,19 +2747,19 @@
         <v>4165</v>
       </c>
       <c r="D27" s="1">
-        <v>4130</v>
+        <v>4160</v>
       </c>
       <c r="E27" s="1">
-        <v>4190</v>
+        <v>4180</v>
       </c>
       <c r="F27" s="6">
-        <v>4085</v>
+        <v>4165</v>
       </c>
       <c r="G27" s="6">
-        <v>4110</v>
+        <v>4230</v>
       </c>
       <c r="H27" s="6">
-        <v>4180</v>
+        <v>3995</v>
       </c>
       <c r="I27" s="6">
         <v>4135</v>
@@ -2775,14 +2778,14 @@
       </c>
       <c r="N27" s="18">
         <f t="shared" si="2"/>
-        <v>4075</v>
+        <v>3995</v>
       </c>
       <c r="O27" s="6">
         <f t="shared" si="5"/>
-        <v>4075</v>
+        <v>3995</v>
       </c>
       <c r="P27" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
@@ -2796,19 +2799,19 @@
         <v>6895</v>
       </c>
       <c r="D28" s="1">
-        <v>7065</v>
+        <v>6920</v>
       </c>
       <c r="E28" s="1">
-        <v>7105</v>
+        <v>6845</v>
       </c>
       <c r="F28" s="6">
-        <v>6965</v>
+        <v>6800</v>
       </c>
       <c r="G28" s="6">
-        <v>7095</v>
+        <v>6945</v>
       </c>
       <c r="H28" s="6">
-        <v>6780</v>
+        <v>7025</v>
       </c>
       <c r="I28" s="6">
         <v>7120</v>
@@ -2827,14 +2830,14 @@
       </c>
       <c r="N28" s="18">
         <f t="shared" si="2"/>
-        <v>6780</v>
+        <v>6800</v>
       </c>
       <c r="O28" s="6">
         <f t="shared" si="5"/>
         <v>6780</v>
       </c>
       <c r="P28" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
@@ -2848,19 +2851,19 @@
         <v>3315</v>
       </c>
       <c r="D29" s="1">
-        <v>3240</v>
+        <v>3390</v>
       </c>
       <c r="E29" s="1">
-        <v>3340</v>
+        <v>3445</v>
       </c>
       <c r="F29" s="6">
-        <v>3310</v>
+        <v>3350</v>
       </c>
       <c r="G29" s="6">
-        <v>3285</v>
+        <v>3485</v>
       </c>
       <c r="H29" s="6">
-        <v>3340</v>
+        <v>3455</v>
       </c>
       <c r="I29" s="6">
         <v>3425</v>
@@ -2879,14 +2882,14 @@
       </c>
       <c r="N29" s="18">
         <f t="shared" si="2"/>
-        <v>3240</v>
+        <v>3245</v>
       </c>
       <c r="O29" s="6">
         <f t="shared" si="5"/>
         <v>3240</v>
       </c>
       <c r="P29" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
@@ -2900,19 +2903,19 @@
         <v>3775</v>
       </c>
       <c r="D30" s="1">
-        <v>3770</v>
+        <v>3795</v>
       </c>
       <c r="E30" s="1">
-        <v>3770</v>
+        <v>3695</v>
       </c>
       <c r="F30" s="6">
-        <v>3595</v>
+        <v>4000</v>
       </c>
       <c r="G30" s="6">
-        <v>3700</v>
+        <v>3930</v>
       </c>
       <c r="H30" s="6">
-        <v>3810</v>
+        <v>3885</v>
       </c>
       <c r="I30" s="6">
         <v>3720</v>
@@ -2931,14 +2934,14 @@
       </c>
       <c r="N30" s="18">
         <f t="shared" si="2"/>
-        <v>3595</v>
+        <v>3635</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="5"/>
         <v>3595</v>
       </c>
       <c r="P30" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
@@ -2952,19 +2955,19 @@
         <v>1925</v>
       </c>
       <c r="D31" s="1">
-        <v>1965</v>
+        <v>1870</v>
       </c>
       <c r="E31" s="1">
-        <v>1910</v>
+        <v>1885</v>
       </c>
       <c r="F31" s="6">
-        <v>1840</v>
+        <v>2005</v>
       </c>
       <c r="G31" s="6">
-        <v>1935</v>
+        <v>1925</v>
       </c>
       <c r="H31" s="6">
-        <v>1940</v>
+        <v>1900</v>
       </c>
       <c r="I31" s="6">
         <v>1920</v>
@@ -2990,7 +2993,7 @@
         <v>1830</v>
       </c>
       <c r="P31" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
@@ -3004,19 +3007,19 @@
         <v>2675</v>
       </c>
       <c r="D32" s="1">
-        <v>2685</v>
+        <v>2625</v>
       </c>
       <c r="E32" s="1">
-        <v>2680</v>
+        <v>2635</v>
       </c>
       <c r="F32" s="6">
-        <v>2645</v>
+        <v>2620</v>
       </c>
       <c r="G32" s="6">
-        <v>2725</v>
+        <v>2555</v>
       </c>
       <c r="H32" s="6">
-        <v>2710</v>
+        <v>2745</v>
       </c>
       <c r="I32" s="6">
         <v>2705</v>
@@ -3035,14 +3038,14 @@
       </c>
       <c r="N32" s="18">
         <f t="shared" si="2"/>
-        <v>2635</v>
+        <v>2555</v>
       </c>
       <c r="O32" s="6">
         <f t="shared" si="5"/>
-        <v>2590</v>
+        <v>2555</v>
       </c>
       <c r="P32" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
@@ -3056,19 +3059,19 @@
         <v>2240</v>
       </c>
       <c r="D33" s="1">
-        <v>2195</v>
+        <v>2120</v>
       </c>
       <c r="E33" s="1">
-        <v>2215</v>
+        <v>2205</v>
       </c>
       <c r="F33" s="6">
-        <v>2200</v>
+        <v>2185</v>
       </c>
       <c r="G33" s="6">
-        <v>2220</v>
+        <v>2210</v>
       </c>
       <c r="H33" s="6">
-        <v>2170</v>
+        <v>2175</v>
       </c>
       <c r="I33" s="6">
         <v>2185</v>
@@ -3087,14 +3090,14 @@
       </c>
       <c r="N33" s="18">
         <f t="shared" si="2"/>
-        <v>2145</v>
+        <v>2120</v>
       </c>
       <c r="O33" s="6">
         <f t="shared" si="5"/>
-        <v>2135</v>
+        <v>2120</v>
       </c>
       <c r="P33" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -3108,19 +3111,19 @@
         <v>2240</v>
       </c>
       <c r="D34" s="17">
-        <v>2180</v>
+        <v>2215</v>
       </c>
       <c r="E34" s="17">
-        <v>2250</v>
+        <v>2210</v>
       </c>
       <c r="F34" s="11">
-        <v>2215</v>
+        <v>2235</v>
       </c>
       <c r="G34" s="11">
-        <v>2180</v>
+        <v>2200</v>
       </c>
       <c r="H34" s="11">
-        <v>2190</v>
+        <v>2240</v>
       </c>
       <c r="I34" s="11">
         <v>2205</v>
@@ -3146,7 +3149,7 @@
         <v>2110</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
bug fix on TSP. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54270" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="55440" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>OldMin</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -87,10 +87,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;w1,w1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ACBR_iFAO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -103,39 +99,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_iBNO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_iFAO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSR_LS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>TSR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_iFAO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_iBNO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACBR_iFAO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSR_RM</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSR_RMIE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -143,15 +107,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_iBNO</t>
+    <t>ACBR_BNO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>BTS</t>
+    <t>TSR_TWW</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>TSR</t>
+    <t>BTS_TWW</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSR_TWW</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -906,7 +878,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -965,9 +937,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1372,7 +1341,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1385,126 +1354,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="B1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="22" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="30"/>
+      <c r="N1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="29"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="28"/>
     </row>
     <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="20" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="29"/>
+        <v>29</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
@@ -1540,11 +1497,11 @@
       </c>
       <c r="I4" s="13">
         <f t="shared" si="0"/>
-        <v>3860.7142857142858</v>
+        <v>3772.5</v>
       </c>
       <c r="J4" s="13">
         <f t="shared" si="0"/>
-        <v>3823.9285714285716</v>
+        <v>3872.5</v>
       </c>
       <c r="K4" s="13">
         <f t="shared" si="0"/>
@@ -1560,11 +1517,11 @@
       </c>
       <c r="N4" s="13">
         <f t="shared" si="0"/>
-        <v>3693.3928571428573</v>
+        <v>3678.0357142857142</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" si="0"/>
-        <v>3678.9285714285716</v>
+        <v>3665.5357142857142</v>
       </c>
       <c r="P4" s="7"/>
     </row>
@@ -1602,11 +1559,11 @@
       </c>
       <c r="I5" s="14">
         <f t="shared" si="1"/>
-        <v>3781.7857142857142</v>
+        <v>3747.1428571428573</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" si="1"/>
-        <v>3757.1428571428573</v>
+        <v>3774.2857142857142</v>
       </c>
       <c r="K5" s="14">
         <f t="shared" si="1"/>
@@ -1622,11 +1579,11 @@
       </c>
       <c r="N5" s="14">
         <f t="shared" si="1"/>
-        <v>3636.0714285714284</v>
+        <v>3630.7142857142858</v>
       </c>
       <c r="O5" s="14">
         <f t="shared" si="1"/>
-        <v>3616.4285714285716</v>
+        <v>3607.5</v>
       </c>
       <c r="P5" s="10">
         <v>1</v>
@@ -1658,10 +1615,10 @@
         <v>4945</v>
       </c>
       <c r="I6" s="1">
-        <v>5240</v>
+        <v>5295</v>
       </c>
       <c r="J6" s="6">
-        <v>5035</v>
+        <v>4810</v>
       </c>
       <c r="K6" s="6">
         <v>5320</v>
@@ -1674,11 +1631,11 @@
       </c>
       <c r="N6" s="18">
         <f>MIN(B6:M6)</f>
-        <v>4855</v>
+        <v>4810</v>
       </c>
       <c r="O6" s="6">
         <f>MIN(A6:N6)</f>
-        <v>4855</v>
+        <v>4810</v>
       </c>
       <c r="P6" s="18" t="s">
         <v>4</v>
@@ -1710,10 +1667,10 @@
         <v>4705</v>
       </c>
       <c r="I7" s="1">
-        <v>4660</v>
+        <v>4430</v>
       </c>
       <c r="J7" s="6">
-        <v>4750</v>
+        <v>5065</v>
       </c>
       <c r="K7" s="6">
         <v>4745</v>
@@ -1726,11 +1683,11 @@
       </c>
       <c r="N7" s="18">
         <f t="shared" ref="N7:N34" si="2">MIN(B7:M7)</f>
-        <v>4445</v>
+        <v>4430</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" ref="O7:O19" si="3">MIN(A7:N7)</f>
-        <v>4445</v>
+        <v>4430</v>
       </c>
       <c r="P7" s="18" t="s">
         <v>5</v>
@@ -1762,10 +1719,10 @@
         <v>3200</v>
       </c>
       <c r="I8" s="1">
-        <v>3180</v>
+        <v>3375</v>
       </c>
       <c r="J8" s="6">
-        <v>3145</v>
+        <v>3175</v>
       </c>
       <c r="K8" s="6">
         <v>3245</v>
@@ -1814,10 +1771,10 @@
         <v>5840</v>
       </c>
       <c r="I9" s="1">
-        <v>5905</v>
+        <v>5790</v>
       </c>
       <c r="J9" s="6">
-        <v>5795</v>
+        <v>5965</v>
       </c>
       <c r="K9" s="6">
         <v>5775</v>
@@ -1866,10 +1823,10 @@
         <v>2185</v>
       </c>
       <c r="I10" s="1">
-        <v>2105</v>
+        <v>2135</v>
       </c>
       <c r="J10" s="6">
-        <v>2205</v>
+        <v>2285</v>
       </c>
       <c r="K10" s="6">
         <v>2085</v>
@@ -1918,10 +1875,10 @@
         <v>4080</v>
       </c>
       <c r="I11" s="1">
-        <v>3980</v>
+        <v>3860</v>
       </c>
       <c r="J11" s="6">
-        <v>4120</v>
+        <v>4065</v>
       </c>
       <c r="K11" s="6">
         <v>3970</v>
@@ -1934,11 +1891,11 @@
       </c>
       <c r="N11" s="18">
         <f t="shared" si="2"/>
-        <v>3925</v>
+        <v>3860</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="3"/>
-        <v>3925</v>
+        <v>3860</v>
       </c>
       <c r="P11" s="18" t="s">
         <v>9</v>
@@ -1973,7 +1930,7 @@
         <v>4280</v>
       </c>
       <c r="J12" s="6">
-        <v>4245</v>
+        <v>4210</v>
       </c>
       <c r="K12" s="6">
         <v>4210</v>
@@ -2022,10 +1979,10 @@
         <v>6925</v>
       </c>
       <c r="I13" s="1">
-        <v>7405</v>
+        <v>6915</v>
       </c>
       <c r="J13" s="6">
-        <v>7035</v>
+        <v>6955</v>
       </c>
       <c r="K13" s="6">
         <v>7215</v>
@@ -2074,10 +2031,10 @@
         <v>3225</v>
       </c>
       <c r="I14" s="1">
-        <v>3140</v>
+        <v>3155</v>
       </c>
       <c r="J14" s="6">
-        <v>3165</v>
+        <v>3205</v>
       </c>
       <c r="K14" s="6">
         <v>3215</v>
@@ -2090,7 +2047,7 @@
       </c>
       <c r="N14" s="18">
         <f t="shared" si="2"/>
-        <v>3140</v>
+        <v>3155</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" si="3"/>
@@ -2126,10 +2083,10 @@
         <v>4305</v>
       </c>
       <c r="I15" s="1">
-        <v>4175</v>
+        <v>4155</v>
       </c>
       <c r="J15" s="6">
-        <v>4100</v>
+        <v>4180</v>
       </c>
       <c r="K15" s="6">
         <v>4210</v>
@@ -2178,10 +2135,10 @@
         <v>1795</v>
       </c>
       <c r="I16" s="1">
-        <v>1865</v>
+        <v>1800</v>
       </c>
       <c r="J16" s="6">
-        <v>1795</v>
+        <v>1840</v>
       </c>
       <c r="K16" s="6">
         <v>1895</v>
@@ -2230,10 +2187,10 @@
         <v>3275</v>
       </c>
       <c r="I17" s="1">
-        <v>2900</v>
+        <v>3105</v>
       </c>
       <c r="J17" s="6">
-        <v>3105</v>
+        <v>3050</v>
       </c>
       <c r="K17" s="6">
         <v>3145</v>
@@ -2246,7 +2203,7 @@
       </c>
       <c r="N17" s="18">
         <f t="shared" si="2"/>
-        <v>2900</v>
+        <v>2935</v>
       </c>
       <c r="O17" s="6">
         <f t="shared" si="3"/>
@@ -2282,10 +2239,10 @@
         <v>1990</v>
       </c>
       <c r="I18" s="1">
-        <v>1990</v>
+        <v>2040</v>
       </c>
       <c r="J18" s="6">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="K18" s="6">
         <v>1970</v>
@@ -2334,10 +2291,10 @@
         <v>2040</v>
       </c>
       <c r="I19" s="1">
-        <v>2120</v>
+        <v>2125</v>
       </c>
       <c r="J19" s="6">
-        <v>2095</v>
+        <v>2035</v>
       </c>
       <c r="K19" s="6">
         <v>2110</v>
@@ -2394,11 +2351,11 @@
       </c>
       <c r="I20" s="15">
         <f t="shared" si="4"/>
-        <v>3939.6428571428573</v>
+        <v>3797.8571428571427</v>
       </c>
       <c r="J20" s="15">
         <f t="shared" si="4"/>
-        <v>3890.7142857142858</v>
+        <v>3970.7142857142858</v>
       </c>
       <c r="K20" s="15">
         <f t="shared" si="4"/>
@@ -2414,11 +2371,11 @@
       </c>
       <c r="N20" s="15">
         <f t="shared" si="4"/>
-        <v>3750.7142857142858</v>
+        <v>3725.3571428571427</v>
       </c>
       <c r="O20" s="15">
         <f t="shared" si="4"/>
-        <v>3741.4285714285716</v>
+        <v>3723.5714285714284</v>
       </c>
       <c r="P20" s="9">
         <v>0</v>
@@ -2450,10 +2407,10 @@
         <v>5575</v>
       </c>
       <c r="I21" s="6">
-        <v>5950</v>
+        <v>5505</v>
       </c>
       <c r="J21" s="6">
-        <v>5425</v>
+        <v>5665</v>
       </c>
       <c r="K21" s="6">
         <v>5505</v>
@@ -2502,10 +2459,10 @@
         <v>5255</v>
       </c>
       <c r="I22" s="6">
-        <v>4735</v>
+        <v>4700</v>
       </c>
       <c r="J22" s="6">
-        <v>4950</v>
+        <v>5175</v>
       </c>
       <c r="K22" s="6">
         <v>4905</v>
@@ -2554,10 +2511,10 @@
         <v>3220</v>
       </c>
       <c r="I23" s="6">
-        <v>3330</v>
+        <v>3230</v>
       </c>
       <c r="J23" s="6">
-        <v>3295</v>
+        <v>3270</v>
       </c>
       <c r="K23" s="6">
         <v>3220</v>
@@ -2606,10 +2563,10 @@
         <v>6295</v>
       </c>
       <c r="I24" s="6">
-        <v>6555</v>
+        <v>5990</v>
       </c>
       <c r="J24" s="6">
-        <v>6385</v>
+        <v>6600</v>
       </c>
       <c r="K24" s="6">
         <v>6205</v>
@@ -2622,11 +2579,11 @@
       </c>
       <c r="N24" s="18">
         <f t="shared" si="2"/>
-        <v>6185</v>
+        <v>5990</v>
       </c>
       <c r="O24" s="6">
         <f t="shared" si="5"/>
-        <v>6160</v>
+        <v>5990</v>
       </c>
       <c r="P24" s="18" t="s">
         <v>7</v>
@@ -2658,10 +2615,10 @@
         <v>2860</v>
       </c>
       <c r="I25" s="6">
-        <v>2685</v>
+        <v>2580</v>
       </c>
       <c r="J25" s="6">
-        <v>2690</v>
+        <v>2905</v>
       </c>
       <c r="K25" s="6">
         <v>2845</v>
@@ -2674,7 +2631,7 @@
       </c>
       <c r="N25" s="18">
         <f t="shared" si="2"/>
-        <v>2615</v>
+        <v>2580</v>
       </c>
       <c r="O25" s="6">
         <f t="shared" si="5"/>
@@ -2710,10 +2667,10 @@
         <v>4895</v>
       </c>
       <c r="I26" s="6">
-        <v>4485</v>
+        <v>4455</v>
       </c>
       <c r="J26" s="6">
-        <v>4585</v>
+        <v>4990</v>
       </c>
       <c r="K26" s="6">
         <v>4585</v>
@@ -2762,10 +2719,10 @@
         <v>3995</v>
       </c>
       <c r="I27" s="6">
-        <v>4135</v>
+        <v>4150</v>
       </c>
       <c r="J27" s="6">
-        <v>4170</v>
+        <v>3970</v>
       </c>
       <c r="K27" s="6">
         <v>4260</v>
@@ -2778,11 +2735,11 @@
       </c>
       <c r="N27" s="18">
         <f t="shared" si="2"/>
-        <v>3995</v>
+        <v>3970</v>
       </c>
       <c r="O27" s="6">
         <f t="shared" si="5"/>
-        <v>3995</v>
+        <v>3970</v>
       </c>
       <c r="P27" s="18" t="s">
         <v>10</v>
@@ -2814,10 +2771,10 @@
         <v>7025</v>
       </c>
       <c r="I28" s="6">
-        <v>7120</v>
+        <v>6745</v>
       </c>
       <c r="J28" s="6">
-        <v>6815</v>
+        <v>6835</v>
       </c>
       <c r="K28" s="6">
         <v>6915</v>
@@ -2830,11 +2787,11 @@
       </c>
       <c r="N28" s="18">
         <f t="shared" si="2"/>
-        <v>6800</v>
+        <v>6745</v>
       </c>
       <c r="O28" s="6">
         <f t="shared" si="5"/>
-        <v>6780</v>
+        <v>6745</v>
       </c>
       <c r="P28" s="18" t="s">
         <v>11</v>
@@ -2866,10 +2823,10 @@
         <v>3455</v>
       </c>
       <c r="I29" s="6">
-        <v>3425</v>
+        <v>3380</v>
       </c>
       <c r="J29" s="6">
-        <v>3410</v>
+        <v>3435</v>
       </c>
       <c r="K29" s="6">
         <v>3450</v>
@@ -2918,10 +2875,10 @@
         <v>3885</v>
       </c>
       <c r="I30" s="6">
-        <v>3720</v>
+        <v>3610</v>
       </c>
       <c r="J30" s="6">
-        <v>3855</v>
+        <v>3755</v>
       </c>
       <c r="K30" s="6">
         <v>3635</v>
@@ -2934,7 +2891,7 @@
       </c>
       <c r="N30" s="18">
         <f t="shared" si="2"/>
-        <v>3635</v>
+        <v>3610</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="5"/>
@@ -2970,10 +2927,10 @@
         <v>1900</v>
       </c>
       <c r="I31" s="6">
-        <v>1920</v>
+        <v>1810</v>
       </c>
       <c r="J31" s="6">
-        <v>1865</v>
+        <v>1895</v>
       </c>
       <c r="K31" s="6">
         <v>1880</v>
@@ -2986,11 +2943,11 @@
       </c>
       <c r="N31" s="18">
         <f t="shared" si="2"/>
-        <v>1830</v>
+        <v>1810</v>
       </c>
       <c r="O31" s="6">
         <f t="shared" si="5"/>
-        <v>1830</v>
+        <v>1810</v>
       </c>
       <c r="P31" s="18" t="s">
         <v>14</v>
@@ -3022,10 +2979,10 @@
         <v>2745</v>
       </c>
       <c r="I32" s="6">
-        <v>2705</v>
+        <v>2680</v>
       </c>
       <c r="J32" s="6">
-        <v>2695</v>
+        <v>2735</v>
       </c>
       <c r="K32" s="6">
         <v>2635</v>
@@ -3074,10 +3031,10 @@
         <v>2175</v>
       </c>
       <c r="I33" s="6">
+        <v>2120</v>
+      </c>
+      <c r="J33" s="6">
         <v>2185</v>
-      </c>
-      <c r="J33" s="6">
-        <v>2145</v>
       </c>
       <c r="K33" s="6">
         <v>2185</v>
@@ -3126,10 +3083,10 @@
         <v>2240</v>
       </c>
       <c r="I34" s="11">
-        <v>2205</v>
+        <v>2215</v>
       </c>
       <c r="J34" s="11">
-        <v>2185</v>
+        <v>2175</v>
       </c>
       <c r="K34" s="11">
         <v>2110</v>

</xml_diff>

<commit_message>
add switch for enable tabu. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/Optima.xlsx
+++ b/INRC2_Simulator/log/Optima.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="55440" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="57780" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>OldMin</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -95,10 +95,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;w1,w1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -124,6 +120,30 @@
   </si>
   <si>
     <t>TSR_TWW</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>seq1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>seq0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;n.2,n.2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;0,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSRi8d8</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -477,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -749,6 +769,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -878,7 +909,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -927,6 +958,9 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -970,6 +1004,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1341,127 +1378,129 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="10.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="10.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.5" style="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="30"/>
-      <c r="N1" s="21" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="21"/>
+      <c r="N1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="20"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="29"/>
+    </row>
+    <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="28"/>
-    </row>
-    <row r="3" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="M3" s="3"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="28"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
@@ -1505,11 +1544,11 @@
       </c>
       <c r="K4" s="13">
         <f t="shared" si="0"/>
-        <v>3837.3214285714284</v>
+        <v>3789.6428571428573</v>
       </c>
       <c r="L4" s="13">
         <f t="shared" si="0"/>
-        <v>3810.3571428571427</v>
+        <v>3760.8928571428573</v>
       </c>
       <c r="M4" s="13">
         <f t="shared" si="0"/>
@@ -1517,11 +1556,11 @@
       </c>
       <c r="N4" s="13">
         <f t="shared" si="0"/>
-        <v>3678.0357142857142</v>
+        <v>3668.9285714285716</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" si="0"/>
-        <v>3665.5357142857142</v>
+        <v>3654.6428571428573</v>
       </c>
       <c r="P4" s="7"/>
     </row>
@@ -1567,11 +1606,11 @@
       </c>
       <c r="K5" s="14">
         <f t="shared" si="1"/>
-        <v>3793.5714285714284</v>
+        <v>3708.9285714285716</v>
       </c>
       <c r="L5" s="14">
         <f t="shared" si="1"/>
-        <v>3748.2142857142858</v>
+        <v>3711.0714285714284</v>
       </c>
       <c r="M5" s="14">
         <f t="shared" si="1"/>
@@ -1579,18 +1618,18 @@
       </c>
       <c r="N5" s="14">
         <f t="shared" si="1"/>
-        <v>3630.7142857142858</v>
+        <v>3614.2857142857142</v>
       </c>
       <c r="O5" s="14">
         <f t="shared" si="1"/>
-        <v>3607.5</v>
-      </c>
-      <c r="P5" s="10">
-        <v>1</v>
+        <v>3592.1428571428573</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="18">
+      <c r="A6" s="19">
         <v>5035</v>
       </c>
       <c r="B6" s="6">
@@ -1621,15 +1660,15 @@
         <v>4810</v>
       </c>
       <c r="K6" s="6">
-        <v>5320</v>
+        <v>5105</v>
       </c>
       <c r="L6" s="1">
-        <v>5225</v>
+        <v>5115</v>
       </c>
       <c r="M6" s="8">
         <v>5280</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="19">
         <f>MIN(B6:M6)</f>
         <v>4810</v>
       </c>
@@ -1637,12 +1676,12 @@
         <f>MIN(A6:N6)</f>
         <v>4810</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="18">
+      <c r="A7" s="19">
         <v>4550</v>
       </c>
       <c r="B7" s="6">
@@ -1673,15 +1712,15 @@
         <v>5065</v>
       </c>
       <c r="K7" s="6">
-        <v>4745</v>
+        <v>4685</v>
       </c>
       <c r="L7" s="1">
-        <v>4550</v>
+        <v>4560</v>
       </c>
       <c r="M7" s="8">
         <v>4615</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="19">
         <f t="shared" ref="N7:N34" si="2">MIN(B7:M7)</f>
         <v>4430</v>
       </c>
@@ -1689,12 +1728,12 @@
         <f t="shared" ref="O7:O19" si="3">MIN(A7:N7)</f>
         <v>4430</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" s="18">
+      <c r="A8" s="19">
         <v>3070</v>
       </c>
       <c r="B8" s="6">
@@ -1725,28 +1764,28 @@
         <v>3175</v>
       </c>
       <c r="K8" s="6">
-        <v>3245</v>
+        <v>3140</v>
       </c>
       <c r="L8" s="1">
-        <v>3070</v>
+        <v>3185</v>
       </c>
       <c r="M8" s="8">
         <v>3230</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="19">
         <f t="shared" si="2"/>
-        <v>3070</v>
+        <v>3140</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="3"/>
         <v>3070</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="18">
+      <c r="A9" s="19">
         <v>5670</v>
       </c>
       <c r="B9" s="6">
@@ -1777,28 +1816,28 @@
         <v>5965</v>
       </c>
       <c r="K9" s="6">
-        <v>5775</v>
+        <v>5685</v>
       </c>
       <c r="L9" s="1">
-        <v>5750</v>
+        <v>5680</v>
       </c>
       <c r="M9" s="8">
         <v>5835</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="19">
         <f t="shared" si="2"/>
-        <v>5690</v>
+        <v>5680</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="3"/>
         <v>5670</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="18">
+      <c r="A10" s="19">
         <v>2085</v>
       </c>
       <c r="B10" s="6">
@@ -1829,28 +1868,28 @@
         <v>2285</v>
       </c>
       <c r="K10" s="6">
-        <v>2085</v>
+        <v>2040</v>
       </c>
       <c r="L10" s="1">
-        <v>2210</v>
+        <v>2130</v>
       </c>
       <c r="M10" s="8">
         <v>2245</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="19">
         <f t="shared" si="2"/>
-        <v>2085</v>
+        <v>2040</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="3"/>
-        <v>2085</v>
-      </c>
-      <c r="P10" s="18" t="s">
+        <v>2040</v>
+      </c>
+      <c r="P10" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A11" s="18">
+      <c r="A11" s="19">
         <v>3970</v>
       </c>
       <c r="B11" s="6">
@@ -1881,15 +1920,15 @@
         <v>4065</v>
       </c>
       <c r="K11" s="6">
-        <v>3970</v>
+        <v>4085</v>
       </c>
       <c r="L11" s="1">
-        <v>4005</v>
+        <v>3930</v>
       </c>
       <c r="M11" s="8">
         <v>4040</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="19">
         <f t="shared" si="2"/>
         <v>3860</v>
       </c>
@@ -1897,12 +1936,12 @@
         <f t="shared" si="3"/>
         <v>3860</v>
       </c>
-      <c r="P11" s="18" t="s">
+      <c r="P11" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="18">
+      <c r="A12" s="19">
         <v>4140</v>
       </c>
       <c r="B12" s="6">
@@ -1933,28 +1972,28 @@
         <v>4210</v>
       </c>
       <c r="K12" s="6">
-        <v>4210</v>
+        <v>4160</v>
       </c>
       <c r="L12" s="1">
-        <v>4195</v>
+        <v>4275</v>
       </c>
       <c r="M12" s="8">
         <v>4345</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="19">
         <f t="shared" si="2"/>
-        <v>4180</v>
+        <v>4160</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="3"/>
         <v>4140</v>
       </c>
-      <c r="P12" s="18" t="s">
+      <c r="P12" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A13" s="18">
+      <c r="A13" s="19">
         <v>6850</v>
       </c>
       <c r="B13" s="6">
@@ -1985,15 +2024,15 @@
         <v>6955</v>
       </c>
       <c r="K13" s="6">
-        <v>7215</v>
+        <v>7050</v>
       </c>
       <c r="L13" s="1">
-        <v>7065</v>
+        <v>6940</v>
       </c>
       <c r="M13" s="8">
         <v>7285</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="19">
         <f t="shared" si="2"/>
         <v>6900</v>
       </c>
@@ -2001,12 +2040,12 @@
         <f t="shared" si="3"/>
         <v>6850</v>
       </c>
-      <c r="P13" s="18" t="s">
+      <c r="P13" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A14" s="18">
+      <c r="A14" s="19">
         <v>2980</v>
       </c>
       <c r="B14" s="6">
@@ -2037,28 +2076,28 @@
         <v>3205</v>
       </c>
       <c r="K14" s="6">
-        <v>3215</v>
+        <v>3200</v>
       </c>
       <c r="L14" s="1">
-        <v>3240</v>
+        <v>3100</v>
       </c>
       <c r="M14" s="8">
         <v>3215</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="19">
         <f t="shared" si="2"/>
-        <v>3155</v>
+        <v>3100</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" si="3"/>
         <v>2980</v>
       </c>
-      <c r="P14" s="18" t="s">
+      <c r="P14" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A15" s="18">
+      <c r="A15" s="19">
         <v>4010</v>
       </c>
       <c r="B15" s="6">
@@ -2089,28 +2128,28 @@
         <v>4180</v>
       </c>
       <c r="K15" s="6">
-        <v>4210</v>
+        <v>3815</v>
       </c>
       <c r="L15" s="1">
-        <v>4090</v>
+        <v>3945</v>
       </c>
       <c r="M15" s="8">
         <v>4205</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="19">
         <f t="shared" si="2"/>
-        <v>3985</v>
+        <v>3815</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="3"/>
-        <v>3985</v>
-      </c>
-      <c r="P15" s="18" t="s">
+        <v>3815</v>
+      </c>
+      <c r="P15" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A16" s="18">
+      <c r="A16" s="19">
         <v>1795</v>
       </c>
       <c r="B16" s="6">
@@ -2141,15 +2180,15 @@
         <v>1840</v>
       </c>
       <c r="K16" s="6">
-        <v>1895</v>
+        <v>1905</v>
       </c>
       <c r="L16" s="1">
-        <v>1895</v>
+        <v>1855</v>
       </c>
       <c r="M16" s="8">
         <v>1890</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="19">
         <f t="shared" si="2"/>
         <v>1795</v>
       </c>
@@ -2157,12 +2196,12 @@
         <f t="shared" si="3"/>
         <v>1795</v>
       </c>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A17" s="18">
+      <c r="A17" s="19">
         <v>2900</v>
       </c>
       <c r="B17" s="6">
@@ -2193,15 +2232,15 @@
         <v>3050</v>
       </c>
       <c r="K17" s="6">
-        <v>3145</v>
+        <v>3015</v>
       </c>
       <c r="L17" s="1">
-        <v>2995</v>
+        <v>3235</v>
       </c>
       <c r="M17" s="8">
         <v>3170</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="19">
         <f t="shared" si="2"/>
         <v>2935</v>
       </c>
@@ -2209,12 +2248,12 @@
         <f t="shared" si="3"/>
         <v>2900</v>
       </c>
-      <c r="P17" s="18" t="s">
+      <c r="P17" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A18" s="18">
+      <c r="A18" s="19">
         <v>1920</v>
       </c>
       <c r="B18" s="6">
@@ -2245,15 +2284,15 @@
         <v>2000</v>
       </c>
       <c r="K18" s="6">
-        <v>1970</v>
+        <v>1985</v>
       </c>
       <c r="L18" s="1">
-        <v>2080</v>
+        <v>1960</v>
       </c>
       <c r="M18" s="8">
         <v>1920</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="19">
         <f t="shared" si="2"/>
         <v>1920</v>
       </c>
@@ -2261,12 +2300,12 @@
         <f t="shared" si="3"/>
         <v>1920</v>
       </c>
-      <c r="P18" s="18" t="s">
+      <c r="P18" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A19" s="18">
+      <c r="A19" s="19">
         <v>2010</v>
       </c>
       <c r="B19" s="6">
@@ -2297,15 +2336,15 @@
         <v>2035</v>
       </c>
       <c r="K19" s="6">
-        <v>2110</v>
+        <v>2055</v>
       </c>
       <c r="L19" s="1">
-        <v>2105</v>
+        <v>2045</v>
       </c>
       <c r="M19" s="8">
         <v>2050</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="19">
         <f t="shared" si="2"/>
         <v>2015</v>
       </c>
@@ -2313,7 +2352,7 @@
         <f t="shared" si="3"/>
         <v>2010</v>
       </c>
-      <c r="P19" s="18" t="s">
+      <c r="P19" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2359,11 +2398,11 @@
       </c>
       <c r="K20" s="15">
         <f t="shared" si="4"/>
-        <v>3881.0714285714284</v>
+        <v>3870.3571428571427</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="4"/>
-        <v>3872.5</v>
+        <v>3810.7142857142858</v>
       </c>
       <c r="M20" s="15">
         <f t="shared" si="4"/>
@@ -2371,18 +2410,18 @@
       </c>
       <c r="N20" s="15">
         <f t="shared" si="4"/>
-        <v>3725.3571428571427</v>
+        <v>3723.5714285714284</v>
       </c>
       <c r="O20" s="15">
         <f t="shared" si="4"/>
-        <v>3723.5714285714284</v>
-      </c>
-      <c r="P20" s="9">
-        <v>0</v>
+        <v>3717.1428571428573</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A21" s="18">
+      <c r="A21" s="19">
         <v>5355</v>
       </c>
       <c r="B21" s="6">
@@ -2413,28 +2452,28 @@
         <v>5665</v>
       </c>
       <c r="K21" s="6">
-        <v>5505</v>
+        <v>5655</v>
       </c>
       <c r="L21" s="6">
-        <v>5655</v>
+        <v>5345</v>
       </c>
       <c r="M21" s="6">
         <v>5355</v>
       </c>
-      <c r="N21" s="18">
+      <c r="N21" s="19">
         <f t="shared" si="2"/>
-        <v>5355</v>
+        <v>5345</v>
       </c>
       <c r="O21" s="6">
         <f>MIN(A21:N21)</f>
-        <v>5355</v>
-      </c>
-      <c r="P21" s="18" t="s">
+        <v>5345</v>
+      </c>
+      <c r="P21" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A22" s="18">
+      <c r="A22" s="19">
         <v>4585</v>
       </c>
       <c r="B22" s="6">
@@ -2465,15 +2504,15 @@
         <v>5175</v>
       </c>
       <c r="K22" s="6">
-        <v>4905</v>
+        <v>4745</v>
       </c>
       <c r="L22" s="6">
-        <v>4820</v>
+        <v>4840</v>
       </c>
       <c r="M22" s="6">
         <v>4870</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="19">
         <f t="shared" si="2"/>
         <v>4590</v>
       </c>
@@ -2481,12 +2520,12 @@
         <f t="shared" ref="O22:O34" si="5">MIN(A22:N22)</f>
         <v>4585</v>
       </c>
-      <c r="P22" s="18" t="s">
+      <c r="P22" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A23" s="18">
+      <c r="A23" s="19">
         <v>3195</v>
       </c>
       <c r="B23" s="6">
@@ -2517,15 +2556,15 @@
         <v>3270</v>
       </c>
       <c r="K23" s="6">
-        <v>3220</v>
+        <v>3275</v>
       </c>
       <c r="L23" s="6">
-        <v>3250</v>
+        <v>3175</v>
       </c>
       <c r="M23" s="6">
         <v>3280</v>
       </c>
-      <c r="N23" s="18">
+      <c r="N23" s="19">
         <f t="shared" si="2"/>
         <v>3170</v>
       </c>
@@ -2533,12 +2572,12 @@
         <f t="shared" si="5"/>
         <v>3170</v>
       </c>
-      <c r="P23" s="18" t="s">
+      <c r="P23" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A24" s="18">
+      <c r="A24" s="19">
         <v>6160</v>
       </c>
       <c r="B24" s="6">
@@ -2569,15 +2608,15 @@
         <v>6600</v>
       </c>
       <c r="K24" s="6">
-        <v>6205</v>
+        <v>6320</v>
       </c>
       <c r="L24" s="6">
-        <v>6275</v>
+        <v>6035</v>
       </c>
       <c r="M24" s="6">
         <v>6290</v>
       </c>
-      <c r="N24" s="18">
+      <c r="N24" s="19">
         <f t="shared" si="2"/>
         <v>5990</v>
       </c>
@@ -2585,12 +2624,12 @@
         <f t="shared" si="5"/>
         <v>5990</v>
       </c>
-      <c r="P24" s="18" t="s">
+      <c r="P24" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A25" s="18">
+      <c r="A25" s="19">
         <v>2580</v>
       </c>
       <c r="B25" s="6">
@@ -2621,28 +2660,28 @@
         <v>2905</v>
       </c>
       <c r="K25" s="6">
-        <v>2845</v>
+        <v>2615</v>
       </c>
       <c r="L25" s="6">
-        <v>2625</v>
+        <v>2535</v>
       </c>
       <c r="M25" s="6">
         <v>2615</v>
       </c>
-      <c r="N25" s="18">
+      <c r="N25" s="19">
         <f t="shared" si="2"/>
-        <v>2580</v>
+        <v>2535</v>
       </c>
       <c r="O25" s="6">
         <f t="shared" si="5"/>
-        <v>2580</v>
-      </c>
-      <c r="P25" s="18" t="s">
+        <v>2535</v>
+      </c>
+      <c r="P25" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A26" s="18">
+      <c r="A26" s="19">
         <v>4435</v>
       </c>
       <c r="B26" s="6">
@@ -2673,15 +2712,15 @@
         <v>4990</v>
       </c>
       <c r="K26" s="6">
-        <v>4585</v>
+        <v>4365</v>
       </c>
       <c r="L26" s="6">
-        <v>4555</v>
+        <v>4635</v>
       </c>
       <c r="M26" s="6">
         <v>4675</v>
       </c>
-      <c r="N26" s="18">
+      <c r="N26" s="19">
         <f t="shared" si="2"/>
         <v>4305</v>
       </c>
@@ -2689,12 +2728,12 @@
         <f t="shared" si="5"/>
         <v>4305</v>
       </c>
-      <c r="P26" s="18" t="s">
+      <c r="P26" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A27" s="18">
+      <c r="A27" s="19">
         <v>4075</v>
       </c>
       <c r="B27" s="6">
@@ -2725,15 +2764,15 @@
         <v>3970</v>
       </c>
       <c r="K27" s="6">
-        <v>4260</v>
+        <v>4225</v>
       </c>
       <c r="L27" s="6">
-        <v>4170</v>
+        <v>4130</v>
       </c>
       <c r="M27" s="6">
         <v>4075</v>
       </c>
-      <c r="N27" s="18">
+      <c r="N27" s="19">
         <f t="shared" si="2"/>
         <v>3970</v>
       </c>
@@ -2741,12 +2780,12 @@
         <f t="shared" si="5"/>
         <v>3970</v>
       </c>
-      <c r="P27" s="18" t="s">
+      <c r="P27" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A28" s="18">
+      <c r="A28" s="19">
         <v>6780</v>
       </c>
       <c r="B28" s="6">
@@ -2777,28 +2816,28 @@
         <v>6835</v>
       </c>
       <c r="K28" s="6">
-        <v>6915</v>
+        <v>6905</v>
       </c>
       <c r="L28" s="6">
-        <v>6830</v>
+        <v>6710</v>
       </c>
       <c r="M28" s="6">
         <v>6985</v>
       </c>
-      <c r="N28" s="18">
+      <c r="N28" s="19">
         <f t="shared" si="2"/>
-        <v>6745</v>
+        <v>6710</v>
       </c>
       <c r="O28" s="6">
         <f t="shared" si="5"/>
-        <v>6745</v>
-      </c>
-      <c r="P28" s="18" t="s">
+        <v>6710</v>
+      </c>
+      <c r="P28" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A29" s="18">
+      <c r="A29" s="19">
         <v>3240</v>
       </c>
       <c r="B29" s="6">
@@ -2829,15 +2868,15 @@
         <v>3435</v>
       </c>
       <c r="K29" s="6">
-        <v>3450</v>
+        <v>3380</v>
       </c>
       <c r="L29" s="6">
-        <v>3340</v>
+        <v>3290</v>
       </c>
       <c r="M29" s="6">
         <v>3470</v>
       </c>
-      <c r="N29" s="18">
+      <c r="N29" s="19">
         <f t="shared" si="2"/>
         <v>3245</v>
       </c>
@@ -2845,12 +2884,12 @@
         <f t="shared" si="5"/>
         <v>3240</v>
       </c>
-      <c r="P29" s="18" t="s">
+      <c r="P29" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A30" s="18">
+      <c r="A30" s="19">
         <v>3595</v>
       </c>
       <c r="B30" s="6">
@@ -2881,15 +2920,15 @@
         <v>3755</v>
       </c>
       <c r="K30" s="6">
-        <v>3635</v>
+        <v>3720</v>
       </c>
       <c r="L30" s="6">
-        <v>3815</v>
+        <v>3660</v>
       </c>
       <c r="M30" s="6">
         <v>3860</v>
       </c>
-      <c r="N30" s="18">
+      <c r="N30" s="19">
         <f t="shared" si="2"/>
         <v>3610</v>
       </c>
@@ -2897,12 +2936,12 @@
         <f t="shared" si="5"/>
         <v>3595</v>
       </c>
-      <c r="P30" s="18" t="s">
+      <c r="P30" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A31" s="18">
+      <c r="A31" s="19">
         <v>1830</v>
       </c>
       <c r="B31" s="6">
@@ -2933,15 +2972,15 @@
         <v>1895</v>
       </c>
       <c r="K31" s="6">
-        <v>1880</v>
+        <v>1905</v>
       </c>
       <c r="L31" s="6">
-        <v>1830</v>
+        <v>1875</v>
       </c>
       <c r="M31" s="6">
         <v>1865</v>
       </c>
-      <c r="N31" s="18">
+      <c r="N31" s="19">
         <f t="shared" si="2"/>
         <v>1810</v>
       </c>
@@ -2949,12 +2988,12 @@
         <f t="shared" si="5"/>
         <v>1810</v>
       </c>
-      <c r="P31" s="18" t="s">
+      <c r="P31" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A32" s="18">
+      <c r="A32" s="19">
         <v>2590</v>
       </c>
       <c r="B32" s="6">
@@ -2985,15 +3024,15 @@
         <v>2735</v>
       </c>
       <c r="K32" s="6">
-        <v>2635</v>
+        <v>2710</v>
       </c>
       <c r="L32" s="6">
-        <v>2635</v>
+        <v>2720</v>
       </c>
       <c r="M32" s="6">
         <v>2665</v>
       </c>
-      <c r="N32" s="18">
+      <c r="N32" s="19">
         <f t="shared" si="2"/>
         <v>2555</v>
       </c>
@@ -3001,12 +3040,12 @@
         <f t="shared" si="5"/>
         <v>2555</v>
       </c>
-      <c r="P32" s="18" t="s">
+      <c r="P32" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A33" s="18">
+      <c r="A33" s="19">
         <v>2135</v>
       </c>
       <c r="B33" s="6">
@@ -3037,15 +3076,15 @@
         <v>2185</v>
       </c>
       <c r="K33" s="6">
-        <v>2185</v>
+        <v>2165</v>
       </c>
       <c r="L33" s="6">
-        <v>2220</v>
+        <v>2165</v>
       </c>
       <c r="M33" s="6">
         <v>2150</v>
       </c>
-      <c r="N33" s="18">
+      <c r="N33" s="19">
         <f t="shared" si="2"/>
         <v>2120</v>
       </c>
@@ -3053,7 +3092,7 @@
         <f t="shared" si="5"/>
         <v>2120</v>
       </c>
-      <c r="P33" s="18" t="s">
+      <c r="P33" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3067,10 +3106,10 @@
       <c r="C34" s="11">
         <v>2240</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="18">
         <v>2215</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="18">
         <v>2210</v>
       </c>
       <c r="F34" s="11">
@@ -3089,17 +3128,17 @@
         <v>2175</v>
       </c>
       <c r="K34" s="11">
-        <v>2110</v>
+        <v>2200</v>
       </c>
       <c r="L34" s="11">
-        <v>2195</v>
+        <v>2235</v>
       </c>
       <c r="M34" s="11">
         <v>2225</v>
       </c>
       <c r="N34" s="4">
         <f t="shared" si="2"/>
-        <v>2110</v>
+        <v>2175</v>
       </c>
       <c r="O34" s="4">
         <f t="shared" si="5"/>
@@ -3113,17 +3152,12 @@
       <c r="N35" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="5">
     <mergeCell ref="N1:N3"/>
     <mergeCell ref="O1:O3"/>
     <mergeCell ref="P1:P3"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:O34">

</xml_diff>